<commit_message>
Add some words for the step which require the Internetworking environment.
</commit_message>
<xml_diff>
--- a/macs+lan.xlsx
+++ b/macs+lan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpsuzuki\Documents\2021_03\初期講習会\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{925070B7-7B69-4261-ACF0-FD788B4F3FE3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F4052B6-C13D-4913-BFCF-5C04C6630115}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="15468" windowHeight="6396" tabRatio="772" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="15468" windowHeight="6396" tabRatio="772" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -5667,8 +5667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6E56ADE-9B9A-41F5-BFC9-8C8E6A100436}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -6614,7 +6614,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
change macs+lan to 2022 ver.
</commit_message>
<xml_diff>
--- a/macs+lan.xlsx
+++ b/macs+lan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hiroshimauniv-my.sharepoint.com/personal/kishiba_hiroshima-u_ac_jp/Documents/Documents/GitHub/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="180" documentId="13_ncr:1_{24C083B2-CEBE-46F8-A593-5C30BCD27FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D129E8C3-DED3-426D-8121-EA5C79B40B1B}"/>
+  <xr:revisionPtr revIDLastSave="185" documentId="13_ncr:1_{24C083B2-CEBE-46F8-A593-5C30BCD27FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{583CE264-7A56-4FD8-AAE8-26380AAE5E0D}"/>
   <bookViews>
-    <workbookView xWindow="4695" yWindow="165" windowWidth="18225" windowHeight="11873" tabRatio="772" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2520" yWindow="795" windowWidth="18225" windowHeight="11873" tabRatio="772" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <sheet name="ch7" sheetId="17" r:id="rId9"/>
     <sheet name="ch8" sheetId="4" r:id="rId10"/>
     <sheet name="ch9" sheetId="8" r:id="rId11"/>
-    <sheet name="ch10" sheetId="16" r:id="rId12"/>
+    <sheet name="ch9a" sheetId="16" r:id="rId12"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -1380,10 +1380,6 @@
   </si>
   <si>
     <t>00_BlankDesktop.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>FRESTA-TEXT-2021 Mac chap.1</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1958,10 +1954,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>bb9-login.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>ESET-info-maOS-update.png</t>
   </si>
   <si>
@@ -2967,24 +2959,6 @@
  &lt;/ul&gt;</t>
     <rPh sb="137" eb="139">
       <t>ニンショウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>macOS 10以前の方は、以下のサイト「ウィルス対策ソフトのインストール手順」をブラウザで開き、説明に従ってください。
-開く際にID,パスワードを要求されたら、広大ID（学生番号）と広大パスワード（学生番号と一緒にもらっていると思います）を入力してください。
-&lt;a href="https://mslicense.office.hiroshima-u.ac.jp/sw-room/ms/endpoint.html"&gt;https://mslicense.office.hiroshima-u.ac.jp/sw-room/ms/endpoint.html&lt;/a&gt;</t>
-    <rPh sb="8" eb="10">
-      <t>イゼン</t>
-    </rPh>
-    <rPh sb="11" eb="12">
-      <t>カタ</t>
-    </rPh>
-    <rPh sb="102" eb="104">
-      <t>バンゴウ</t>
-    </rPh>
-    <rPh sb="115" eb="116">
-      <t>オモ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -4311,6 +4285,34 @@
     </rPh>
     <rPh sb="336" eb="338">
       <t>セツメイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FRESTA-TEXT-2022 Mac chap.1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>以下のサイト「ウィルス対策ソフトのインストール手順」をブラウザで開き、説明に従ってください。
+開く際にID,パスワードを要求されたら、広大ID（学生番号）と広大パスワード（学生番号と一緒にもらっていると思います）を入力してください。
+&lt;a href="https://mslicense.office.hiroshima-u.ac.jp/sw-room/ms/endpoint.html"&gt;https://mslicense.office.hiroshima-u.ac.jp/sw-room/ms/endpoint.html&lt;/a&gt;</t>
+    <rPh sb="88" eb="90">
+      <t>バンゴウ</t>
+    </rPh>
+    <rPh sb="101" eb="102">
+      <t>オモ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">次のリンクから広島大学Moodleにアクセスしてください。
+&lt;a href="https://moodle.huc.hiroshima-u.ac.jp/"&gt;https://moodle.huc.hiroshima-u.ac.jp/&lt;/a&gt;
+</t>
+    <rPh sb="0" eb="1">
+      <t>ツギ</t>
+    </rPh>
+    <rPh sb="7" eb="11">
+      <t>ヒロシマダイガク</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -4720,7 +4722,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4736,7 +4738,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -4744,7 +4746,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -4779,7 +4781,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -4819,17 +4821,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -4851,7 +4853,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
@@ -4928,7 +4930,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -4944,7 +4946,7 @@
         <v>108</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4968,12 +4970,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -4981,12 +4983,12 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -4996,7 +4998,7 @@
     </row>
     <row r="11" spans="1:4" ht="165.75" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -5021,843 +5023,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A14737B-27B4-430E-A2C9-8E4453FC8EAA}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="C11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="C13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="C14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="C16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="C17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="51" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="C18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="C19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="92.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="C20" t="s">
-        <v>123</v>
-      </c>
-      <c r="D20" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="C21" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="C22" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="C23" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="C24" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>4</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="C25" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="51" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>4</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="C26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D26" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B27" s="1" t="s">
-        <v>247</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D30"/>
-  <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="84.1328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="51" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C20" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C21" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C22" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C23" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B24" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C24" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B25" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C25" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B26" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D26" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C27" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B28" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C28" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B29" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="C29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>4</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="C30" t="s">
-        <v>10</v>
-      </c>
-      <c r="D30" t="s">
-        <v>161</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D14"/>
-  <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="102" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="51" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="51" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="C12" t="s">
-        <v>123</v>
-      </c>
-      <c r="D12" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="C13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="C14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" t="s">
-        <v>171</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6E56ADE-9B9A-41F5-BFC9-8C8E6A100436}">
-  <dimension ref="A1:D32"/>
-  <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -5874,7 +5040,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>276</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5882,7 +5048,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>201</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5898,27 +5064,863 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>278</v>
+        <v>315</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="51" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="92.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C20" t="s">
+        <v>123</v>
+      </c>
+      <c r="D20" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C24" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="51" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="84.1328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="51" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C24" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C30" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" t="s">
+        <v>161</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="102" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="51" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="51" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C12" t="s">
+        <v>123</v>
+      </c>
+      <c r="D12" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>170</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6E56ADE-9B9A-41F5-BFC9-8C8E6A100436}">
+  <dimension ref="A1:D32"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>255</v>
+        <v>322</v>
       </c>
       <c r="D9" t="s">
         <v>110</v>
@@ -5929,13 +5931,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -5943,15 +5945,15 @@
         <v>105</v>
       </c>
       <c r="D11" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -5967,18 +5969,18 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
         <v>205</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -6094,7 +6096,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6102,7 +6104,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6118,7 +6120,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -6126,7 +6128,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6193,7 +6195,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6201,7 +6203,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6217,7 +6219,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="102" x14ac:dyDescent="0.25">
@@ -6225,7 +6227,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6272,29 +6274,29 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -6321,7 +6323,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C15" t="s">
         <v>10</v>
@@ -6332,10 +6334,10 @@
     </row>
     <row r="16" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D16" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -6357,7 +6359,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C18" t="s">
         <v>10</v>
@@ -6387,8 +6389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView topLeftCell="B10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -6404,7 +6406,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6412,7 +6414,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6428,7 +6430,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -6436,7 +6438,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6447,7 +6449,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -6455,7 +6457,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -6463,7 +6465,7 @@
     </row>
     <row r="9" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>283</v>
+        <v>323</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -6471,13 +6473,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>217</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="191.25" x14ac:dyDescent="0.25">
@@ -6485,13 +6487,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -6499,7 +6501,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -6510,7 +6512,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -6521,7 +6523,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -6607,7 +6609,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
@@ -6615,7 +6617,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6639,7 +6641,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
@@ -6653,10 +6655,10 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -6664,7 +6666,7 @@
         <v>77</v>
       </c>
       <c r="D11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -6672,58 +6674,58 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
         <v>181</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D14" t="s">
         <v>183</v>
-      </c>
-      <c r="D14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D16" t="s">
         <v>186</v>
-      </c>
-      <c r="D16" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D18" t="s">
         <v>190</v>
-      </c>
-      <c r="D18" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -6731,13 +6733,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -6751,7 +6753,7 @@
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -6759,13 +6761,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -6779,7 +6781,7 @@
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -6787,13 +6789,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -6807,7 +6809,7 @@
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -6932,7 +6934,7 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
@@ -6993,8 +6995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A687F900-5547-4D89-8494-B67FCE27BE96}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView topLeftCell="B19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -7010,7 +7012,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -7034,7 +7036,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="229.5" x14ac:dyDescent="0.25">
@@ -7042,7 +7044,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7136,13 +7138,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -7150,7 +7152,7 @@
         <v>77</v>
       </c>
       <c r="D15" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -7164,7 +7166,7 @@
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -7186,7 +7188,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -7261,7 +7263,7 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
@@ -7294,7 +7296,7 @@
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
@@ -7305,7 +7307,7 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
@@ -7316,7 +7318,7 @@
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
@@ -7330,7 +7332,7 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
@@ -7349,7 +7351,7 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
@@ -7377,7 +7379,7 @@
         <v>4</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C36" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
macs+lan change to 2022 ver.
</commit_message>
<xml_diff>
--- a/macs+lan.xlsx
+++ b/macs+lan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hiroshimauniv-my.sharepoint.com/personal/kishiba_hiroshima-u_ac_jp/Documents/Documents/GitHub/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="185" documentId="13_ncr:1_{24C083B2-CEBE-46F8-A593-5C30BCD27FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{583CE264-7A56-4FD8-AAE8-26380AAE5E0D}"/>
+  <xr:revisionPtr revIDLastSave="186" documentId="13_ncr:1_{24C083B2-CEBE-46F8-A593-5C30BCD27FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{754A68D5-C66C-4CA6-821C-C59E86256914}"/>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="795" windowWidth="18225" windowHeight="11873" tabRatio="772" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1103" yWindow="1103" windowWidth="18225" windowHeight="11872" tabRatio="772" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <sheet name="ch7" sheetId="17" r:id="rId9"/>
     <sheet name="ch8" sheetId="4" r:id="rId10"/>
     <sheet name="ch9" sheetId="8" r:id="rId11"/>
-    <sheet name="ch9a" sheetId="16" r:id="rId12"/>
+    <sheet name="ch91" sheetId="16" r:id="rId12"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -5023,7 +5023,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A14737B-27B4-430E-A2C9-8E4453FC8EAA}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -6389,7 +6389,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
change macs+lan 2022 ver.
</commit_message>
<xml_diff>
--- a/macs+lan.xlsx
+++ b/macs+lan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hiroshimauniv-my.sharepoint.com/personal/kishiba_hiroshima-u_ac_jp/Documents/Documents/GitHub/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hiroshimauniv-my.sharepoint.com/personal/kishiba_hiroshima-u_ac_jp/Documents/Documents/fresta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="186" documentId="13_ncr:1_{24C083B2-CEBE-46F8-A593-5C30BCD27FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{754A68D5-C66C-4CA6-821C-C59E86256914}"/>
+  <xr:revisionPtr revIDLastSave="203" documentId="13_ncr:1_{24C083B2-CEBE-46F8-A593-5C30BCD27FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9A164F1-4241-4ACA-9E1E-3209BDA54347}"/>
   <bookViews>
-    <workbookView xWindow="1103" yWindow="1103" windowWidth="18225" windowHeight="11872" tabRatio="772" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1103" yWindow="1103" windowWidth="18225" windowHeight="11872" tabRatio="772" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="326">
   <si>
     <t>header1</t>
   </si>
@@ -46,10 +46,6 @@
   </si>
   <si>
     <t/>
-  </si>
-  <si>
-    <t xml:space="preserve">必携PC初期講習会では、みなさんのパソコンを広島大学のキャンパスで使用するための準備をおこないます。本日おこなうことを以下にあげます。
-  </t>
   </si>
   <si>
     <t>初期設定</t>
@@ -253,11 +249,6 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;h2&gt;&lt;a name="mymomiji"&gt;&lt;/a&gt;MYもみじ (履修登録や掲示板など)&lt;/h2&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">広島大学では履修登録、成績確認、各種通知は「MYもみじ」を利用して行います。「MYもみじ」へログインしてみましょう。
-広大ID（学生番号）、広大パスワードを入力し、「Myもみじへログイン」をクリックしてください。
-   </t>
   </si>
   <si>
     <t>win10-6-10.svg</t>
@@ -3336,34 +3327,6 @@
     </rPh>
     <rPh sb="24" eb="26">
       <t>セッテイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;h2&gt;&lt;a name="moodle"&gt;&lt;/a&gt;Moodle (オンライン学習支援サイト)&lt;/h2&gt; </t>
-    <rPh sb="38" eb="40">
-      <t>ガクシュウ</t>
-    </rPh>
-    <rPh sb="40" eb="42">
-      <t>シエン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>次のURLから広島大学Moodleにアクセスしてください。
-https://moodle.huc.hiroshima-u.ac.jp/
-（※ できればIMCホームページからのリンク場所を指示したい）</t>
-    <rPh sb="0" eb="1">
-      <t>ツギ</t>
-    </rPh>
-    <rPh sb="7" eb="11">
-      <t>ヒロシマダイガク</t>
-    </rPh>
-    <rPh sb="90" eb="92">
-      <t>バショ</t>
-    </rPh>
-    <rPh sb="93" eb="95">
-      <t>シジ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -3958,28 +3921,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">以下の手順はMoodleが利用可能になる4/2 以降に実施してください。
-「Moodle」は、オープンソースで提供されているオンライン学習環境です。広島大学ではMoodleを広大IDでログインして利用できるようにしています。
-ここに授業で使う資料が掲載されたり、テストを受けたり、課題を提出したりすることがあります。
-</t>
-    <rPh sb="55" eb="57">
-      <t>テイキョウ</t>
-    </rPh>
-    <rPh sb="67" eb="69">
-      <t>ガクシュウ</t>
-    </rPh>
-    <rPh sb="69" eb="71">
-      <t>カンキョウ</t>
-    </rPh>
-    <rPh sb="87" eb="89">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="98" eb="100">
-      <t>リヨウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>FRESTA-TEXT-2022 macOS appendix A</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -4313,6 +4254,102 @@
     </rPh>
     <rPh sb="7" eb="11">
       <t>ヒロシマダイガク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">必携PC初期実習では、みなさんのパソコンを広島大学のキャンパスで使用するための準備をおこないます。本日おこなうことを以下にあげます。
+  </t>
+    <rPh sb="6" eb="8">
+      <t>ジッシュウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">「Moodle」は、オープンソースで提供されているオンライン学習環境です。広島大学ではMoodleを広大IDでログインして利用できるようにしています。
+ここに授業で使う資料が掲載されたり、テストを受けたり、課題を提出したりすることがあります。
+</t>
+    <rPh sb="18" eb="20">
+      <t>テイキョウ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>ガクシュウ</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>カンキョウ</t>
+    </rPh>
+    <rPh sb="50" eb="52">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="61" eb="63">
+      <t>リヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;h2&gt;&lt;a name="moodle"&gt;&lt;/a&gt;Moodle (オンライン学習支援システム)&lt;/h2&gt; </t>
+    <rPh sb="38" eb="40">
+      <t>ガクシュウ</t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t>シエン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>次のリンクから広島大学Moodleにアクセスしてください。
+&lt;a href="https://moodle.huc.hiroshima-u.ac.jp/"&gt;https://moodle.huc.hiroshima-u.ac.jp/&lt;/a&gt;</t>
+    <rPh sb="0" eb="1">
+      <t>ツギ</t>
+    </rPh>
+    <rPh sb="7" eb="11">
+      <t>ヒロシマダイガク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「コース一覧」の中にある「ノートパソコン点検届」から、点検届を提出してください。</t>
+    <rPh sb="4" eb="6">
+      <t>イチラン</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>ナカ</t>
+    </rPh>
+    <rPh sb="20" eb="23">
+      <t>テンケントドケ</t>
+    </rPh>
+    <rPh sb="27" eb="30">
+      <t>テンケントドケ</t>
+    </rPh>
+    <rPh sb="31" eb="33">
+      <t>テイシュツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">広島大学では履修登録、成績確認、各種通知は「MYもみじ」を利用して行います。「MYもみじ」へログインしてみましょう。
+「Myもみじへログイン」をクリックしてください。
+   </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">広大ID（学生番号）、広大パスワードを入力してログインしましょう。
+※ 学外からの場合は、さらに多要素認証（MFA）のコード入力も必要です。
+   </t>
+    <rPh sb="36" eb="38">
+      <t>ガクガイ</t>
+    </rPh>
+    <rPh sb="41" eb="43">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="48" eb="53">
+      <t>タヨウソニンショウ</t>
+    </rPh>
+    <rPh sb="62" eb="64">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="65" eb="67">
+      <t>ヒツヨウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -4706,7 +4743,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -4722,7 +4759,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4738,7 +4775,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -4746,7 +4783,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -4760,7 +4797,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>319</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -4780,8 +4817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -4794,10 +4831,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4805,7 +4842,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -4813,7 +4850,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -4821,17 +4858,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -4839,13 +4876,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
@@ -4853,13 +4890,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -4867,13 +4904,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
         <v>20</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -4881,13 +4918,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
         <v>22</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -4895,13 +4932,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
         <v>24</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -4909,13 +4946,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -4927,10 +4964,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -4943,10 +4980,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4954,7 +4991,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -4962,7 +4999,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -4970,12 +5007,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -4983,32 +5020,37 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="165.75" x14ac:dyDescent="0.25">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="165.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5023,7 +5065,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A14737B-27B4-430E-A2C9-8E4453FC8EAA}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -5037,10 +5079,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5048,7 +5090,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5056,7 +5098,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -5064,7 +5106,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -5072,7 +5114,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -5086,7 +5128,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -5096,13 +5138,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -5110,24 +5152,24 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -5135,13 +5177,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -5149,40 +5191,40 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -5190,13 +5232,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -5204,24 +5246,24 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="92.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C20" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D20" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -5229,13 +5271,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -5243,35 +5285,35 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -5279,13 +5321,13 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -5293,18 +5335,18 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D26" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -5319,7 +5361,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -5332,10 +5374,10 @@
   <sheetData>
     <row r="1" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5343,7 +5385,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5351,7 +5393,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -5359,7 +5401,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -5367,7 +5409,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -5381,13 +5423,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
         <v>9</v>
       </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
       <c r="D7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -5395,13 +5437,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -5409,24 +5451,24 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -5434,13 +5476,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -5448,13 +5490,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -5462,24 +5504,24 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -5487,13 +5529,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -5501,13 +5543,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -5515,13 +5557,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
@@ -5529,134 +5571,134 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D26" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D27" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D28" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D29" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -5664,13 +5706,13 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D30" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -5684,8 +5726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -5698,10 +5740,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5709,7 +5751,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5717,7 +5759,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -5725,7 +5767,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="102" x14ac:dyDescent="0.25">
@@ -5733,7 +5775,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -5747,13 +5789,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -5761,13 +5803,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -5775,13 +5817,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -5789,13 +5831,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -5803,24 +5845,24 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D12" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -5828,24 +5870,24 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -5860,7 +5902,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -5873,10 +5915,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5884,7 +5926,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5892,7 +5934,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -5900,30 +5942,30 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="D9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -5931,37 +5973,37 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D11" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D12" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D13" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -5969,18 +6011,18 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -6080,7 +6122,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -6093,10 +6135,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6104,7 +6146,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6112,7 +6154,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -6120,7 +6162,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -6128,7 +6170,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6139,18 +6181,18 @@
     </row>
     <row r="7" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -6158,13 +6200,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -6178,8 +6220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -6192,10 +6234,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6203,7 +6245,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6211,7 +6253,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -6219,7 +6261,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="102" x14ac:dyDescent="0.25">
@@ -6227,7 +6269,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6238,7 +6280,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -6246,13 +6288,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -6260,13 +6302,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -6274,34 +6316,34 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -6309,13 +6351,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -6323,21 +6365,21 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D16" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -6345,13 +6387,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
@@ -6359,13 +6401,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -6389,8 +6431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -6403,10 +6445,10 @@
   <sheetData>
     <row r="1" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6414,7 +6456,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6422,7 +6464,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -6430,7 +6472,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -6438,7 +6480,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6449,15 +6491,15 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>314</v>
+        <v>320</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -6465,7 +6507,7 @@
     </row>
     <row r="9" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -6473,13 +6515,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="191.25" x14ac:dyDescent="0.25">
@@ -6487,13 +6529,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -6501,7 +6543,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -6512,7 +6554,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -6523,7 +6565,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -6568,8 +6610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -6582,10 +6624,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6593,7 +6635,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6601,7 +6643,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -6609,7 +6651,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
@@ -6617,7 +6659,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6628,12 +6670,12 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="102" x14ac:dyDescent="0.25">
@@ -6641,13 +6683,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -6655,18 +6697,18 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D10" t="s">
         <v>210</v>
-      </c>
-      <c r="D10" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D11" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -6674,58 +6716,58 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D14" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="D15" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D16" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D17" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D18" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -6733,13 +6775,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -6747,13 +6789,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -6761,13 +6803,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -6775,13 +6817,13 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -6789,13 +6831,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -6803,18 +6845,18 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -6822,13 +6864,13 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
       </c>
       <c r="D26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -6836,13 +6878,13 @@
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
       </c>
       <c r="D27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -6850,13 +6892,13 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -6864,13 +6906,13 @@
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -6878,13 +6920,13 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
       </c>
       <c r="D30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -6892,13 +6934,13 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -6906,13 +6948,13 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -6920,13 +6962,13 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -6934,13 +6976,13 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -6948,13 +6990,13 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -6962,13 +7004,13 @@
         <v>4</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C36" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D36" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -6976,13 +7018,13 @@
         <v>4</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C37" t="s">
         <v>4</v>
       </c>
       <c r="D37" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -6993,10 +7035,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A687F900-5547-4D89-8494-B67FCE27BE96}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView topLeftCell="B19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -7009,10 +7051,10 @@
   <sheetData>
     <row r="1" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -7020,7 +7062,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7028,7 +7070,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -7036,7 +7078,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="229.5" x14ac:dyDescent="0.25">
@@ -7044,7 +7086,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7055,7 +7097,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -7077,13 +7119,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
         <v>49</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -7091,18 +7133,18 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
         <v>51</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -7124,13 +7166,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
         <v>54</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -7138,21 +7180,21 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D15" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -7160,13 +7202,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -7174,13 +7216,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" t="s">
         <v>56</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>57</v>
-      </c>
-      <c r="D17" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
@@ -7188,13 +7230,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -7202,13 +7244,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
         <v>60</v>
-      </c>
-      <c r="C19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -7216,18 +7258,18 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" t="s">
         <v>62</v>
-      </c>
-      <c r="C20" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -7245,60 +7287,60 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>4</v>
-      </c>
       <c r="B23" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" t="s">
         <v>65</v>
       </c>
-      <c r="C23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" t="s">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="C24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>4</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>313</v>
+        <v>4</v>
       </c>
       <c r="C27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" t="s">
         <v>4</v>
       </c>
     </row>
@@ -7307,7 +7349,7 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
@@ -7318,88 +7360,99 @@
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
       </c>
-      <c r="D29" t="s">
+    </row>
+    <row r="30" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="127.5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="127.5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>4</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="C30" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" t="s">
+    <row r="35" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C36" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="102" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="C37" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1" t="s">
+    <row r="38" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>4</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="C34" t="s">
-        <v>4</v>
-      </c>
-      <c r="D34" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>4</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C35" t="s">
-        <v>10</v>
-      </c>
-      <c r="D35" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="102" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>4</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="C36" t="s">
-        <v>10</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="C38" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>4</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C37" t="s">
-        <v>10</v>
-      </c>
-      <c r="D37" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some screen confirmed about ESET
</commit_message>
<xml_diff>
--- a/macs+lan.xlsx
+++ b/macs+lan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hiroshimauniv-my.sharepoint.com/personal/kishiba_hiroshima-u_ac_jp/Documents/Documents/fresta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="323" documentId="13_ncr:1_{24C083B2-CEBE-46F8-A593-5C30BCD27FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BFA73A99-0F15-47D5-B729-9BB1162D37E8}"/>
+  <xr:revisionPtr revIDLastSave="334" documentId="13_ncr:1_{24C083B2-CEBE-46F8-A593-5C30BCD27FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F468B8E-385E-403E-A3F3-34794C559F12}"/>
   <bookViews>
     <workbookView xWindow="1837" yWindow="1837" windowWidth="18226" windowHeight="11873" tabRatio="772" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2720,11 +2720,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">ここでは、Google Chromeのインストールを行います。
-</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>ここでは、Microsoft Officeのインストールを行います。
  &lt;ul&gt;
 &lt;li&gt;&lt;a href="#office_install"&gt;Officeを入れる&lt;/a&gt;
@@ -4137,44 +4132,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>&lt;font color="red"&gt;※ 現在の学生向けインストールページの確認が必要&lt;/font&gt;
-下のほうにある「ESET Endpoint Antivirus for Mac」からダウンロードします。※ このページの「インストールマニュアル」をクリックすると、インストール手順を書いたマニュアルが表示されます。できればこのマニュアルを別ウィンドウで表示したままにしておくと、あとの作業がやりやすいでしょう。&lt;/p&gt;</t>
-    <rPh sb="20" eb="22">
-      <t>ゲンザイ</t>
-    </rPh>
-    <rPh sb="23" eb="25">
-      <t>ガクセイ</t>
-    </rPh>
-    <rPh sb="25" eb="26">
-      <t>ム</t>
-    </rPh>
-    <rPh sb="37" eb="39">
-      <t>カクニン</t>
-    </rPh>
-    <rPh sb="40" eb="42">
-      <t>ヒツヨウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;font color="red"&gt;最新バージョンのESETでは画面構成が少し違うかもしれません&lt;/font&gt;
- 次にウイルス対策ソフトの設定を確認しましょう。 画面右上にある青い「e」のアイコンをクリックしましょう。 表示されるメニューから「ESET Endpoint Antivirus を開く」をクリックします。  
- </t>
-    <rPh sb="18" eb="20">
-      <t>サイシン</t>
-    </rPh>
-    <rPh sb="32" eb="36">
-      <t>ガメンコウセイ</t>
-    </rPh>
-    <rPh sb="37" eb="38">
-      <t>スコ</t>
-    </rPh>
-    <rPh sb="39" eb="40">
-      <t>チガ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve">次のリンクから広島大学Moodleにアクセスしてください。
 &lt;a href="https://moodle.huc.hiroshima-u.ac.jp/"&gt;https://moodle.huc.hiroshima-u.ac.jp/&lt;/a&gt;
 &lt;font color="red"&gt; ※ 授業用Moodleに変更予定。もしくはセンターのMFA説明ページへ&lt;/font&gt;
@@ -4193,49 +4150,6 @@
     </rPh>
     <rPh sb="168" eb="170">
       <t>セツメイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>するとログイン画面が開きます。
-「ユーザ名」には広大ID（学生番号と同じ）を、「パスワード」には広大パスワードを入力してください。
-入力したら「ログイン」をクリックします。
- ※ 最近（たとえばこのテキストの第２章）で広大IDとパスワードを使ってログインしたあと続けて同じブラウザで作業している場合、この画面が出ずに次の画面に進むことがあります。これは「シングルサインオン」といい、何度も同じログイン作業をしなくて済む機能なのでそのまま作業を進めても大丈夫です。</t>
-    <rPh sb="152" eb="154">
-      <t>ガメン</t>
-    </rPh>
-    <rPh sb="155" eb="156">
-      <t>デ</t>
-    </rPh>
-    <rPh sb="158" eb="159">
-      <t>ツギ</t>
-    </rPh>
-    <rPh sb="160" eb="162">
-      <t>ガメン</t>
-    </rPh>
-    <rPh sb="163" eb="164">
-      <t>スス</t>
-    </rPh>
-    <rPh sb="191" eb="193">
-      <t>ナンド</t>
-    </rPh>
-    <rPh sb="194" eb="195">
-      <t>オナ</t>
-    </rPh>
-    <rPh sb="200" eb="202">
-      <t>サギョウ</t>
-    </rPh>
-    <rPh sb="207" eb="208">
-      <t>ス</t>
-    </rPh>
-    <rPh sb="209" eb="211">
-      <t>キノウ</t>
-    </rPh>
-    <rPh sb="218" eb="220">
-      <t>サギョウ</t>
-    </rPh>
-    <rPh sb="221" eb="222">
-      <t>スス</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -4640,31 +4554,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">図のようなパネルが出ます。中にこのMacに関する情報がたくさん表示されています。
-「macOS Catalina」というのがこのOSの名前ですね。その下に小さな文字で「バージョン10.15.7」とあります。このMacのOSのバージョンは10.15.7です。MacのOSはすべて64ビットです。&lt;span class="check"&gt;check-1,2&lt;/span&gt;
-&lt;strong&gt;※ 現在最新のmacOSの名前は Big Sur です。OSのバージョンやパソコンのスペックは、必ず自分のPCで確認してください。&lt;/strong&gt;
-パソコンの名称も書かれています。「MacBook Air」がこのMacのハードウェアの種類です。その下がCPUに関する情報、その下に主記憶装置の容量があります。メモリは8GB（ギガバイト)実装されているということですね。この容量が大きいほど、大量のデータを一括して扱ったり、多くのプログラムを同時に動作させたりすることがスムーズにできるようになります。   </t>
-    <rPh sb="193" eb="195">
-      <t>ゲンザイ</t>
-    </rPh>
-    <rPh sb="195" eb="197">
-      <t>サイシン</t>
-    </rPh>
-    <rPh sb="204" eb="206">
-      <t>ナマエ</t>
-    </rPh>
-    <rPh sb="239" eb="240">
-      <t>カナラ</t>
-    </rPh>
-    <rPh sb="241" eb="243">
-      <t>ジブン</t>
-    </rPh>
-    <rPh sb="247" eb="249">
-      <t>カクニン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>点検届の提出と、問い合わせ先紹介</t>
     <rPh sb="0" eb="3">
       <t>テンケントドケ</t>
@@ -4709,6 +4598,129 @@
     </rPh>
     <rPh sb="148" eb="150">
       <t>セッテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">図のようなパネルが出ます。中にこのMacに関する情報がたくさん表示されています。
+「macOS Catalina」というのがこのOSの名前ですね。その下に小さな文字で「バージョン10.15.7」とあります。このMacのOSのバージョンは10.15.7です。MacのOSはすべて64ビットです。&lt;span class="check"&gt;check-1,2&lt;/span&gt;
+&lt;strong&gt;※ 現在最新のmacOSの名前は Monterey です。OSのバージョンやパソコンのスペックは、必ず自分のPCで確認してください。&lt;/strong&gt;
+パソコンの名称も書かれています。「MacBook Air」がこのMacのハードウェアの種類です。その下がCPUに関する情報、その下に主記憶装置の容量があります。メモリは8GB（ギガバイト)実装されているということですね。この容量が大きいほど、大量のデータを一括して扱ったり、多くのプログラムを同時に動作させたりすることがスムーズにできるようになります。   </t>
+    <rPh sb="193" eb="195">
+      <t>ゲンザイ</t>
+    </rPh>
+    <rPh sb="195" eb="197">
+      <t>サイシン</t>
+    </rPh>
+    <rPh sb="204" eb="206">
+      <t>ナマエ</t>
+    </rPh>
+    <rPh sb="240" eb="241">
+      <t>カナラ</t>
+    </rPh>
+    <rPh sb="242" eb="244">
+      <t>ジブン</t>
+    </rPh>
+    <rPh sb="248" eb="250">
+      <t>カクニン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 次にウイルス対策ソフトの設定を確認しましょう。 画面右上にある青い「e」のアイコンをクリックしましょう。 表示されるメニューから「ESET Endpoint Antivirus を開く」をクリックします。  
+ </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;font color="red"&gt;※ 図のスクリーンイメージは現在のものと少し異なりますが、作業内容は下記のとおりです&lt;/font&gt;
+下のほうにある「ESET Endpoint Antivirus for Mac」からダウンロードします。
+※ このページの「インストールマニュアル」をクリックすると、インストール手順を書いたマニュアルが表示されます。できればこのマニュアルを別ウィンドウで表示したままにしておくと、あとの作業がやりやすいでしょう。&lt;/p&gt;</t>
+    <rPh sb="20" eb="21">
+      <t>ズ</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>ゲンザイ</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t>スコ</t>
+    </rPh>
+    <rPh sb="40" eb="41">
+      <t>コト</t>
+    </rPh>
+    <rPh sb="47" eb="49">
+      <t>サギョウ</t>
+    </rPh>
+    <rPh sb="49" eb="51">
+      <t>ナイヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ここでは、Google Chromeのインストールを行います。Chromeを既にインストールしている場合は、この章を飛ばして第４章に進んでください。
+</t>
+    <rPh sb="38" eb="39">
+      <t>スデ</t>
+    </rPh>
+    <rPh sb="50" eb="52">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="56" eb="57">
+      <t>ショウ</t>
+    </rPh>
+    <rPh sb="58" eb="59">
+      <t>ト</t>
+    </rPh>
+    <rPh sb="62" eb="63">
+      <t>ダイ</t>
+    </rPh>
+    <rPh sb="64" eb="65">
+      <t>ショウ</t>
+    </rPh>
+    <rPh sb="66" eb="67">
+      <t>スス</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>するとログイン画面が開きます。
+「ユーザ名」には広大ID（学生番号と同じ）を、「パスワード」には広大パスワードを入力してください。
+入力したら「ログイン」をクリックします。
+ ※ このテキストの第２章などで広大IDとパスワードを使ってログインしたあと続けて同じブラウザで作業している場合、この画面が出ずに次の画面に進むことがあります。これは「シングルサインオン」といい、何度も同じログイン作業をしなくて済む機能なのでそのまま作業を進めても大丈夫です。</t>
+    <rPh sb="146" eb="148">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="149" eb="150">
+      <t>デ</t>
+    </rPh>
+    <rPh sb="152" eb="153">
+      <t>ツギ</t>
+    </rPh>
+    <rPh sb="154" eb="156">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="157" eb="158">
+      <t>スス</t>
+    </rPh>
+    <rPh sb="185" eb="187">
+      <t>ナンド</t>
+    </rPh>
+    <rPh sb="188" eb="189">
+      <t>オナ</t>
+    </rPh>
+    <rPh sb="194" eb="196">
+      <t>サギョウ</t>
+    </rPh>
+    <rPh sb="201" eb="202">
+      <t>ス</t>
+    </rPh>
+    <rPh sb="203" eb="205">
+      <t>キノウ</t>
+    </rPh>
+    <rPh sb="212" eb="214">
+      <t>サギョウ</t>
+    </rPh>
+    <rPh sb="215" eb="216">
+      <t>スス</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -5118,7 +5130,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5134,7 +5146,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -5142,7 +5154,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -5156,7 +5168,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -5217,7 +5229,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -5227,7 +5239,7 @@
     </row>
     <row r="7" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -5249,7 +5261,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -5342,7 +5354,7 @@
         <v>100</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5366,17 +5378,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -5384,17 +5396,17 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -5404,7 +5416,7 @@
     </row>
     <row r="13" spans="1:4" ht="165.75" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -5470,7 +5482,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -5478,7 +5490,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -5492,7 +5504,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -5516,7 +5528,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
@@ -5527,7 +5539,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
@@ -5541,7 +5553,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
@@ -5621,7 +5633,7 @@
     </row>
     <row r="20" spans="1:4" ht="92.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C20" t="s">
         <v>114</v>
@@ -5765,7 +5777,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
@@ -5773,7 +5785,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6070,7 +6082,7 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C30" t="s">
         <v>8</v>
@@ -6090,8 +6102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -6131,7 +6143,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="102" x14ac:dyDescent="0.25">
@@ -6167,13 +6179,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -6181,7 +6193,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -6265,8 +6277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6E56ADE-9B9A-41F5-BFC9-8C8E6A100436}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -6282,7 +6294,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6306,43 +6318,43 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="D9" t="s">
         <v>301</v>
-      </c>
-      <c r="D9" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D10" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>304</v>
+        <v>327</v>
       </c>
       <c r="D11" t="s">
         <v>196</v>
@@ -6372,7 +6384,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -6472,7 +6484,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -6488,7 +6500,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6512,15 +6524,15 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>235</v>
+        <v>328</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6571,7 +6583,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -6587,7 +6599,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6611,7 +6623,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="102" x14ac:dyDescent="0.25">
@@ -6666,29 +6678,29 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -6696,12 +6708,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="51" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>305</v>
+        <v>326</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
@@ -6715,7 +6727,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
@@ -6743,7 +6755,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
@@ -6790,7 +6802,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6798,7 +6810,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6814,7 +6826,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="102" x14ac:dyDescent="0.25">
@@ -6822,7 +6834,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6833,7 +6845,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -6841,7 +6853,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -6849,7 +6861,7 @@
     </row>
     <row r="9" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -6857,13 +6869,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>307</v>
+        <v>329</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="191.25" x14ac:dyDescent="0.25">
@@ -6871,18 +6883,18 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -6890,7 +6902,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -6901,7 +6913,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -6912,7 +6924,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -6974,7 +6986,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6998,7 +7010,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
@@ -7006,7 +7018,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7030,7 +7042,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -7074,7 +7086,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -7087,7 +7099,7 @@
     </row>
     <row r="15" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D15" t="s">
         <v>174</v>
@@ -7323,7 +7335,7 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
@@ -7401,7 +7413,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -7425,7 +7437,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="229.5" x14ac:dyDescent="0.25">
@@ -7433,7 +7445,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7486,7 +7498,7 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -7538,7 +7550,7 @@
     </row>
     <row r="15" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="D15" t="s">
         <v>200</v>
@@ -7560,7 +7572,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -7582,7 +7594,7 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -7640,13 +7652,13 @@
     </row>
     <row r="24" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -7654,13 +7666,13 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -7668,7 +7680,7 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
@@ -7701,7 +7713,7 @@
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
@@ -7712,7 +7724,7 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
@@ -7723,7 +7735,7 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
@@ -7737,7 +7749,7 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
@@ -7748,13 +7760,13 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -7762,7 +7774,7 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
@@ -7773,7 +7785,7 @@
     </row>
     <row r="35" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -7786,7 +7798,7 @@
         <v>4</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C38" t="s">
         <v>4</v>
@@ -7814,7 +7826,7 @@
         <v>4</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C40" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
change "office download" in win10
</commit_message>
<xml_diff>
--- a/macs+lan.xlsx
+++ b/macs+lan.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="365" documentId="13_ncr:1_{24C083B2-CEBE-46F8-A593-5C30BCD27FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0001ACD-BB61-4F6F-9EFE-6B74529AFD46}"/>
   <bookViews>
-    <workbookView xWindow="10635" yWindow="-15555" windowWidth="16215" windowHeight="13590" tabRatio="772" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" tabRatio="772" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -6343,8 +6343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6E56ADE-9B9A-41F5-BFC9-8C8E6A100436}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -6649,7 +6649,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -6852,7 +6852,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -7038,8 +7038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -7465,8 +7465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A687F900-5547-4D89-8494-B67FCE27BE96}">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add some pics for win10
</commit_message>
<xml_diff>
--- a/macs+lan.xlsx
+++ b/macs+lan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hiroshimauniv-my.sharepoint.com/personal/kishiba_hiroshima-u_ac_jp/Documents/Documents/fresta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="365" documentId="13_ncr:1_{24C083B2-CEBE-46F8-A593-5C30BCD27FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0001ACD-BB61-4F6F-9EFE-6B74529AFD46}"/>
+  <xr:revisionPtr revIDLastSave="373" documentId="13_ncr:1_{24C083B2-CEBE-46F8-A593-5C30BCD27FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E678D6AF-9EF0-4134-B59A-09F5B96FDFFB}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" tabRatio="772" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4125" yWindow="2228" windowWidth="16215" windowHeight="13590" tabRatio="772" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -3063,16 +3063,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Moodleへのログインと多要素認証（MFA）の設定</t>
-    <rPh sb="13" eb="18">
-      <t>タヨウソニンショウ</t>
-    </rPh>
-    <rPh sb="24" eb="26">
-      <t>セッテイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>以下は、ESETを既にインストールした方が対象です。別に購入したウィルス対策ソフトを使う場合は、そのマニュアルでパターンファイルの更新の設定手順とフルスキャンの方法を確認し、実施してください。</t>
     <rPh sb="0" eb="2">
       <t>イカ</t>
@@ -3142,34 +3132,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>下の方にある「IMCアカウントのMFA設定」の説明に従ってIMCアカウントの多要素認証（MFA）設定を行ってください。&lt;span class="check"&gt;check-9&lt;/span&gt;</t>
-    <rPh sb="0" eb="1">
-      <t>シタ</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>ホウ</t>
-    </rPh>
-    <rPh sb="19" eb="21">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="23" eb="25">
-      <t>セツメイ</t>
-    </rPh>
-    <rPh sb="26" eb="27">
-      <t>シタガ</t>
-    </rPh>
-    <rPh sb="38" eb="43">
-      <t>タヨウソニンショウ</t>
-    </rPh>
-    <rPh sb="48" eb="50">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="51" eb="52">
-      <t>オコナ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>下の方にある「広大IDのMFA設定」の説明に従って広大IDの多要素認証（MFA）設定を行ってください。&lt;span class="check"&gt;check-10&lt;/span&gt;</t>
     <rPh sb="0" eb="1">
       <t>シタ</t>
@@ -3480,16 +3442,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">&lt;h2&gt;&lt;a name="moodle"&gt;&lt;/a&gt;Moodle (オンライン学習支援システム)&lt;/h2&gt; </t>
-    <rPh sb="38" eb="40">
-      <t>ガクシュウ</t>
-    </rPh>
-    <rPh sb="40" eb="42">
-      <t>シエン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve">広島大学では履修登録、成績確認、各種通知は「MYもみじ」を利用して行います。「MYもみじ」へログインしてみましょう。
 「Myもみじへログイン」をクリックしてください。
    </t>
@@ -3739,34 +3691,6 @@
   </si>
   <si>
     <t>オンライン履修登録などをおこなう「もみじ」、電子メールやクラウドストレージが使えるOffice365、オンライン学習支援システムのBb9など、大学で提供されているネットワークサービスを使えるようにします。</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>広島大学のオンライン学習支援システムMoodleにログインし、その中にある説明に従って多要素認証（MFA）の設定を行いましょう。</t>
-    <rPh sb="0" eb="4">
-      <t>ヒロシマダイガク</t>
-    </rPh>
-    <rPh sb="10" eb="14">
-      <t>ガクシュウシエン</t>
-    </rPh>
-    <rPh sb="33" eb="34">
-      <t>ナカ</t>
-    </rPh>
-    <rPh sb="37" eb="39">
-      <t>セツメイ</t>
-    </rPh>
-    <rPh sb="40" eb="41">
-      <t>シタガ</t>
-    </rPh>
-    <rPh sb="43" eb="48">
-      <t>タヨウソニンショウ</t>
-    </rPh>
-    <rPh sb="54" eb="56">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="57" eb="58">
-      <t>オコナ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -4200,22 +4124,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>大学で提供されているオンラインサービスはいくつもありますが、まずオンライン学習支援システムのMoodleにログインしてみましょう。
- &lt;ul&gt;
-&lt;li&gt;&lt;a href="#moodle"&gt;Moodleにログインする&lt;/a&gt;
-&lt;/li&gt;
-&lt;li&gt;&lt;a href="#mfa"&gt;多要素認証(MFA)の設定&lt;/a&gt;
-&lt;/li&gt;
- &lt;/ul&gt;</t>
-    <rPh sb="137" eb="142">
-      <t>タヨウソニンショウ</t>
-    </rPh>
-    <rPh sb="148" eb="150">
-      <t>セッテイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve">図のようなパネルが出ます。中にこのMacに関する情報がたくさん表示されています。
 「macOS Catalina」というのがこのOSの名前ですね。その下に小さな文字で「バージョン10.15.7」とあります。このMacのOSのバージョンは10.15.7です。MacのOSはすべて64ビットです。&lt;span class="check"&gt;check-1,2&lt;/span&gt;
 &lt;strong&gt;※ 現在最新のmacOSの名前は Monterey です。OSのバージョンやパソコンのスペックは、必ず自分のPCで確認してください。&lt;/strong&gt;
@@ -4339,51 +4247,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>※ ここまでの実習の中で、広島大学には２つのオンライン学習支援システム「Moodle」「Bb9」があることに気づかれたと思います。
-広島大学では今年度「Moodle」「Bb9」の２つのオンライン学習支援システムを併用します。来年度からは「Moodle」に一本化する予定です。
-しばらく面倒をおかけしますが、ご了解ください。</t>
-    <rPh sb="7" eb="9">
-      <t>ジッシュウ</t>
-    </rPh>
-    <rPh sb="10" eb="11">
-      <t>ナカ</t>
-    </rPh>
-    <rPh sb="13" eb="17">
-      <t>ヒロシマダイガク</t>
-    </rPh>
-    <rPh sb="27" eb="31">
-      <t>ガクシュウシエン</t>
-    </rPh>
-    <rPh sb="54" eb="55">
-      <t>キ</t>
-    </rPh>
-    <rPh sb="60" eb="61">
-      <t>オモ</t>
-    </rPh>
-    <rPh sb="97" eb="101">
-      <t>ガクシュウシエン</t>
-    </rPh>
-    <rPh sb="106" eb="108">
-      <t>ヘイヨウ</t>
-    </rPh>
-    <rPh sb="112" eb="115">
-      <t>ライネンド</t>
-    </rPh>
-    <rPh sb="127" eb="130">
-      <t>イッポンカ</t>
-    </rPh>
-    <rPh sb="132" eb="134">
-      <t>ヨテイ</t>
-    </rPh>
-    <rPh sb="142" eb="144">
-      <t>メンドウ</t>
-    </rPh>
-    <rPh sb="154" eb="156">
-      <t>リョウカイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>以下のサイト「ダウンロード（マイクロソフト包括ライセンス）」をsafariブラウザで開いて、その中の「WindowsOS, ウィルス対策ソフト(ESET)」「学生の個人所有PC用のダウンロードはこちらから」のリンクをクリックしてください。
 ※ ESET はマイクロソフト製品ではありませんが、大学で提供するソフトウェアとしてまとめてサービスしています
 &lt;a href="https://www.media.hiroshima-u.ac.jp/services/ms-ees/ms-download/"&gt;https://www.media.hiroshima-u.ac.jp/services/ms-ees/ms-download/&lt;/a&gt;</t>
@@ -4421,24 +4284,6 @@
   </si>
   <si>
     <t>moodle-login.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>次のリンクから広島大学オンライン学習支援システム（Moodle）にアクセスしてください。
-&lt;a href="https://moodle.vle.hiroshima-u.ac.jp/local/hulogin/"&gt;https://moodle.vle.hiroshima-u.ac.jp/local/hulogin/&lt;/a&gt;
-「広大IDでログイン」をクリックしましょう。</t>
-    <rPh sb="0" eb="1">
-      <t>ツギ</t>
-    </rPh>
-    <rPh sb="7" eb="11">
-      <t>ヒロシマダイガク</t>
-    </rPh>
-    <rPh sb="16" eb="20">
-      <t>ガクシュウシエン</t>
-    </rPh>
-    <rPh sb="164" eb="166">
-      <t>ヒロダイ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -4581,31 +4426,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Moodleの「コース概要」の中の「MFA21 MFA設定ガイド」をクリックして、まず表示される「広大IDとIMCアカウントの概要」を読んでください。</t>
-    <rPh sb="11" eb="13">
-      <t>ガイヨウ</t>
-    </rPh>
-    <rPh sb="15" eb="16">
-      <t>ナカ</t>
-    </rPh>
-    <rPh sb="27" eb="29">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="43" eb="45">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="49" eb="51">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="63" eb="65">
-      <t>ガイヨウ</t>
-    </rPh>
-    <rPh sb="67" eb="68">
-      <t>ヨ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>次のリンクから広島大学オンライン学習支援システム（Moodle）にアクセスしてください。
 &lt;a href="https://moodle.vle.hiroshima-u.ac.jp/local/hulogin/"&gt;https://moodle.vle.hiroshima-u.ac.jp/local/hulogin/&lt;/a&gt;
 「広大IDでログイン」をクリックしてログインしましょう。</t>
@@ -4784,6 +4604,216 @@
     </rPh>
     <rPh sb="122" eb="123">
       <t>ト</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>広島大学のオンライン学習支援システム（広大moodle）にログインし、その中にある説明に従って多要素認証（MFA）の設定を行いましょう。</t>
+    <rPh sb="0" eb="4">
+      <t>ヒロシマダイガク</t>
+    </rPh>
+    <rPh sb="10" eb="14">
+      <t>ガクシュウシエン</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="37" eb="38">
+      <t>ナカ</t>
+    </rPh>
+    <rPh sb="41" eb="43">
+      <t>セツメイ</t>
+    </rPh>
+    <rPh sb="44" eb="45">
+      <t>シタガ</t>
+    </rPh>
+    <rPh sb="47" eb="52">
+      <t>タヨウソニンショウ</t>
+    </rPh>
+    <rPh sb="58" eb="60">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="61" eb="62">
+      <t>オコナ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>広大moodleへのログインと多要素認証（MFA）の設定</t>
+    <rPh sb="0" eb="2">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="15" eb="20">
+      <t>タヨウソニンショウ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>セッテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>大学で提供されているオンラインサービスはいくつもありますが、まずオンライン学習支援システムの広大moodleにログインしてみましょう。
+ &lt;ul&gt;
+&lt;li&gt;&lt;a href="#moodle"&gt;広大moodleにログインする&lt;/a&gt;
+&lt;/li&gt;
+&lt;li&gt;&lt;a href="#mfa"&gt;多要素認証(MFA)の設定&lt;/a&gt;
+&lt;/li&gt;
+ &lt;/ul&gt;</t>
+    <rPh sb="46" eb="48">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="96" eb="98">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="141" eb="146">
+      <t>タヨウソニンショウ</t>
+    </rPh>
+    <rPh sb="152" eb="154">
+      <t>セッテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;h2&gt;&lt;a name="moodle"&gt;&lt;/a&gt;広大moodle (オンライン学習支援システム)&lt;/h2&gt; </t>
+    <rPh sb="25" eb="27">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t>ガクシュウ</t>
+    </rPh>
+    <rPh sb="42" eb="44">
+      <t>シエン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>次のリンクから広島大学オンライン学習支援システム（広大moodle）にアクセスしてください。
+&lt;a href="https://moodle.vle.hiroshima-u.ac.jp/local/hulogin/"&gt;https://moodle.vle.hiroshima-u.ac.jp/local/hulogin/&lt;/a&gt;
+「広大IDでログイン」をクリックしましょう。</t>
+    <rPh sb="0" eb="1">
+      <t>ツギ</t>
+    </rPh>
+    <rPh sb="7" eb="11">
+      <t>ヒロシマダイガク</t>
+    </rPh>
+    <rPh sb="16" eb="20">
+      <t>ガクシュウシエン</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="166" eb="168">
+      <t>ヒロダイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>広大moodleの「コース概要」の中の「MFA21 MFA設定ガイド」をクリックして、まず表示される「広大IDとIMCアカウントの概要」を読んでください。</t>
+    <rPh sb="0" eb="2">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>ガイヨウ</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>ナカ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="51" eb="53">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="65" eb="67">
+      <t>ガイヨウ</t>
+    </rPh>
+    <rPh sb="69" eb="70">
+      <t>ヨ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>さらに下の方にある「IMCアカウントのMFA設定」の説明に従ってIMCアカウントの多要素認証（MFA）設定を行ってください。&lt;span class="check"&gt;check-9&lt;/span&gt;</t>
+    <rPh sb="3" eb="4">
+      <t>シタ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>ホウ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>セツメイ</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>シタガ</t>
+    </rPh>
+    <rPh sb="41" eb="46">
+      <t>タヨウソニンショウ</t>
+    </rPh>
+    <rPh sb="51" eb="53">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="54" eb="55">
+      <t>オコナ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>※ ここまでの実習の中で、広島大学には２つのオンライン学習支援システム「広大moodle」「Bb9」があることに気づかれたと思います。
+広島大学では今年度「広大moodle」「Bb9」の２つのオンライン学習支援システムを併用します。来年度からは「広大moodle」に一本化する予定です。
+しばらく面倒をおかけしますが、ご了解ください。</t>
+    <rPh sb="7" eb="9">
+      <t>ジッシュウ</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>ナカ</t>
+    </rPh>
+    <rPh sb="13" eb="17">
+      <t>ヒロシマダイガク</t>
+    </rPh>
+    <rPh sb="27" eb="31">
+      <t>ガクシュウシエン</t>
+    </rPh>
+    <rPh sb="36" eb="38">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="56" eb="57">
+      <t>キ</t>
+    </rPh>
+    <rPh sb="62" eb="63">
+      <t>オモ</t>
+    </rPh>
+    <rPh sb="78" eb="80">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="101" eb="105">
+      <t>ガクシュウシエン</t>
+    </rPh>
+    <rPh sb="110" eb="112">
+      <t>ヘイヨウ</t>
+    </rPh>
+    <rPh sb="116" eb="119">
+      <t>ライネンド</t>
+    </rPh>
+    <rPh sb="123" eb="125">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="133" eb="136">
+      <t>イッポンカ</t>
+    </rPh>
+    <rPh sb="138" eb="140">
+      <t>ヨテイ</t>
+    </rPh>
+    <rPh sb="148" eb="150">
+      <t>メンドウ</t>
+    </rPh>
+    <rPh sb="160" eb="162">
+      <t>リョウカイ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -5231,7 +5261,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -5292,7 +5322,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -5302,7 +5332,7 @@
     </row>
     <row r="7" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -5324,7 +5354,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -5417,7 +5447,7 @@
         <v>96</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5441,17 +5471,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -5459,30 +5489,30 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="D9" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="165.75" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -5548,7 +5578,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -5556,7 +5586,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -5570,7 +5600,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -5851,7 +5881,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6209,7 +6239,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="102" x14ac:dyDescent="0.25">
@@ -6245,7 +6275,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -6360,7 +6390,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6389,7 +6419,7 @@
     </row>
     <row r="6" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -6404,23 +6434,23 @@
     </row>
     <row r="9" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="D9" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="D10" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="D11" t="s">
         <v>192</v>
@@ -6566,7 +6596,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6598,7 +6628,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6689,7 +6719,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="102" x14ac:dyDescent="0.25">
@@ -6766,7 +6796,7 @@
     </row>
     <row r="12" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -6779,7 +6809,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
@@ -6793,7 +6823,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
@@ -6821,7 +6851,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
@@ -6852,7 +6882,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -6868,7 +6898,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>284</v>
+        <v>322</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6876,7 +6906,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>253</v>
+        <v>323</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6900,7 +6930,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>306</v>
+        <v>324</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6911,7 +6941,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>276</v>
+        <v>325</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -6919,7 +6949,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -6927,10 +6957,10 @@
     </row>
     <row r="9" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>315</v>
+        <v>326</v>
       </c>
       <c r="D9" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -6938,13 +6968,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="191.25" x14ac:dyDescent="0.25">
@@ -6952,18 +6982,18 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -6971,7 +7001,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>318</v>
+        <v>327</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -6982,7 +7012,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>257</v>
+        <v>328</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -6993,7 +7023,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -7055,7 +7085,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -7079,7 +7109,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
@@ -7111,7 +7141,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -7155,7 +7185,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -7168,7 +7198,7 @@
     </row>
     <row r="15" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D15" t="s">
         <v>170</v>
@@ -7404,7 +7434,7 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
@@ -7465,8 +7495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A687F900-5547-4D89-8494-B67FCE27BE96}">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="99" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -7482,7 +7512,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -7506,7 +7536,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="229.5" x14ac:dyDescent="0.25">
@@ -7514,7 +7544,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7567,7 +7597,7 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -7608,7 +7638,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -7619,7 +7649,7 @@
     </row>
     <row r="15" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="D15" t="s">
         <v>196</v>
@@ -7641,7 +7671,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -7649,13 +7679,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="C18" t="s">
         <v>53</v>
       </c>
       <c r="D18" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
@@ -7663,7 +7693,7 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -7721,13 +7751,13 @@
     </row>
     <row r="24" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -7735,13 +7765,13 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -7749,7 +7779,7 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
@@ -7782,7 +7812,7 @@
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
@@ -7793,7 +7823,7 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
@@ -7804,7 +7834,7 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
@@ -7818,7 +7848,7 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
@@ -7829,13 +7859,13 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -7843,7 +7873,7 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
@@ -7854,7 +7884,7 @@
     </row>
     <row r="35" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>312</v>
+        <v>329</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -7867,7 +7897,7 @@
         <v>4</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C38" t="s">
         <v>4</v>
@@ -7895,7 +7925,7 @@
         <v>4</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C40" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
add setup procedure of Edge win10(ja)
</commit_message>
<xml_diff>
--- a/macs+lan.xlsx
+++ b/macs+lan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hiroshimauniv-my.sharepoint.com/personal/kishiba_hiroshima-u_ac_jp/Documents/Documents/fresta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="383" documentId="13_ncr:1_{24C083B2-CEBE-46F8-A593-5C30BCD27FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07E1C0A6-8E46-442A-A03C-8249640C14CA}"/>
+  <xr:revisionPtr revIDLastSave="384" documentId="13_ncr:1_{24C083B2-CEBE-46F8-A593-5C30BCD27FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AFFCA3E0-FDD7-4672-BB7C-B18F2EC6D67D}"/>
   <bookViews>
-    <workbookView xWindow="13245" yWindow="-14655" windowWidth="17205" windowHeight="14160" tabRatio="772" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7635" yWindow="-14895" windowWidth="17205" windowHeight="14160" tabRatio="772" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -4556,42 +4556,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">自分の履修科目についての「Bb9」のコース全体を見ることもできます。もみじTOPページに戻って、今度は「Bb9」のバナーをクリックしましょう。
-&lt;strong&gt;※ 学外にいる場合はこの方法での「Bb9」へのログインはできません。項目[21]まで飛んでください。&lt;/strong&gt;
-</t>
-    <rPh sb="0" eb="2">
-      <t>ジブン</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>リシュウ</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>カモク</t>
-    </rPh>
-    <rPh sb="21" eb="23">
-      <t>ゼンタイ</t>
-    </rPh>
-    <rPh sb="24" eb="25">
-      <t>ミ</t>
-    </rPh>
-    <rPh sb="82" eb="84">
-      <t>ガクガイ</t>
-    </rPh>
-    <rPh sb="87" eb="89">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="92" eb="94">
-      <t>ホウホウ</t>
-    </rPh>
-    <rPh sb="114" eb="116">
-      <t>コウモク</t>
-    </rPh>
-    <rPh sb="122" eb="123">
-      <t>ト</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>広島大学のオンライン学習支援システム（広大moodle）にログインし、その中にある説明に従って多要素認証（MFA）の設定を行いましょう。</t>
     <rPh sb="0" eb="4">
       <t>ヒロシマダイガク</t>
@@ -4887,6 +4851,42 @@
     </rPh>
     <rPh sb="160" eb="162">
       <t>サンショウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">自分の履修科目についての「Bb9」のコース全体を見ることもできます。もみじTOPページに戻って、今度は「Bb9」のバナーをクリックしましょう。
+&lt;strong&gt;※ 学外にいる場合はこの方法での「Bb9」へのログインはできません。項目[22]まで飛んでください。&lt;/strong&gt;
+</t>
+    <rPh sb="0" eb="2">
+      <t>ジブン</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>リシュウ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>カモク</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>ゼンタイ</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>ミ</t>
+    </rPh>
+    <rPh sb="82" eb="84">
+      <t>ガクガイ</t>
+    </rPh>
+    <rPh sb="87" eb="89">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="92" eb="94">
+      <t>ホウホウ</t>
+    </rPh>
+    <rPh sb="114" eb="116">
+      <t>コウモク</t>
+    </rPh>
+    <rPh sb="122" eb="123">
+      <t>ト</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -6971,7 +6971,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6979,7 +6979,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7003,7 +7003,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7014,7 +7014,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -7030,7 +7030,7 @@
     </row>
     <row r="9" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D9" t="s">
         <v>306</v>
@@ -7074,7 +7074,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -7085,7 +7085,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -7568,8 +7568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A687F900-5547-4D89-8494-B67FCE27BE96}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B23" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="B34" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -7849,10 +7849,10 @@
     </row>
     <row r="26" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D26" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -7860,7 +7860,7 @@
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
@@ -7915,7 +7915,7 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
@@ -7940,7 +7940,7 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>319</v>
+        <v>331</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
@@ -7965,7 +7965,7 @@
     </row>
     <row r="36" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix text title of all
</commit_message>
<xml_diff>
--- a/macs+lan.xlsx
+++ b/macs+lan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hiroshimauniv-my.sharepoint.com/personal/kishiba_hiroshima-u_ac_jp/Documents/Documents/fresta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="384" documentId="13_ncr:1_{24C083B2-CEBE-46F8-A593-5C30BCD27FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AFFCA3E0-FDD7-4672-BB7C-B18F2EC6D67D}"/>
+  <xr:revisionPtr revIDLastSave="385" documentId="13_ncr:1_{24C083B2-CEBE-46F8-A593-5C30BCD27FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A54CC814-93B9-448C-BB53-BE7C06E1D493}"/>
   <bookViews>
-    <workbookView xWindow="7635" yWindow="-14895" windowWidth="17205" windowHeight="14160" tabRatio="772" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3308" yWindow="3308" windowWidth="18225" windowHeight="11872" tabRatio="772" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -2966,19 +2966,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>広島大学必携PC初期実習（自習用テキスト）</t>
-    <rPh sb="10" eb="12">
-      <t>ジッシュウ</t>
-    </rPh>
-    <rPh sb="13" eb="15">
-      <t>ジシュウ</t>
-    </rPh>
-    <rPh sb="15" eb="16">
-      <t>ヨウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>FRESTA-TEXT-2022 Mac chap.0</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -4887,6 +4874,16 @@
     </rPh>
     <rPh sb="122" eb="123">
       <t>ト</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>広島大学 2022年度 必携PC初期実習テキスト</t>
+    <rPh sb="9" eb="11">
+      <t>ネンド</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>ジッシュウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -5279,8 +5276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -5296,7 +5293,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>246</v>
+        <v>331</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5334,7 +5331,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -5395,7 +5392,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -5405,7 +5402,7 @@
     </row>
     <row r="7" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -5427,7 +5424,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -5520,7 +5517,7 @@
         <v>96</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5544,17 +5541,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -5562,30 +5559,30 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="165.75" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -5651,7 +5648,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -5659,7 +5656,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -5673,7 +5670,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -5946,7 +5943,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
@@ -5954,7 +5951,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6312,7 +6309,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="102" x14ac:dyDescent="0.25">
@@ -6348,7 +6345,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -6362,7 +6359,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -6463,7 +6460,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6487,43 +6484,43 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D10" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D11" t="s">
         <v>192</v>
@@ -6669,7 +6666,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6693,7 +6690,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -6701,7 +6698,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6792,7 +6789,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="102" x14ac:dyDescent="0.25">
@@ -6869,7 +6866,7 @@
     </row>
     <row r="12" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -6882,7 +6879,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
@@ -6896,7 +6893,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
@@ -6924,7 +6921,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
@@ -6971,7 +6968,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6979,7 +6976,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7003,7 +7000,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7014,7 +7011,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -7022,7 +7019,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -7030,10 +7027,10 @@
     </row>
     <row r="9" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -7041,13 +7038,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="191.25" x14ac:dyDescent="0.25">
@@ -7055,18 +7052,18 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -7074,7 +7071,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -7085,7 +7082,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -7096,7 +7093,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -7158,7 +7155,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -7182,7 +7179,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
@@ -7214,7 +7211,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -7258,7 +7255,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -7271,7 +7268,7 @@
     </row>
     <row r="15" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D15" t="s">
         <v>170</v>
@@ -7507,7 +7504,7 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
@@ -7568,7 +7565,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A687F900-5547-4D89-8494-B67FCE27BE96}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B34" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="B34" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
@@ -7585,7 +7582,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -7609,7 +7606,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="229.5" x14ac:dyDescent="0.25">
@@ -7617,7 +7614,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7670,7 +7667,7 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -7711,7 +7708,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -7722,7 +7719,7 @@
     </row>
     <row r="15" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D15" t="s">
         <v>196</v>
@@ -7744,7 +7741,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -7752,13 +7749,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C18" t="s">
         <v>53</v>
       </c>
       <c r="D18" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
@@ -7766,7 +7763,7 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -7824,13 +7821,13 @@
     </row>
     <row r="24" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -7838,21 +7835,21 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D26" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -7860,7 +7857,7 @@
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
@@ -7893,7 +7890,7 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
@@ -7904,7 +7901,7 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
@@ -7915,7 +7912,7 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
@@ -7929,7 +7926,7 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
@@ -7940,13 +7937,13 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -7954,7 +7951,7 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
@@ -7965,7 +7962,7 @@
     </row>
     <row r="36" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -7978,7 +7975,7 @@
         <v>4</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C39" t="s">
         <v>4</v>
@@ -8006,7 +8003,7 @@
         <v>4</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C41" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
omit cautioh for MFA Hirodai ID
</commit_message>
<xml_diff>
--- a/macs+lan.xlsx
+++ b/macs+lan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hiroshimauniv-my.sharepoint.com/personal/kishiba_hiroshima-u_ac_jp/Documents/Documents/fresta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="416" documentId="13_ncr:1_{24C083B2-CEBE-46F8-A593-5C30BCD27FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E64E108-858A-41D1-9E00-C4AD4BDB1FD2}"/>
+  <xr:revisionPtr revIDLastSave="417" documentId="13_ncr:1_{24C083B2-CEBE-46F8-A593-5C30BCD27FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E1D550C-636C-4DD1-94BE-4A4BFACA2F94}"/>
   <bookViews>
-    <workbookView xWindow="5190" yWindow="4118" windowWidth="18225" windowHeight="11872" tabRatio="772" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6030" yWindow="-15765" windowWidth="21600" windowHeight="11595" tabRatio="772" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -5129,8 +5129,8 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>教材の下の方にある「広大IDのMFA利用設定実習」をクリックして、説明に従って広大IDの多要素認証（MFA）設定を進めましょう。詳細は教材の各項目の資料を見てください。&lt;span class="check"&gt;check-10&lt;/span&gt;
-※ 学外から設定する場合は第７章に説明のある「VPN」を使います。もしVPNの使用が難しい場合は、残りの設定はあとで学内ネットワークに接続してから行いましょう。</t>
+    <t xml:space="preserve">教材の下の方にある「広大IDのMFA利用設定実習」をクリックして、説明に従って広大IDの多要素認証（MFA）設定を進めましょう。詳細は教材の各項目の資料を見てください。&lt;span class="check"&gt;check-10&lt;/span&gt;
+</t>
     <rPh sb="0" eb="2">
       <t>キョウザイ</t>
     </rPh>
@@ -5169,39 +5169,6 @@
     </rPh>
     <rPh sb="77" eb="78">
       <t>ミ</t>
-    </rPh>
-    <rPh sb="122" eb="124">
-      <t>ガクガイ</t>
-    </rPh>
-    <rPh sb="126" eb="128">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="130" eb="132">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="159" eb="161">
-      <t>シヨウ</t>
-    </rPh>
-    <rPh sb="162" eb="163">
-      <t>ムズカ</t>
-    </rPh>
-    <rPh sb="165" eb="167">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="169" eb="170">
-      <t>ノコ</t>
-    </rPh>
-    <rPh sb="172" eb="174">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="178" eb="180">
-      <t>ガクナイ</t>
-    </rPh>
-    <rPh sb="187" eb="189">
-      <t>セツゾク</t>
-    </rPh>
-    <rPh sb="193" eb="194">
-      <t>オコナ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -7279,7 +7246,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B17" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -7488,7 +7455,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="51" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
mac: office install update
</commit_message>
<xml_diff>
--- a/macs+lan.xlsx
+++ b/macs+lan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8179045-D32B-4DBC-AE37-347E52492229}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69724849-E347-4B6F-B8CE-CFC6BE6CE0F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6036" yWindow="-15768" windowWidth="9324" windowHeight="11592" tabRatio="772" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="399">
   <si>
     <t>header1</t>
   </si>
@@ -219,10 +219,6 @@
   </si>
   <si>
     <t xml:space="preserve">  いろんな設定をするためのアイコンが並んでいます。 「ソフトウェア・アップデート」をクリックしてください。  </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> このパソコンに入っているアプリケーションのアイコンがずらっと表示されます。 この中から、Officeに含まれるアプリを起動しましょう。どれでもよいのですが、ここではMicrosoft Wordを起動します。  </t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -5829,72 +5825,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>起動した時に、左下に「ライセンス認証」のアイコンが出ている場合は、以下の手順に従って認証してください。もし無かった場合は、&lt;a href="#check_activation"&gt;この章の末尾の手順&lt;/a&gt;に従ってライセンス認証ずみであることを確認してください。</t>
-    <rPh sb="0" eb="2">
-      <t>キドウ</t>
-    </rPh>
-    <rPh sb="4" eb="5">
-      <t>トキ</t>
-    </rPh>
-    <rPh sb="7" eb="9">
-      <t>ヒダリシタ</t>
-    </rPh>
-    <rPh sb="16" eb="18">
-      <t>ニンショウ</t>
-    </rPh>
-    <rPh sb="25" eb="26">
-      <t>デ</t>
-    </rPh>
-    <rPh sb="29" eb="31">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="33" eb="35">
-      <t>イカ</t>
-    </rPh>
-    <rPh sb="36" eb="38">
-      <t>テジュン</t>
-    </rPh>
-    <rPh sb="39" eb="40">
-      <t>シタガ</t>
-    </rPh>
-    <rPh sb="42" eb="44">
-      <t>ニンショウ</t>
-    </rPh>
-    <rPh sb="53" eb="54">
-      <t>ナ</t>
-    </rPh>
-    <rPh sb="57" eb="59">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="91" eb="92">
-      <t>ショウ</t>
-    </rPh>
-    <rPh sb="93" eb="95">
-      <t>マツビ</t>
-    </rPh>
-    <rPh sb="96" eb="98">
-      <t>テジュン</t>
-    </rPh>
-    <rPh sb="103" eb="104">
-      <t>シタガ</t>
-    </rPh>
-    <rPh sb="111" eb="113">
-      <t>ニンショウ</t>
-    </rPh>
-    <rPh sb="121" eb="123">
-      <t>カクニン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">「今すぐWordを使ってみる」をクリックしてください。  </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">次に、Officeのライセンス認証をします。ソフトウェアが正当なコピーであることを確認し、PCで使えるようにするための処理です。 Dockの中から、ロケットのアイコンの「Launchpad」をクリックしてください。  </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Microsoft365のインストールが終わると、少しして勝手に②のような更新ウィンドウが開いてMicrosoft365のアップデートが自動的に開始されます。この時タスクバーに①のような更新中のアイコンが出てきますが、後で操作しますので、今は放置しておきます。</t>
     <rPh sb="20" eb="21">
       <t>オ</t>
@@ -5938,11 +5868,6 @@
     <rPh sb="121" eb="123">
       <t>ホウチ</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Wordの新規作成の画面が開きました。 これで、PowerPointやExcelなどMicrosoft Officeの他のアプリケーションも使えるようになります。&lt;span class="check"&gt;check-12&lt;/span&gt;
-  </t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -6055,6 +5980,81 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>するとOfficeアプリの概要を示すダイヤログが表示されます。「ライセンス」の行を確認してください。</t>
+  </si>
+  <si>
+    <t>「Microsoftのアプリを自動で常に最新の状態にする」(①)にチェックを入れた上で、「更新プログラムを確認」(②)をクリックします。</t>
+    <rPh sb="15" eb="17">
+      <t>ジドウ</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>ツネ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>サイシン</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>ジョウタイ</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t>イ</t>
+    </rPh>
+    <rPh sb="41" eb="42">
+      <t>ウエ</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>コウシン</t>
+    </rPh>
+    <rPh sb="53" eb="55">
+      <t>カクニン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>メニューの「Microsoft Autoupdateを終了します」をクリックすると、終了できます。 ウィンドウを閉じるのでも構いません。</t>
+    <rPh sb="56" eb="57">
+      <t>ト</t>
+    </rPh>
+    <rPh sb="62" eb="63">
+      <t>カマ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>次に、Officeのライセンス認証をします。ソフトウェアが正当なコピーであることを確認し、PCで使えるようにするための処理です。 Dockの中から、「Launchpad」を起動してください。 アイコンはmacOSのバージョンごとに頻繁に変わるので、マウスで指したときのツールチップに出てくる名前で探すのがよいでしょう。</t>
+    <rPh sb="86" eb="88">
+      <t>キドウ</t>
+    </rPh>
+    <rPh sb="115" eb="117">
+      <t>ヒンパン</t>
+    </rPh>
+    <rPh sb="118" eb="119">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="128" eb="129">
+      <t>サ</t>
+    </rPh>
+    <rPh sb="141" eb="142">
+      <t>デ</t>
+    </rPh>
+    <rPh sb="145" eb="147">
+      <t>ナマエ</t>
+    </rPh>
+    <rPh sb="148" eb="149">
+      <t>サガ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">「今すぐExcelを使ってみる」をクリックしてください。  </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Excelの新規作成の画面が開きました。 これで、PowerPointやWordなどMicrosoft Officeの他のアプリケーションも使えるようになります。&lt;span class="check"&gt;check-12&lt;/span&gt;
+  </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>ここではOfficeのライセンス状況確認手順を説明します。Officeのソフトのどれかを起動し、メニューバーのアプリ名(Wordを起動したなら「Word」、Excelを起動したなら「Excel」)をクリックして展開し、「概要」または「バージョン情報」選びます。</t>
     <rPh sb="16" eb="18">
       <t>ジョウキョウ</t>
@@ -6068,70 +6068,172 @@
     <rPh sb="23" eb="25">
       <t>セツメイ</t>
     </rPh>
-    <rPh sb="44" eb="46">
+    <rPh sb="48" eb="50">
       <t>キドウ</t>
     </rPh>
-    <rPh sb="58" eb="59">
+    <rPh sb="62" eb="63">
       <t>メイ</t>
     </rPh>
-    <rPh sb="65" eb="67">
+    <rPh sb="69" eb="71">
       <t>キドウ</t>
     </rPh>
+    <rPh sb="88" eb="90">
+      <t>キドウ</t>
+    </rPh>
+    <rPh sb="109" eb="111">
+      <t>テンカイ</t>
+    </rPh>
+    <rPh sb="114" eb="116">
+      <t>ガイヨウ</t>
+    </rPh>
+    <rPh sb="126" eb="128">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="129" eb="130">
+      <t>エラ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> このパソコンに入っているアプリケーションのアイコンがずらっと表示されます。 この中から、Officeに含まれるアプリを起動しましょう。どれでもよいのですが、このテキストの例ではMicrosoft Excelを起動します。 見当たらない場合はLaunchpadの上部にある検索フォームに「Excel」と入力して検索しましょう。</t>
+    <rPh sb="86" eb="87">
+      <t>レイ</t>
+    </rPh>
+    <rPh sb="112" eb="114">
+      <t>ミア</t>
+    </rPh>
+    <rPh sb="118" eb="120">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="131" eb="133">
+      <t>ウエブ</t>
+    </rPh>
+    <rPh sb="136" eb="138">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="151" eb="153">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="155" eb="157">
+      <t>ケンサク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「Microsoftはお客様のプライバシーの保護に～」などと出てくることがありますが、「次へ」を押すしか選択肢がありません。</t>
+    <rPh sb="12" eb="14">
+      <t>キャクサマ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>ホゴ</t>
+    </rPh>
+    <rPh sb="30" eb="31">
+      <t>デ</t>
+    </rPh>
+    <rPh sb="44" eb="45">
+      <t>ツギ</t>
+    </rPh>
+    <rPh sb="48" eb="49">
+      <t>オ</t>
+    </rPh>
+    <rPh sb="52" eb="55">
+      <t>センタクシ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mac-4-7a.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mac-4-7b.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mac-4-7c.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「一緒に進歩する」というダイヤログが出てくることがありますが、これはユーザのデータをMicrosoftに送るかどうかという選択です。少しでもプライバシーを守るため拒否を選択し(①)、「承諾」(②)で進めましょう。</t>
+    <rPh sb="1" eb="3">
+      <t>イッショ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>シンポ</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>デ</t>
+    </rPh>
+    <rPh sb="52" eb="53">
+      <t>オク</t>
+    </rPh>
+    <rPh sb="61" eb="63">
+      <t>センタク</t>
+    </rPh>
+    <rPh sb="66" eb="67">
+      <t>スコ</t>
+    </rPh>
+    <rPh sb="77" eb="78">
+      <t>マモ</t>
+    </rPh>
+    <rPh sb="81" eb="83">
+      <t>キョヒ</t>
+    </rPh>
     <rPh sb="84" eb="86">
-      <t>キドウ</t>
-    </rPh>
-    <rPh sb="105" eb="107">
-      <t>テンカイ</t>
-    </rPh>
-    <rPh sb="110" eb="112">
-      <t>ガイヨウ</t>
-    </rPh>
-    <rPh sb="122" eb="124">
-      <t>ジョウホウ</t>
-    </rPh>
-    <rPh sb="125" eb="126">
-      <t>エラ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>するとOfficeアプリの概要を示すダイヤログが表示されます。「ライセンス」の行を確認してください。</t>
-  </si>
-  <si>
-    <t>「Microsoftのアプリを自動で常に最新の状態にする」(①)にチェックを入れた上で、「更新プログラムを確認」(②)をクリックします。</t>
-    <rPh sb="15" eb="17">
-      <t>ジドウ</t>
-    </rPh>
-    <rPh sb="18" eb="19">
-      <t>ツネ</t>
-    </rPh>
-    <rPh sb="20" eb="22">
-      <t>サイシン</t>
-    </rPh>
-    <rPh sb="23" eb="25">
-      <t>ジョウタイ</t>
-    </rPh>
-    <rPh sb="38" eb="39">
-      <t>イ</t>
-    </rPh>
-    <rPh sb="41" eb="42">
-      <t>ウエ</t>
+      <t>センタク</t>
+    </rPh>
+    <rPh sb="92" eb="94">
+      <t>ショウダク</t>
+    </rPh>
+    <rPh sb="99" eb="100">
+      <t>スス</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「エクスペリエンスの強化」というダイヤログが出てくることがありますが、あとでプライバシーの設定をしますので、「完了」をで進めます。</t>
+    <rPh sb="10" eb="12">
+      <t>キョウカ</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>デ</t>
     </rPh>
     <rPh sb="45" eb="47">
-      <t>コウシン</t>
-    </rPh>
-    <rPh sb="53" eb="55">
-      <t>カクニン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>メニューの「Microsoft Autoupdateを終了します」をクリックすると、終了できます。 ウィンドウを閉じるのでも構いません。</t>
-    <rPh sb="56" eb="57">
-      <t>ト</t>
-    </rPh>
-    <rPh sb="62" eb="63">
-      <t>カマ</t>
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="55" eb="57">
+      <t>カンリョウ</t>
+    </rPh>
+    <rPh sb="60" eb="61">
+      <t>スス</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Excelで新規ファイル作成のウィンドウになりますが、広大の包括ライセンスでインストールした場合、左下に「ライセンス認証」のマークが出ています。</t>
+    <rPh sb="6" eb="8">
+      <t>シンキ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>サクセイ</t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>ホウカツ</t>
+    </rPh>
+    <rPh sb="46" eb="48">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="49" eb="51">
+      <t>ヒダリシタ</t>
+    </rPh>
+    <rPh sb="58" eb="60">
+      <t>ニンショウ</t>
+    </rPh>
+    <rPh sb="66" eb="67">
+      <t>デ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -6553,7 +6655,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6569,7 +6671,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -6577,7 +6679,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -6591,7 +6693,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6652,17 +6754,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -6670,13 +6772,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
@@ -6684,13 +6786,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6718,7 +6820,7 @@
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -6732,7 +6834,7 @@
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -6740,7 +6842,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -6774,10 +6876,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6801,17 +6903,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6819,33 +6921,33 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D10" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="171.6" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -6887,7 +6989,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6895,7 +6997,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6911,7 +7013,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -6919,7 +7021,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6933,7 +7035,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -6943,13 +7045,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6957,24 +7059,24 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -6982,13 +7084,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -6996,40 +7098,40 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C16" t="s">
         <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -7037,13 +7139,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C18" t="s">
         <v>8</v>
       </c>
       <c r="D18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7051,24 +7153,24 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
       </c>
       <c r="D19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="92.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -7076,13 +7178,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C21" t="s">
         <v>8</v>
       </c>
       <c r="D21" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7090,35 +7192,35 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C22" t="s">
         <v>8</v>
       </c>
       <c r="D22" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C23" t="s">
         <v>8</v>
       </c>
       <c r="D23" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C24" t="s">
         <v>8</v>
       </c>
       <c r="D24" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7126,13 +7228,13 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C25" t="s">
         <v>8</v>
       </c>
       <c r="D25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -7140,18 +7242,18 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C26" t="s">
         <v>8</v>
       </c>
       <c r="D26" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -7182,7 +7284,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7206,7 +7308,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
@@ -7214,7 +7316,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7234,7 +7336,7 @@
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7242,13 +7344,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7256,24 +7358,24 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7281,13 +7383,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7295,13 +7397,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7315,18 +7417,18 @@
         <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7334,13 +7436,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
       </c>
       <c r="D15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -7354,7 +7456,7 @@
         <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7368,7 +7470,7 @@
         <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
@@ -7376,134 +7478,134 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C18" t="s">
         <v>8</v>
       </c>
       <c r="D18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
       </c>
       <c r="D19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C20" t="s">
         <v>8</v>
       </c>
       <c r="D20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C21" t="s">
         <v>8</v>
       </c>
       <c r="D21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C22" t="s">
         <v>8</v>
       </c>
       <c r="D22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C23" t="s">
         <v>8</v>
       </c>
       <c r="D23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C24" t="s">
         <v>8</v>
       </c>
       <c r="D24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C25" t="s">
         <v>8</v>
       </c>
       <c r="D25" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C26" t="s">
         <v>8</v>
       </c>
       <c r="D26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C27" t="s">
         <v>8</v>
       </c>
       <c r="D27" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C28" t="s">
         <v>8</v>
       </c>
       <c r="D28" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C29" t="s">
         <v>8</v>
       </c>
       <c r="D29" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7511,13 +7613,13 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C30" t="s">
         <v>8</v>
       </c>
       <c r="D30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -7572,7 +7674,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
@@ -7580,7 +7682,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7594,13 +7696,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7608,13 +7710,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7622,21 +7724,21 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="D10" t="s">
         <v>363</v>
-      </c>
-      <c r="D10" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -7644,13 +7746,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -7658,24 +7760,24 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" t="s">
         <v>118</v>
-      </c>
-      <c r="C13" t="s">
-        <v>76</v>
-      </c>
-      <c r="D13" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7683,24 +7785,24 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
       </c>
       <c r="D15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -7731,7 +7833,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7739,7 +7841,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7755,54 +7857,54 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7810,18 +7912,18 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
         <v>154</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7829,10 +7931,10 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="D15" t="s">
         <v>324</v>
-      </c>
-      <c r="D15" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7840,26 +7942,26 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D16" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D17" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="D18" t="s">
         <v>349</v>
-      </c>
-      <c r="D18" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7867,10 +7969,10 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D19" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7878,10 +7980,10 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D20" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7889,18 +7991,18 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D21" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D22" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7908,10 +8010,10 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D23" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7919,10 +8021,10 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D24" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -7930,10 +8032,10 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D25" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7941,10 +8043,10 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D26" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7952,10 +8054,10 @@
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D27" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7963,10 +8065,10 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D28" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7974,10 +8076,10 @@
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D29" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7985,10 +8087,10 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="D30" t="s">
         <v>342</v>
-      </c>
-      <c r="D30" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -7996,10 +8098,10 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D31" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -8007,15 +8109,15 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D33" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
   </sheetData>
@@ -8046,7 +8148,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8054,7 +8156,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8070,7 +8172,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8078,7 +8180,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8089,18 +8191,18 @@
     </row>
     <row r="7" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -8108,13 +8210,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -8145,7 +8247,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8153,7 +8255,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8169,7 +8271,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -8177,7 +8279,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8224,34 +8326,34 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8259,7 +8361,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
@@ -8273,7 +8375,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
@@ -8287,7 +8389,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C16" t="s">
         <v>8</v>
@@ -8301,7 +8403,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
@@ -8348,7 +8450,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8356,7 +8458,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8372,7 +8474,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="132" x14ac:dyDescent="0.2">
@@ -8380,7 +8482,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8391,12 +8493,12 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -8409,7 +8511,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -8420,18 +8522,18 @@
     </row>
     <row r="11" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
         <v>262</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8439,29 +8541,29 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
         <v>265</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D14" t="s">
         <v>267</v>
-      </c>
-      <c r="D14" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D15" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -8469,13 +8571,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="198" x14ac:dyDescent="0.2">
@@ -8483,18 +8585,18 @@
         <v>4</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
         <v>270</v>
-      </c>
-      <c r="C17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8502,21 +8604,21 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
         <v>272</v>
-      </c>
-      <c r="C19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D20" t="s">
         <v>274</v>
-      </c>
-      <c r="D20" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8524,21 +8626,21 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
         <v>276</v>
-      </c>
-      <c r="C21" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="D22" t="s">
         <v>278</v>
-      </c>
-      <c r="D22" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8546,13 +8648,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -8592,10 +8694,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -8603,7 +8705,7 @@
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="100.6640625" style="4" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="4" max="4" width="34.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -8611,7 +8713,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8619,7 +8721,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8635,7 +8737,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -8643,7 +8745,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8654,12 +8756,12 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="132" x14ac:dyDescent="0.2">
@@ -8667,13 +8769,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -8681,10 +8783,10 @@
         <v>4</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8692,7 +8794,7 @@
         <v>48</v>
       </c>
       <c r="D11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8700,58 +8802,58 @@
         <v>4</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
         <v>130</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B14" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D14" t="s">
         <v>132</v>
-      </c>
-      <c r="D14" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B15" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B16" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D16" t="s">
         <v>135</v>
-      </c>
-      <c r="D16" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B17" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D18" t="s">
         <v>139</v>
-      </c>
-      <c r="D18" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8759,13 +8861,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -8779,7 +8881,7 @@
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -8787,13 +8889,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -8801,13 +8903,13 @@
         <v>4</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8815,13 +8917,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8829,34 +8931,34 @@
         <v>4</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B25" s="4" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="D25" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>4</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
@@ -8865,12 +8967,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>4</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>53</v>
+        <v>391</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
@@ -8879,141 +8981,165 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B29" s="4" t="s">
-        <v>379</v>
+        <v>392</v>
       </c>
       <c r="D29" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="66" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>4</v>
-      </c>
+        <v>393</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B30" s="4" t="s">
-        <v>376</v>
-      </c>
-      <c r="C30" t="s">
-        <v>4</v>
+        <v>396</v>
       </c>
       <c r="D30" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="D31" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B32" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="D32" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="66" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>4</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>380</v>
-      </c>
-      <c r="C31" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="C33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="C34" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>4</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>383</v>
-      </c>
-      <c r="C32" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" t="s">
+    <row r="35" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B33" s="4" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="55.8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="4" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="55.8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="4" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B36" s="4" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>4</v>
-      </c>
+        <v>381</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B37" s="4" t="s">
-        <v>387</v>
-      </c>
-      <c r="C37" t="s">
-        <v>4</v>
-      </c>
-      <c r="D37" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B38" s="4" t="s">
-        <v>391</v>
-      </c>
-      <c r="D38" t="s">
-        <v>313</v>
+        <v>384</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B39" s="4" t="s">
-        <v>371</v>
-      </c>
-      <c r="D39" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>4</v>
+      </c>
       <c r="B40" s="4" t="s">
-        <v>372</v>
+        <v>382</v>
+      </c>
+      <c r="C40" t="s">
+        <v>4</v>
       </c>
       <c r="D40" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B41" s="4" t="s">
-        <v>373</v>
+        <v>385</v>
       </c>
       <c r="D41" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B42" s="4" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="D42" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>4</v>
-      </c>
       <c r="B43" s="4" t="s">
-        <v>392</v>
-      </c>
-      <c r="C43" t="s">
-        <v>4</v>
+        <v>371</v>
       </c>
       <c r="D43" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B44" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="D44" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B45" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="D45" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="C46" t="s">
+        <v>4</v>
+      </c>
+      <c r="D46" t="s">
         <v>34</v>
       </c>
     </row>
@@ -9045,7 +9171,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -9069,7 +9195,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="264" x14ac:dyDescent="0.2">
@@ -9077,7 +9203,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -9096,13 +9222,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -9115,64 +9241,64 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
         <v>284</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D11" t="s">
         <v>286</v>
-      </c>
-      <c r="D11" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="D12" t="s">
         <v>288</v>
-      </c>
-      <c r="D12" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D13" t="s">
         <v>290</v>
-      </c>
-      <c r="D13" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B14" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="D15" t="s">
         <v>293</v>
-      </c>
-      <c r="D15" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
         <v>295</v>
-      </c>
-      <c r="C16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -9183,7 +9309,7 @@
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -9193,13 +9319,13 @@
     </row>
     <row r="19" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -9207,21 +9333,21 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D21" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -9229,13 +9355,13 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
         <v>298</v>
-      </c>
-      <c r="C22" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -9248,7 +9374,7 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
@@ -9256,24 +9382,24 @@
     </row>
     <row r="25" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" t="s">
         <v>300</v>
-      </c>
-      <c r="C25" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
         <v>302</v>
-      </c>
-      <c r="C26" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -9281,7 +9407,7 @@
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
@@ -9295,7 +9421,7 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
@@ -9306,13 +9432,13 @@
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" t="s">
         <v>306</v>
-      </c>
-      <c r="C29" t="s">
-        <v>4</v>
-      </c>
-      <c r="D29" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -9320,7 +9446,7 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -9333,7 +9459,7 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
@@ -9361,7 +9487,7 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C35" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
moodle -> HIRODAI moodle
</commit_message>
<xml_diff>
--- a/macs+lan.xlsx
+++ b/macs+lan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57BA4FC0-34EC-4020-AB3D-0D6AE5B0041B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8B2292-FE25-4F3E-B331-9E8B179A9DAC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6036" yWindow="-15768" windowWidth="9324" windowHeight="11592" tabRatio="772" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6036" yWindow="-15768" windowWidth="9324" windowHeight="11592" tabRatio="772" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -6274,20 +6274,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">右側にある「moodle」のバナーをクリックして、広島大学オンライン学習支援システムのページに進みます。
-  </t>
-    <rPh sb="25" eb="29">
-      <t>ヒロシマダイガク</t>
-    </rPh>
-    <rPh sb="34" eb="38">
-      <t>ガクシュウシエン</t>
-    </rPh>
-    <rPh sb="47" eb="48">
-      <t>スス</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>momiji-moodle.png</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -6353,6 +6339,23 @@
     </rPh>
     <rPh sb="191" eb="193">
       <t>ヒロダイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">右側にある「広大 moodle」のバナーをクリックして、広島大学オンライン学習支援システムのページに進みます。
+  </t>
+    <rPh sb="6" eb="8">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="28" eb="32">
+      <t>ヒロシマダイガク</t>
+    </rPh>
+    <rPh sb="37" eb="41">
+      <t>ガクシュウシエン</t>
+    </rPh>
+    <rPh sb="50" eb="51">
+      <t>スス</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -6978,7 +6981,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -7042,7 +7045,7 @@
     </row>
     <row r="9" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D9" t="s">
         <v>221</v>
@@ -8581,8 +8584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -8689,13 +8692,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
         <v>391</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -9333,7 +9336,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -9365,7 +9368,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -9384,7 +9387,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -9517,7 +9520,7 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
remove references printer figure (win10-6-24a.svg)
</commit_message>
<xml_diff>
--- a/macs+lan.xlsx
+++ b/macs+lan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C29A5BC-94B3-4AF0-B8DD-EC798959FC55}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F5DC3F-D227-4F6F-BCA5-0F3B6D684AC4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6036" yWindow="-15768" windowWidth="9324" windowHeight="11592" tabRatio="772" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="397">
   <si>
     <t>header1</t>
   </si>
@@ -165,18 +165,6 @@
   <si>
     <t xml:space="preserve">Office365にサインインする画面になります。まず「IMCアカウント名@hiroshima-u.ac.jp」を記入し「次へ」をクリックします。
 </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">まず、大学のプリンタへの印刷について。
-学内ネットワークからであれば、必携PCから大学のプリンタへ印刷できます。印刷したいものをPDFで用意し、Webブラウザで印刷用のWebサーバに送ります。そのあと、プリンタが設置してあるところに行って、印刷操作をしてください。その際、印刷料金がかかります。白黒印刷は1枚4円、カラー印刷は1枚13円です。MYple（学生証にチャージする生協の電子マネー）で支払ってください。 
-詳細はメディアセンターWebサイトの&lt;a href="https://www.media.hiroshima-u.ac.jp/services/print/webprint"&gt;「Webプリントサービス」&lt;/a&gt;
-で。
-  </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win10-6-24a.svg</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -6468,6 +6456,13 @@
     <t xml:space="preserve">ここにはひとりあたり3TBまで、データを置いておくことができます。
 データのバックアップをとっておいたり、外出先でもデータを取り出したりできるようになるので、活用しましょう。
 OneDriveにもアプリがありますので、スマホでも活用できます。
+  </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">まず、大学のプリンタへの印刷について。
+学内ネットワークからであれば、必携PCから大学のプリンタへ印刷できます。印刷したいものをPDFで用意し、Webブラウザで印刷用のWebサーバに送ります。そのあと、プリンタが設置してあるところに行って、印刷操作をしてください(料金がかかります)。詳細はメディアセンターWebサイトの&lt;a href="https://www.media.hiroshima-u.ac.jp/services/print/webprint"&gt;「Webプリントサービス」&lt;/a&gt;
+で。
   </t>
     <phoneticPr fontId="1"/>
   </si>
@@ -6889,7 +6884,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6905,7 +6900,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -6913,7 +6908,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -6927,7 +6922,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6988,17 +6983,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7006,7 +7001,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -7017,13 +7012,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7031,7 +7026,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -7045,13 +7040,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -7059,13 +7054,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -7073,7 +7068,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -7107,10 +7102,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7134,17 +7129,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7152,33 +7147,33 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D9" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D10" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="171.6" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -7220,7 +7215,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7228,7 +7223,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7244,7 +7239,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -7252,7 +7247,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7266,7 +7261,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -7276,13 +7271,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7290,24 +7285,24 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -7315,13 +7310,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -7329,40 +7324,40 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C16" t="s">
         <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -7370,13 +7365,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C18" t="s">
         <v>8</v>
       </c>
       <c r="D18" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7384,24 +7379,24 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
       </c>
       <c r="D19" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="92.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D20" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -7409,13 +7404,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C21" t="s">
         <v>8</v>
       </c>
       <c r="D21" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7423,35 +7418,35 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C22" t="s">
         <v>8</v>
       </c>
       <c r="D22" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C23" t="s">
         <v>8</v>
       </c>
       <c r="D23" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C24" t="s">
         <v>8</v>
       </c>
       <c r="D24" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7459,13 +7454,13 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C25" t="s">
         <v>8</v>
       </c>
       <c r="D25" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -7473,18 +7468,18 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C26" t="s">
         <v>8</v>
       </c>
       <c r="D26" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -7515,7 +7510,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7539,7 +7534,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
@@ -7547,7 +7542,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7558,10 +7553,10 @@
     </row>
     <row r="7" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D7" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7575,7 +7570,7 @@
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7583,13 +7578,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7597,24 +7592,24 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7622,13 +7617,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7636,13 +7631,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7656,18 +7651,18 @@
         <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
       </c>
       <c r="D15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7675,13 +7670,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C16" t="s">
         <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -7695,7 +7690,7 @@
         <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7709,7 +7704,7 @@
         <v>8</v>
       </c>
       <c r="D18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
@@ -7717,134 +7712,134 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
       </c>
       <c r="D19" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C20" t="s">
         <v>8</v>
       </c>
       <c r="D20" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C21" t="s">
         <v>8</v>
       </c>
       <c r="D21" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C22" t="s">
         <v>8</v>
       </c>
       <c r="D22" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C23" t="s">
         <v>8</v>
       </c>
       <c r="D23" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C24" t="s">
         <v>8</v>
       </c>
       <c r="D24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C25" t="s">
         <v>8</v>
       </c>
       <c r="D25" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C26" t="s">
         <v>8</v>
       </c>
       <c r="D26" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C27" t="s">
         <v>8</v>
       </c>
       <c r="D27" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C28" t="s">
         <v>8</v>
       </c>
       <c r="D28" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C29" t="s">
         <v>8</v>
       </c>
       <c r="D29" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C30" t="s">
         <v>8</v>
       </c>
       <c r="D30" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7852,13 +7847,13 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C31" t="s">
         <v>8</v>
       </c>
       <c r="D31" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -7913,7 +7908,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
@@ -7921,7 +7916,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7935,13 +7930,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -7949,13 +7944,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7963,21 +7958,21 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D10" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -7985,13 +7980,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -7999,24 +7994,24 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D13" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8024,24 +8019,24 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
       </c>
       <c r="D15" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -8072,7 +8067,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8080,7 +8075,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8096,54 +8091,54 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D9" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D10" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D11" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8151,26 +8146,26 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D15" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8178,18 +8173,18 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D16" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D17" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8197,34 +8192,34 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D18" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D19" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D20" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D21" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8232,10 +8227,10 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D22" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8243,10 +8238,10 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D23" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8254,18 +8249,18 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D24" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D25" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -8273,10 +8268,10 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D26" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8284,10 +8279,10 @@
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D27" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -8295,10 +8290,10 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D28" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8306,10 +8301,10 @@
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D29" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8317,10 +8312,10 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D30" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8328,10 +8323,10 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D31" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8339,10 +8334,10 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D32" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8350,10 +8345,10 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D33" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -8361,10 +8356,10 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D34" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -8372,15 +8367,15 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D36" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
   </sheetData>
@@ -8411,7 +8406,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8419,7 +8414,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8435,7 +8430,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8443,7 +8438,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8454,18 +8449,18 @@
     </row>
     <row r="7" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" t="s">
         <v>60</v>
-      </c>
-      <c r="D7" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -8473,13 +8468,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -8510,7 +8505,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8518,7 +8513,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8534,7 +8529,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -8542,7 +8537,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8561,7 +8556,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -8575,7 +8570,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -8589,34 +8584,34 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8624,7 +8619,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
@@ -8638,7 +8633,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
@@ -8652,7 +8647,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C16" t="s">
         <v>8</v>
@@ -8666,7 +8661,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
@@ -8713,7 +8708,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8721,7 +8716,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8737,7 +8732,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -8745,7 +8740,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8756,12 +8751,12 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -8774,7 +8769,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -8785,18 +8780,18 @@
     </row>
     <row r="11" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8804,29 +8799,29 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D14" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D15" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -8834,13 +8829,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="198" x14ac:dyDescent="0.2">
@@ -8848,18 +8843,18 @@
         <v>4</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8867,21 +8862,21 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D20" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8889,21 +8884,21 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D22" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8911,13 +8906,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -8976,7 +8971,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8984,7 +8979,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -9000,7 +8995,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -9008,7 +9003,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -9019,12 +9014,12 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="132" x14ac:dyDescent="0.2">
@@ -9032,13 +9027,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -9046,10 +9041,10 @@
         <v>4</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9057,7 +9052,7 @@
         <v>41</v>
       </c>
       <c r="D11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9065,58 +9060,58 @@
         <v>4</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B14" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D14" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B15" s="4" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B16" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D16" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B17" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D17" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D18" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9124,13 +9119,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -9144,7 +9139,7 @@
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -9152,13 +9147,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -9166,13 +9161,13 @@
         <v>4</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9180,13 +9175,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9194,26 +9189,26 @@
         <v>4</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B25" s="4" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D25" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -9221,7 +9216,7 @@
         <v>4</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
@@ -9235,7 +9230,7 @@
         <v>4</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
@@ -9246,34 +9241,34 @@
     </row>
     <row r="29" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B29" s="4" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D29" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B30" s="4" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D30" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="4" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D31" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B32" s="4" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D32" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -9281,13 +9276,13 @@
         <v>4</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -9295,7 +9290,7 @@
         <v>4</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
@@ -9309,7 +9304,7 @@
         <v>4</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
@@ -9320,36 +9315,36 @@
     </row>
     <row r="36" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B36" s="4" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D36" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B37" s="4" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="4" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D38" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B39" s="4" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D39" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B40" s="4" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -9357,53 +9352,53 @@
         <v>4</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C41" t="s">
         <v>4</v>
       </c>
       <c r="D41" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B42" s="4" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D42" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B43" s="4" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D43" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B44" s="4" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D44" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B45" s="4" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D45" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B46" s="4" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D46" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9411,7 +9406,7 @@
         <v>4</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C47" t="s">
         <v>4</v>
@@ -9431,8 +9426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A687F900-5547-4D89-8494-B67FCE27BE96}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -9448,7 +9443,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -9472,7 +9467,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="184.8" x14ac:dyDescent="0.2">
@@ -9480,7 +9475,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -9499,13 +9494,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -9518,75 +9513,75 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D11" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D12" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D13" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B14" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D14" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D15" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -9596,13 +9591,13 @@
     </row>
     <row r="19" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -9610,21 +9605,21 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D21" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -9632,13 +9627,13 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -9651,7 +9646,7 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
@@ -9660,26 +9655,23 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>42</v>
+        <v>396</v>
       </c>
       <c r="C26" t="s">
         <v>8</v>
       </c>
-      <c r="D26" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="27" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C27" t="s">
         <v>8</v>
@@ -9693,7 +9685,7 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C28" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
the last revision mac+lan.xlsx is broken?
</commit_message>
<xml_diff>
--- a/macs+lan.xlsx
+++ b/macs+lan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20407"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/norita/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\fresta2024\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{937EF984-13F2-0346-9BF3-AE3FB881C33E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A703D67-B014-477B-AE34-AE159B5DDD9C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19200" tabRatio="772" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="504" windowWidth="33600" windowHeight="19200" tabRatio="772" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -31,16 +31,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -6384,7 +6374,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6465,9 +6455,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -6505,9 +6495,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6540,9 +6530,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6575,9 +6582,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -6757,7 +6781,7 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
@@ -6765,7 +6789,7 @@
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6773,7 +6797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -6781,7 +6805,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -6789,7 +6813,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="60">
+    <row r="5" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -6803,7 +6827,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="45">
+    <row r="6" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -6832,7 +6856,7 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
@@ -6840,7 +6864,7 @@
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -6848,7 +6872,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -6856,7 +6880,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -6864,7 +6888,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -6872,17 +6896,17 @@
         <v>373</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30">
+    <row r="6" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30">
+    <row r="7" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="45">
+    <row r="8" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -6893,7 +6917,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="135">
+    <row r="9" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -6907,7 +6931,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30">
+    <row r="10" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -6921,7 +6945,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15">
+    <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -6935,7 +6959,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="90">
+    <row r="12" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -6949,7 +6973,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="60">
+    <row r="13" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -6978,7 +7002,7 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
@@ -6986,7 +7010,7 @@
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>387</v>
       </c>
@@ -6994,7 +7018,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -7002,7 +7026,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -7010,7 +7034,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -7018,17 +7042,17 @@
         <v>390</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30">
+    <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -7036,7 +7060,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="60">
+    <row r="9" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>394</v>
       </c>
@@ -7044,7 +7068,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>395</v>
       </c>
@@ -7052,17 +7076,17 @@
         <v>396</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="195">
+    <row r="13" spans="1:4" ht="171.6" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -7088,7 +7112,7 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
@@ -7096,7 +7120,7 @@
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -7104,7 +7128,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -7112,7 +7136,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -7120,7 +7144,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -7128,7 +7152,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="75">
+    <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -7142,7 +7166,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="75">
+    <row r="8" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -7150,12 +7174,12 @@
         <v>402</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>403</v>
       </c>
@@ -7166,7 +7190,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30">
+    <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -7180,7 +7204,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>407</v>
       </c>
@@ -7191,7 +7215,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -7205,7 +7229,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -7219,12 +7243,12 @@
         <v>412</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="30">
+    <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>414</v>
       </c>
@@ -7235,7 +7259,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="45">
+    <row r="17" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>416</v>
       </c>
@@ -7246,7 +7270,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="60">
+    <row r="18" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -7260,7 +7284,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="30">
+    <row r="19" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -7274,7 +7298,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="92.5" customHeight="1">
+    <row r="20" spans="1:4" ht="92.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>422</v>
       </c>
@@ -7285,7 +7309,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="75">
+    <row r="21" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -7299,7 +7323,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="45">
+    <row r="22" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -7313,7 +7337,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="30">
+    <row r="23" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>428</v>
       </c>
@@ -7324,7 +7348,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="60">
+    <row r="24" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>430</v>
       </c>
@@ -7335,7 +7359,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="30">
+    <row r="25" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -7349,7 +7373,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="60">
+    <row r="26" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -7363,7 +7387,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="45">
+    <row r="27" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
         <v>436</v>
       </c>
@@ -7379,19 +7403,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="84.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="84.109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" customWidth="1"/>
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15">
+    <row r="1" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -7399,7 +7423,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -7407,7 +7431,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -7415,7 +7439,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -7423,7 +7447,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="135">
+    <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -7437,7 +7461,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="90">
+    <row r="7" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
@@ -7445,7 +7469,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -7459,7 +7483,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="45">
+    <row r="9" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -7473,7 +7497,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15">
+    <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>22</v>
       </c>
@@ -7484,7 +7508,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -7498,7 +7522,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15">
+    <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -7512,7 +7536,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="30">
+    <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>26</v>
       </c>
@@ -7523,7 +7547,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="30">
+    <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -7537,7 +7561,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15">
+    <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -7551,7 +7575,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -7565,7 +7589,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>34</v>
       </c>
@@ -7576,7 +7600,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>36</v>
       </c>
@@ -7587,7 +7611,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="120">
+    <row r="19" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>38</v>
       </c>
@@ -7598,7 +7622,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="30">
+    <row r="20" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>40</v>
       </c>
@@ -7609,7 +7633,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="45">
+    <row r="21" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>42</v>
       </c>
@@ -7620,7 +7644,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="45">
+    <row r="22" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>43</v>
       </c>
@@ -7631,7 +7655,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="30">
+    <row r="23" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>45</v>
       </c>
@@ -7642,7 +7666,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="30">
+    <row r="24" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>47</v>
       </c>
@@ -7653,7 +7677,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>49</v>
       </c>
@@ -7664,7 +7688,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30">
+    <row r="26" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>51</v>
       </c>
@@ -7675,7 +7699,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="30">
+    <row r="27" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -7704,15 +7728,15 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="77.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="77.77734375" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" customWidth="1"/>
     <col min="4" max="4" width="30.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30">
+    <row r="1" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -7720,7 +7744,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -7728,7 +7752,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -7736,7 +7760,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -7744,7 +7768,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="120">
+    <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -7758,7 +7782,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="45">
+    <row r="7" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -7772,7 +7796,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="90">
+    <row r="8" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -7786,7 +7810,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="45">
+    <row r="9" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -7800,7 +7824,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30">
+    <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>65</v>
       </c>
@@ -7808,7 +7832,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="105">
+    <row r="11" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -7822,7 +7846,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="45">
+    <row r="12" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -7836,7 +7860,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="45">
+    <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>71</v>
       </c>
@@ -7847,7 +7871,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="45">
+    <row r="14" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -7861,7 +7885,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="90">
+    <row r="15" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>76</v>
       </c>
@@ -7887,15 +7911,15 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="74.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="5.1640625" customWidth="1"/>
-    <col min="4" max="4" width="49.1640625" customWidth="1"/>
+    <col min="2" max="2" width="74.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="5.109375" customWidth="1"/>
+    <col min="4" max="4" width="49.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30">
+    <row r="1" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -7903,7 +7927,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -7911,7 +7935,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -7919,7 +7943,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -7927,22 +7951,22 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="60">
+    <row r="6" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30">
+    <row r="7" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="45">
+    <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="105">
+    <row r="9" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>84</v>
       </c>
@@ -7950,7 +7974,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="45">
+    <row r="10" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>86</v>
       </c>
@@ -7958,7 +7982,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="120">
+    <row r="11" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>88</v>
       </c>
@@ -7966,7 +7990,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30">
+    <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>437</v>
       </c>
@@ -7974,7 +7998,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="45">
+    <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -7988,7 +8012,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="30">
+    <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>93</v>
       </c>
@@ -7996,7 +8020,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>95</v>
       </c>
@@ -8004,7 +8028,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -8015,7 +8039,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>98</v>
       </c>
@@ -8023,7 +8047,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -8034,7 +8058,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="30">
+    <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>102</v>
       </c>
@@ -8042,7 +8066,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="45">
+    <row r="20" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>104</v>
       </c>
@@ -8050,7 +8074,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="83" customHeight="1">
+    <row r="21" spans="1:4" ht="82.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>106</v>
       </c>
@@ -8058,7 +8082,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -8069,7 +8093,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -8080,7 +8104,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -8091,7 +8115,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>114</v>
       </c>
@@ -8099,7 +8123,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -8110,7 +8134,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="30">
+    <row r="27" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -8121,7 +8145,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="30">
+    <row r="28" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -8132,7 +8156,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="30">
+    <row r="29" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -8143,7 +8167,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -8154,7 +8178,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>6</v>
       </c>
@@ -8165,7 +8189,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>6</v>
       </c>
@@ -8176,7 +8200,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="30">
+    <row r="33" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>6</v>
       </c>
@@ -8187,7 +8211,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="30">
+    <row r="34" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>6</v>
       </c>
@@ -8198,7 +8222,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>6</v>
       </c>
@@ -8209,7 +8233,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="30">
+    <row r="36" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
         <v>136</v>
       </c>
@@ -8217,7 +8241,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
         <v>138</v>
       </c>
@@ -8225,7 +8249,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
         <v>140</v>
       </c>
@@ -8233,7 +8257,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="30">
+    <row r="39" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
         <v>142</v>
       </c>
@@ -8241,7 +8265,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
         <v>144</v>
       </c>
@@ -8249,7 +8273,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
         <v>146</v>
       </c>
@@ -8257,7 +8281,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
         <v>148</v>
       </c>
@@ -8265,7 +8289,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
         <v>140</v>
       </c>
@@ -8273,7 +8297,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
         <v>151</v>
       </c>
@@ -8281,7 +8305,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
         <v>153</v>
       </c>
@@ -8289,7 +8313,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="30">
+    <row r="46" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s">
         <v>155</v>
       </c>
@@ -8297,7 +8321,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="30">
+    <row r="47" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
         <v>157</v>
       </c>
@@ -8305,7 +8329,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="30">
+    <row r="48" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B48" s="1" t="s">
         <v>159</v>
       </c>
@@ -8313,7 +8337,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="49" spans="2:4" ht="15">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B49" s="1" t="s">
         <v>161</v>
       </c>
@@ -8321,7 +8345,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="50" spans="2:4" ht="15">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B50" s="1" t="s">
         <v>163</v>
       </c>
@@ -8344,7 +8368,7 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
@@ -8352,7 +8376,7 @@
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -8360,7 +8384,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -8368,7 +8392,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -8376,7 +8400,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -8384,7 +8408,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="45">
+    <row r="6" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -8398,7 +8422,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="75">
+    <row r="7" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>169</v>
       </c>
@@ -8406,7 +8430,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="60">
+    <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -8431,11 +8455,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
@@ -8443,7 +8467,7 @@
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -8451,7 +8475,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -8459,7 +8483,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -8467,7 +8491,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -8475,7 +8499,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="105">
+    <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -8489,12 +8513,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30">
+    <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -8508,7 +8532,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -8522,7 +8546,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -8536,7 +8560,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30">
+    <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>184</v>
       </c>
@@ -8547,7 +8571,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>442</v>
       </c>
@@ -8555,7 +8579,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15">
+    <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>187</v>
       </c>
@@ -8563,7 +8587,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -8577,7 +8601,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -8591,7 +8615,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="30">
+    <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -8602,7 +8626,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -8613,7 +8637,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="45">
+    <row r="18" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -8624,7 +8648,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="30">
+    <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -8635,7 +8659,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="30">
+    <row r="20" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>199</v>
       </c>
@@ -8643,7 +8667,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>201</v>
       </c>
@@ -8651,7 +8675,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="90">
+    <row r="22" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>203</v>
       </c>
@@ -8659,7 +8683,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>205</v>
       </c>
@@ -8667,7 +8691,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>207</v>
       </c>
@@ -8675,7 +8699,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>209</v>
       </c>
@@ -8683,7 +8707,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>211</v>
       </c>
@@ -8691,7 +8715,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="75">
+    <row r="27" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
         <v>213</v>
       </c>
@@ -8699,7 +8723,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
         <v>215</v>
       </c>
@@ -8707,7 +8731,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
         <v>217</v>
       </c>
@@ -8715,7 +8739,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
         <v>219</v>
       </c>
@@ -8738,7 +8762,7 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
@@ -8746,7 +8770,7 @@
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30">
+    <row r="1" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -8754,7 +8778,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -8762,7 +8786,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -8770,7 +8794,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -8778,7 +8802,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="105">
+    <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -8792,22 +8816,22 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30">
+    <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="90">
+    <row r="10" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -8821,7 +8845,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="60">
+    <row r="11" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>230</v>
       </c>
@@ -8832,12 +8856,12 @@
         <v>231</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="30">
+    <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -8851,7 +8875,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="60">
+    <row r="14" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>235</v>
       </c>
@@ -8859,7 +8883,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>237</v>
       </c>
@@ -8867,7 +8891,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="90">
+    <row r="16" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -8881,7 +8905,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="225">
+    <row r="17" spans="1:4" ht="198" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -8895,12 +8919,12 @@
         <v>241</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="30">
+    <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -8914,7 +8938,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>245</v>
       </c>
@@ -8922,7 +8946,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="30">
+    <row r="21" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -8936,7 +8960,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>249</v>
       </c>
@@ -8944,7 +8968,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="45">
+    <row r="23" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -8958,12 +8982,12 @@
         <v>252</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -8971,17 +8995,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -9001,15 +9025,15 @@
       <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="100.6640625" style="3" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="34.83203125" customWidth="1"/>
+    <col min="4" max="4" width="34.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -9017,7 +9041,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -9025,7 +9049,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -9033,7 +9057,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -9041,7 +9065,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="105">
+    <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -9055,17 +9079,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="45">
+    <row r="8" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="150">
+    <row r="9" spans="1:4" ht="132" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -9079,7 +9103,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="45">
+    <row r="10" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -9090,7 +9114,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30">
+    <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
         <v>263</v>
       </c>
@@ -9098,7 +9122,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30">
+    <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -9112,12 +9136,12 @@
         <v>266</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="3" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="30">
+    <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B14" s="3" t="s">
         <v>268</v>
       </c>
@@ -9125,7 +9149,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="45">
+    <row r="15" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
         <v>270</v>
       </c>
@@ -9133,7 +9157,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="30">
+    <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B16" s="3" t="s">
         <v>272</v>
       </c>
@@ -9141,7 +9165,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
         <v>274</v>
       </c>
@@ -9149,7 +9173,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
         <v>276</v>
       </c>
@@ -9157,7 +9181,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="30">
+    <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -9171,7 +9195,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="60">
+    <row r="20" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -9185,7 +9209,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="60">
+    <row r="21" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -9199,7 +9223,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="45">
+    <row r="22" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -9213,7 +9237,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="30">
+    <row r="23" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -9227,7 +9251,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="30">
+    <row r="24" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -9241,7 +9265,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="30">
+    <row r="25" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B25" s="3" t="s">
         <v>290</v>
       </c>
@@ -9249,7 +9273,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30">
+    <row r="26" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B26" s="3" t="s">
         <v>292</v>
       </c>
@@ -9257,12 +9281,12 @@
         <v>293</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" s="3" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="45">
+    <row r="28" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -9276,7 +9300,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="45">
+    <row r="29" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -9290,7 +9314,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B30" s="3" t="s">
         <v>299</v>
       </c>
@@ -9298,12 +9322,12 @@
         <v>300</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="75">
+    <row r="31" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B31" s="3" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B32" s="3" t="s">
         <v>302</v>
       </c>
@@ -9311,7 +9335,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="43.25" customHeight="1">
+    <row r="33" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="3" t="s">
         <v>304</v>
       </c>
@@ -9319,7 +9343,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B34" s="3" t="s">
         <v>306</v>
       </c>
@@ -9327,7 +9351,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>6</v>
       </c>
@@ -9341,7 +9365,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="60">
+    <row r="36" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>6</v>
       </c>
@@ -9355,7 +9379,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15">
+    <row r="37" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B37" s="3" t="s">
         <v>312</v>
       </c>
@@ -9363,12 +9387,12 @@
         <v>313</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B38" s="3" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="42" customHeight="1">
+    <row r="39" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="3" t="s">
         <v>315</v>
       </c>
@@ -9376,7 +9400,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="45">
+    <row r="40" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B40" s="3" t="s">
         <v>317</v>
       </c>
@@ -9384,12 +9408,12 @@
         <v>318</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B41" s="3" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="60">
+    <row r="42" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>6</v>
       </c>
@@ -9403,7 +9427,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15">
+    <row r="43" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B43" s="3" t="s">
         <v>322</v>
       </c>
@@ -9411,7 +9435,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B44" s="3" t="s">
         <v>324</v>
       </c>
@@ -9419,7 +9443,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B45" s="3" t="s">
         <v>326</v>
       </c>
@@ -9427,7 +9451,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B46" s="3" t="s">
         <v>328</v>
       </c>
@@ -9435,7 +9459,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B47" s="3" t="s">
         <v>330</v>
       </c>
@@ -9443,7 +9467,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="30">
+    <row r="48" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>6</v>
       </c>
@@ -9472,7 +9496,7 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
@@ -9480,7 +9504,7 @@
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30">
+    <row r="1" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -9488,7 +9512,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -9496,7 +9520,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -9504,7 +9528,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -9512,7 +9536,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="195">
+    <row r="6" spans="1:4" ht="184.8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -9526,12 +9550,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="45">
+    <row r="8" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -9545,12 +9569,12 @@
         <v>231</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -9564,7 +9588,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="60">
+    <row r="11" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>342</v>
       </c>
@@ -9572,7 +9596,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="60">
+    <row r="12" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>344</v>
       </c>
@@ -9580,7 +9604,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="30">
+    <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>346</v>
       </c>
@@ -9588,7 +9612,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15">
+    <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>348</v>
       </c>
@@ -9596,7 +9620,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="30">
+    <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>350</v>
       </c>
@@ -9604,7 +9628,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="45">
+    <row r="16" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>352</v>
       </c>
@@ -9615,7 +9639,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="60">
+    <row r="17" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>354</v>
       </c>
@@ -9626,12 +9650,12 @@
         <v>355</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="45">
+    <row r="19" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>357</v>
       </c>
@@ -9642,7 +9666,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="75">
+    <row r="20" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -9656,7 +9680,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="60">
+    <row r="21" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>360</v>
       </c>
@@ -9664,7 +9688,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="120">
+    <row r="22" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -9678,12 +9702,12 @@
         <v>363</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="30">
+    <row r="25" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -9697,7 +9721,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="90">
+    <row r="26" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -9708,7 +9732,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="120">
+    <row r="27" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -9722,7 +9746,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="150">
+    <row r="28" spans="1:4" ht="132" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
mac: mention about no-network case
</commit_message>
<xml_diff>
--- a/macs+lan.xlsx
+++ b/macs+lan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27504"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20407"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/norita/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7DC0903B-A26A-40B7-BC83-04EE469CFA7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{994B0864-DD5F-4FB4-8734-8147005953D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" tabRatio="772" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7764" tabRatio="772" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -31,16 +31,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -451,10 +441,6 @@
   </si>
   <si>
     <t>0_3.jpeg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WiFiネットワークを選択の画面。自分が使用できるSSIDを選択してください。 </t>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>0_4.jpeg</t>
@@ -6359,12 +6345,56 @@
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>WiFiネットワークを選択の画面。自分が使用できるSSIDを選択してください。 
+このスクリーンショットではパスワードのみの認証の場合を示しますが、アカウントとパスワードの両方が必要なWiFiにも接続できる筈です。もしどうしても接続できない場合(macOSが古いとできない場合があります)は&lt;a href="../../2023/mac+lan/"&gt;2023年版&lt;/a&gt;を参照してください。</t>
+    <rPh sb="62" eb="64">
+      <t>ニンショウ</t>
+    </rPh>
+    <rPh sb="65" eb="67">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="68" eb="69">
+      <t>シメ</t>
+    </rPh>
+    <rPh sb="86" eb="88">
+      <t>リョウホウ</t>
+    </rPh>
+    <rPh sb="89" eb="91">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <rPh sb="98" eb="100">
+      <t>セツゾク</t>
+    </rPh>
+    <rPh sb="103" eb="104">
+      <t>ハズ</t>
+    </rPh>
+    <rPh sb="114" eb="116">
+      <t>セツゾク</t>
+    </rPh>
+    <rPh sb="120" eb="122">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="129" eb="130">
+      <t>フル</t>
+    </rPh>
+    <rPh sb="136" eb="138">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="179" eb="181">
+      <t>ネンバン</t>
+    </rPh>
+    <rPh sb="186" eb="188">
+      <t>サンショウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6445,9 +6475,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -6485,9 +6515,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6520,9 +6550,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6555,9 +6602,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -6737,15 +6801,15 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.1"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.625" customWidth="1"/>
-    <col min="2" max="2" width="100.625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.625" customWidth="1"/>
-    <col min="4" max="4" width="20.625" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6753,7 +6817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -6761,7 +6825,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -6769,7 +6833,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="60">
+    <row r="5" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -6783,7 +6847,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="45">
+    <row r="6" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -6812,31 +6876,31 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.1"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.625" customWidth="1"/>
-    <col min="2" max="2" width="100.625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.625" customWidth="1"/>
-    <col min="4" max="4" width="20.625" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -6844,103 +6908,103 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30">
-      <c r="B6" s="1" t="s">
+    <row r="7" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30">
-      <c r="B7" s="1" t="s">
+    <row r="8" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="45">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>382</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="135">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>383</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
       </c>
       <c r="D9" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="30">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
         <v>385</v>
       </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" t="s">
+    </row>
+    <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="15">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
         <v>387</v>
       </c>
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" t="s">
+    </row>
+    <row r="12" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="90">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
         <v>389</v>
       </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" t="s">
+    </row>
+    <row r="13" spans="1:4" ht="66" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="60">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
         <v>391</v>
-      </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" t="s">
-        <v>392</v>
       </c>
     </row>
   </sheetData>
@@ -6958,31 +7022,31 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.1"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.625" customWidth="1"/>
-    <col min="2" max="2" width="100.625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.625" customWidth="1"/>
-    <col min="4" max="4" width="20.625" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>392</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -6990,59 +7054,59 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15">
-      <c r="B6" s="1" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15">
-      <c r="B7" s="1" t="s">
+    <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
+    <row r="9" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="60">
-      <c r="B9" s="1" t="s">
+      <c r="D9" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="D9" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15">
-      <c r="B10" s="1" t="s">
+      <c r="D10" t="s">
         <v>401</v>
       </c>
-      <c r="D10" t="s">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15">
-      <c r="B12" s="1" t="s">
+    <row r="13" spans="1:4" ht="171.6" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="195">
-      <c r="B13" s="1" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -7068,31 +7132,31 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.1"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.625" customWidth="1"/>
-    <col min="2" max="2" width="100.625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.625" customWidth="1"/>
-    <col min="4" max="4" width="20.625" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -7100,252 +7164,252 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="75">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="75">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
         <v>408</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15">
-      <c r="B10" s="1" t="s">
-        <v>409</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
       </c>
       <c r="D10" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>410</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="30">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>411</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
       </c>
       <c r="D11" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
         <v>412</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15">
-      <c r="B12" s="1" t="s">
-        <v>413</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
       </c>
       <c r="D12" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>414</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>415</v>
       </c>
       <c r="C13" t="s">
         <v>18</v>
       </c>
       <c r="D13" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>416</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15">
-      <c r="A14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>417</v>
       </c>
       <c r="C14" t="s">
         <v>18</v>
       </c>
       <c r="D14" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15">
-      <c r="B15" s="1" t="s">
+    <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
         <v>419</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="30">
-      <c r="B16" s="1" t="s">
-        <v>420</v>
       </c>
       <c r="C16" t="s">
         <v>18</v>
       </c>
       <c r="D16" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
         <v>421</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="45">
-      <c r="B17" s="1" t="s">
-        <v>422</v>
       </c>
       <c r="C17" t="s">
         <v>18</v>
       </c>
       <c r="D17" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>423</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="60">
-      <c r="A18" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>424</v>
       </c>
       <c r="C18" t="s">
         <v>18</v>
       </c>
       <c r="D18" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>425</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="30">
-      <c r="A19" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>426</v>
       </c>
       <c r="C19" t="s">
         <v>18</v>
       </c>
       <c r="D19" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="92.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="92.45" customHeight="1">
-      <c r="B20" s="1" t="s">
+      <c r="C20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" t="s">
         <v>428</v>
       </c>
-      <c r="C20" t="s">
-        <v>75</v>
-      </c>
-      <c r="D20" t="s">
+    </row>
+    <row r="21" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>429</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="75">
-      <c r="A21" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>430</v>
       </c>
       <c r="C21" t="s">
         <v>18</v>
       </c>
       <c r="D21" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>431</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="45">
-      <c r="A22" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>432</v>
       </c>
       <c r="C22" t="s">
         <v>18</v>
       </c>
       <c r="D22" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
         <v>433</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="30">
-      <c r="B23" s="1" t="s">
-        <v>434</v>
       </c>
       <c r="C23" t="s">
         <v>18</v>
       </c>
       <c r="D23" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="66" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
         <v>435</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="60">
-      <c r="B24" s="1" t="s">
-        <v>436</v>
       </c>
       <c r="C24" t="s">
         <v>18</v>
       </c>
       <c r="D24" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>437</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="30">
-      <c r="A25" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>438</v>
       </c>
       <c r="C25" t="s">
         <v>18</v>
       </c>
       <c r="D25" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="66" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>439</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="60">
-      <c r="A26" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>440</v>
       </c>
       <c r="C26" t="s">
         <v>18</v>
       </c>
       <c r="D26" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
         <v>441</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="45">
-      <c r="B27" s="1" t="s">
-        <v>442</v>
       </c>
     </row>
   </sheetData>
@@ -7359,19 +7423,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.1"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.625" customWidth="1"/>
-    <col min="2" max="2" width="84.125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.625" customWidth="1"/>
-    <col min="4" max="4" width="20.625" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="84.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15">
+    <row r="1" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -7379,7 +7443,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -7387,7 +7451,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -7395,7 +7459,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -7403,7 +7467,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="135">
+    <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -7417,7 +7481,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="90">
+    <row r="7" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
@@ -7425,7 +7489,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -7439,7 +7503,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="45">
+    <row r="9" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -7453,7 +7517,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15">
+    <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>22</v>
       </c>
@@ -7464,209 +7528,209 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15">
+    <row r="11" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>442</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
       </c>
       <c r="D11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
       </c>
       <c r="D12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="30">
-      <c r="B13" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="C13" t="s">
         <v>18</v>
       </c>
       <c r="D13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="30">
-      <c r="A14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="C14" t="s">
         <v>18</v>
       </c>
       <c r="D14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="C15" t="s">
         <v>18</v>
       </c>
       <c r="D15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15">
-      <c r="A16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="C16" t="s">
         <v>18</v>
       </c>
       <c r="D16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15">
-      <c r="B17" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="C17" t="s">
         <v>18</v>
       </c>
       <c r="D17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15">
-      <c r="B18" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="C18" t="s">
         <v>18</v>
       </c>
       <c r="D18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="120">
-      <c r="B19" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="C19" t="s">
         <v>18</v>
       </c>
       <c r="D19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="30">
-      <c r="B20" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="C20" t="s">
         <v>18</v>
       </c>
       <c r="D20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="45">
-      <c r="B21" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="C21" t="s">
         <v>18</v>
       </c>
       <c r="D21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="45">
-      <c r="B22" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="C22" t="s">
         <v>18</v>
       </c>
       <c r="D22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="30">
-      <c r="B23" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="C23" t="s">
         <v>18</v>
       </c>
       <c r="D23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="30">
-      <c r="B24" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="C24" t="s">
         <v>18</v>
       </c>
       <c r="D24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="15">
-      <c r="B25" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="C25" t="s">
         <v>18</v>
       </c>
       <c r="D25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="30">
-      <c r="B26" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="C26" t="s">
         <v>18</v>
       </c>
       <c r="D26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="30">
-      <c r="A27" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="C27" t="s">
         <v>18</v>
       </c>
       <c r="D27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -7684,31 +7748,31 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.1"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.625" customWidth="1"/>
-    <col min="2" max="2" width="77.875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.625" customWidth="1"/>
-    <col min="4" max="4" width="30.375" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="77.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="30.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30">
+    <row r="1" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -7716,140 +7780,140 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="120">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="45">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
         <v>62</v>
       </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s">
+    </row>
+    <row r="8" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="90">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
       </c>
       <c r="D8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="45">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
         <v>66</v>
       </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" t="s">
+    </row>
+    <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="30">
-      <c r="B10" s="1" t="s">
+      <c r="D10" t="s">
         <v>68</v>
       </c>
-      <c r="D10" t="s">
+    </row>
+    <row r="11" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="105">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
       </c>
       <c r="D11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="45">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
       </c>
       <c r="D12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="45">
-      <c r="B13" s="1" t="s">
+      <c r="C13" t="s">
         <v>74</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>75</v>
       </c>
-      <c r="D13" t="s">
+    </row>
+    <row r="14" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="45">
-      <c r="A14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="C14" t="s">
         <v>18</v>
       </c>
       <c r="D14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="90">
-      <c r="B15" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="C15" t="s">
         <v>18</v>
       </c>
       <c r="D15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -7867,31 +7931,31 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.1"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.625" customWidth="1"/>
-    <col min="2" max="2" width="74.875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="5.125" customWidth="1"/>
-    <col min="4" max="4" width="49.125" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="74.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="5.109375" customWidth="1"/>
+    <col min="4" max="4" width="49.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30">
+    <row r="1" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -7899,414 +7963,414 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="60">
-      <c r="B6" s="1" t="s">
+    <row r="7" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30">
-      <c r="B7" s="1" t="s">
+    <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="45">
-      <c r="B8" s="1" t="s">
+    <row r="9" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="105">
-      <c r="B9" s="1" t="s">
+      <c r="D9" t="s">
         <v>87</v>
       </c>
-      <c r="D9" t="s">
+    </row>
+    <row r="10" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="45">
-      <c r="B10" s="1" t="s">
+      <c r="D10" t="s">
         <v>89</v>
       </c>
-      <c r="D10" t="s">
+    </row>
+    <row r="11" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="120">
-      <c r="B11" s="1" t="s">
+      <c r="D11" t="s">
         <v>91</v>
       </c>
-      <c r="D11" t="s">
+    </row>
+    <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="30">
-      <c r="B12" s="1" t="s">
+      <c r="D12" t="s">
         <v>93</v>
       </c>
-      <c r="D12" t="s">
+    </row>
+    <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="45">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
         <v>95</v>
       </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" t="s">
+    </row>
+    <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="30">
-      <c r="B14" s="1" t="s">
+      <c r="D14" t="s">
         <v>97</v>
       </c>
-      <c r="D14" t="s">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="15">
-      <c r="B15" s="1" t="s">
+      <c r="D15" t="s">
         <v>99</v>
       </c>
-      <c r="D15" t="s">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="15">
-      <c r="A16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="1" t="s">
+      <c r="D16" t="s">
         <v>101</v>
       </c>
-      <c r="D16" t="s">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="15">
-      <c r="B17" s="1" t="s">
+      <c r="D17" t="s">
         <v>103</v>
       </c>
-      <c r="D17" t="s">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="15">
-      <c r="A18" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="1" t="s">
+      <c r="D18" t="s">
         <v>105</v>
       </c>
-      <c r="D18" t="s">
+    </row>
+    <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="30">
-      <c r="B19" s="1" t="s">
+      <c r="D19" t="s">
         <v>107</v>
       </c>
-      <c r="D19" t="s">
+    </row>
+    <row r="20" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="45">
-      <c r="B20" s="1" t="s">
+      <c r="D20" t="s">
         <v>109</v>
       </c>
-      <c r="D20" t="s">
+    </row>
+    <row r="21" spans="1:4" ht="83.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="83.1" customHeight="1">
-      <c r="B21" s="1" t="s">
+      <c r="D21" t="s">
         <v>111</v>
       </c>
-      <c r="D21" t="s">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="15">
-      <c r="A22" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="1" t="s">
+      <c r="D22" t="s">
         <v>113</v>
       </c>
-      <c r="D22" t="s">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="15">
-      <c r="A23" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" s="1" t="s">
+      <c r="D23" t="s">
         <v>115</v>
       </c>
-      <c r="D23" t="s">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="15">
-      <c r="A24" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" s="1" t="s">
+      <c r="D24" t="s">
         <v>117</v>
       </c>
-      <c r="D24" t="s">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="15">
-      <c r="B25" s="1" t="s">
+      <c r="D25" t="s">
         <v>119</v>
       </c>
-      <c r="D25" t="s">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="15">
-      <c r="A26" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="1" t="s">
+      <c r="D26" t="s">
         <v>121</v>
       </c>
-      <c r="D26" t="s">
+    </row>
+    <row r="27" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="30">
-      <c r="A27" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="1" t="s">
+      <c r="D27" t="s">
         <v>123</v>
       </c>
-      <c r="D27" t="s">
+    </row>
+    <row r="28" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="30">
-      <c r="A28" t="s">
-        <v>6</v>
-      </c>
-      <c r="B28" s="1" t="s">
+      <c r="D28" t="s">
         <v>125</v>
       </c>
-      <c r="D28" t="s">
+    </row>
+    <row r="29" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="30">
-      <c r="A29" t="s">
-        <v>6</v>
-      </c>
-      <c r="B29" s="1" t="s">
+      <c r="D29" t="s">
         <v>127</v>
       </c>
-      <c r="D29" t="s">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="15">
-      <c r="A30" t="s">
-        <v>6</v>
-      </c>
-      <c r="B30" s="1" t="s">
+      <c r="D30" t="s">
         <v>129</v>
       </c>
-      <c r="D30" t="s">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="15">
-      <c r="A31" t="s">
-        <v>6</v>
-      </c>
-      <c r="B31" s="1" t="s">
+      <c r="D31" t="s">
         <v>131</v>
       </c>
-      <c r="D31" t="s">
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="15">
-      <c r="A32" t="s">
-        <v>6</v>
-      </c>
-      <c r="B32" s="1" t="s">
+      <c r="D32" t="s">
         <v>133</v>
       </c>
-      <c r="D32" t="s">
+    </row>
+    <row r="33" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="30">
-      <c r="A33" t="s">
-        <v>6</v>
-      </c>
-      <c r="B33" s="1" t="s">
+      <c r="D33" t="s">
         <v>135</v>
       </c>
-      <c r="D33" t="s">
+    </row>
+    <row r="34" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="30">
-      <c r="A34" t="s">
-        <v>6</v>
-      </c>
-      <c r="B34" s="1" t="s">
+      <c r="D34" t="s">
         <v>137</v>
       </c>
-      <c r="D34" t="s">
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="15">
-      <c r="A35" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" s="1" t="s">
+      <c r="D35" t="s">
         <v>139</v>
       </c>
-      <c r="D35" t="s">
+    </row>
+    <row r="36" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B36" s="1" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="30">
-      <c r="B36" s="1" t="s">
+      <c r="D36" t="s">
         <v>141</v>
       </c>
-      <c r="D36" t="s">
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B37" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="15">
-      <c r="B37" s="1" t="s">
+      <c r="D37" t="s">
         <v>143</v>
       </c>
-      <c r="D37" t="s">
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B38" s="1" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" ht="15">
-      <c r="B38" s="1" t="s">
+      <c r="D38" t="s">
         <v>145</v>
       </c>
-      <c r="D38" t="s">
+    </row>
+    <row r="39" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B39" s="1" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" ht="30">
-      <c r="B39" s="1" t="s">
+      <c r="D39" t="s">
         <v>147</v>
       </c>
-      <c r="D39" t="s">
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B40" s="1" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="15">
-      <c r="B40" s="1" t="s">
+      <c r="D40" t="s">
         <v>149</v>
       </c>
-      <c r="D40" t="s">
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B41" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" ht="15">
-      <c r="B41" s="1" t="s">
+      <c r="D41" t="s">
         <v>151</v>
       </c>
-      <c r="D41" t="s">
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B42" s="1" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" ht="15">
-      <c r="B42" s="1" t="s">
+      <c r="D42" t="s">
         <v>153</v>
       </c>
-      <c r="D42" t="s">
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B43" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D43" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15">
-      <c r="B43" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D43" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B44" s="1" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" ht="15">
-      <c r="B44" s="1" t="s">
+      <c r="D44" t="s">
         <v>156</v>
       </c>
-      <c r="D44" t="s">
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B45" s="1" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" ht="15">
-      <c r="B45" s="1" t="s">
+      <c r="D45" t="s">
         <v>158</v>
       </c>
-      <c r="D45" t="s">
+    </row>
+    <row r="46" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B46" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" ht="30">
-      <c r="B46" s="1" t="s">
+      <c r="D46" t="s">
         <v>160</v>
       </c>
-      <c r="D46" t="s">
+    </row>
+    <row r="47" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B47" s="1" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" ht="30">
-      <c r="B47" s="1" t="s">
+      <c r="D47" t="s">
         <v>162</v>
       </c>
-      <c r="D47" t="s">
+    </row>
+    <row r="48" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B48" s="1" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" ht="30">
-      <c r="B48" s="1" t="s">
+      <c r="D48" t="s">
         <v>164</v>
       </c>
-      <c r="D48" t="s">
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B49" s="1" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="49" spans="2:4" ht="15">
-      <c r="B49" s="1" t="s">
+      <c r="D49" t="s">
         <v>166</v>
       </c>
-      <c r="D49" t="s">
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B50" s="1" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="50" spans="2:4" ht="15">
-      <c r="B50" s="1" t="s">
+      <c r="D50" t="s">
         <v>168</v>
-      </c>
-      <c r="D50" t="s">
-        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -8324,31 +8388,31 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.1"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.625" customWidth="1"/>
-    <col min="2" max="2" width="100.625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.625" customWidth="1"/>
-    <col min="4" max="4" width="20.625" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -8356,48 +8420,48 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="45">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="66" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="75">
-      <c r="B7" s="1" t="s">
+      <c r="D7" t="s">
         <v>174</v>
       </c>
-      <c r="D7" t="s">
+    </row>
+    <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="60">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
         <v>176</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
-        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -8415,31 +8479,31 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.1"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.625" customWidth="1"/>
-    <col min="2" max="2" width="100.625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.625" customWidth="1"/>
-    <col min="4" max="4" width="20.625" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -8447,260 +8511,260 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="105">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15">
-      <c r="B7" s="1" t="s">
+    </row>
+    <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="30">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
         <v>183</v>
       </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>184</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
       </c>
       <c r="D9" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>186</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>187</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
       </c>
       <c r="D10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
         <v>188</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="30">
-      <c r="B11" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
       </c>
       <c r="D11" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="15">
-      <c r="B12" s="1" t="s">
+      <c r="D12" t="s">
         <v>191</v>
       </c>
-      <c r="D12" t="s">
+    </row>
+    <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="15">
-      <c r="B13" s="1" t="s">
+      <c r="D13" t="s">
         <v>193</v>
       </c>
-      <c r="D13" t="s">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>194</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15">
-      <c r="A14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>195</v>
       </c>
       <c r="C14" t="s">
         <v>18</v>
       </c>
       <c r="D14" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>196</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="C15" t="s">
         <v>18</v>
       </c>
       <c r="D15" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>198</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="30">
-      <c r="A16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>199</v>
       </c>
       <c r="C16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="45">
+    <row r="18" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>6</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D18" t="s">
         <v>201</v>
       </c>
-      <c r="D18" t="s">
+    </row>
+    <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="30">
-      <c r="A19" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="1" t="s">
+      <c r="D19" t="s">
         <v>203</v>
       </c>
-      <c r="D19" t="s">
+    </row>
+    <row r="20" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="30">
-      <c r="B20" s="1" t="s">
+      <c r="D20" t="s">
         <v>205</v>
       </c>
-      <c r="D20" t="s">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="15">
-      <c r="B21" s="1" t="s">
+      <c r="D21" t="s">
         <v>207</v>
       </c>
-      <c r="D21" t="s">
+    </row>
+    <row r="22" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="90">
-      <c r="B22" s="1" t="s">
+      <c r="D22" t="s">
         <v>209</v>
       </c>
-      <c r="D22" t="s">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="15">
-      <c r="B23" s="1" t="s">
+      <c r="D23" t="s">
         <v>211</v>
       </c>
-      <c r="D23" t="s">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="15">
-      <c r="B24" s="1" t="s">
+      <c r="D24" t="s">
         <v>213</v>
       </c>
-      <c r="D24" t="s">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="15">
-      <c r="B25" s="1" t="s">
+      <c r="D25" t="s">
         <v>215</v>
       </c>
-      <c r="D25" t="s">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="15">
-      <c r="B26" s="1" t="s">
+      <c r="D26" t="s">
         <v>217</v>
       </c>
-      <c r="D26" t="s">
+    </row>
+    <row r="27" spans="1:4" ht="66" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="75">
-      <c r="B27" s="1" t="s">
+      <c r="D27" t="s">
         <v>219</v>
       </c>
-      <c r="D27" t="s">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B28" s="1" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="15">
-      <c r="B28" s="1" t="s">
+      <c r="D28" t="s">
         <v>221</v>
       </c>
-      <c r="D28" t="s">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B29" s="1" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="15">
-      <c r="B29" s="1" t="s">
+      <c r="D29" t="s">
         <v>223</v>
       </c>
-      <c r="D29" t="s">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B30" s="1" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="15">
-      <c r="B30" s="1" t="s">
+      <c r="D30" t="s">
         <v>225</v>
-      </c>
-      <c r="D30" t="s">
-        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -8718,31 +8782,31 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.1"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.625" customWidth="1"/>
-    <col min="2" max="2" width="100.625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.625" customWidth="1"/>
-    <col min="4" max="4" width="20.625" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30">
+    <row r="1" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -8750,200 +8814,200 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="105">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15">
-      <c r="B7" s="1" t="s">
+    </row>
+    <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30">
-      <c r="B8" s="1" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15">
-      <c r="B9" s="1" t="s">
+    <row r="10" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="90">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
         <v>234</v>
       </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" t="s">
+    </row>
+    <row r="11" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="60">
-      <c r="B11" s="1" t="s">
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
         <v>236</v>
       </c>
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" t="s">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15">
-      <c r="B12" s="1" t="s">
+    <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="30">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
         <v>239</v>
       </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" t="s">
+    </row>
+    <row r="14" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="60">
-      <c r="B14" s="1" t="s">
+      <c r="D14" t="s">
         <v>241</v>
       </c>
-      <c r="D14" t="s">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="15">
-      <c r="B15" s="1" t="s">
+      <c r="D15" t="s">
         <v>243</v>
       </c>
-      <c r="D15" t="s">
+    </row>
+    <row r="16" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="90">
-      <c r="A16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="198" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="C16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="225">
-      <c r="A17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
         <v>246</v>
       </c>
-      <c r="C17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" t="s">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15">
-      <c r="B18" s="1" t="s">
+    <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="30">
-      <c r="A19" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s">
         <v>249</v>
       </c>
-      <c r="C19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" t="s">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="15">
-      <c r="B20" s="1" t="s">
+      <c r="D20" t="s">
         <v>251</v>
       </c>
-      <c r="D20" t="s">
+    </row>
+    <row r="21" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="30">
-      <c r="A21" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
         <v>253</v>
       </c>
-      <c r="C21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" t="s">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="15">
-      <c r="B22" s="1" t="s">
+      <c r="D22" t="s">
         <v>255</v>
       </c>
-      <c r="D22" t="s">
+    </row>
+    <row r="23" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="45">
-      <c r="A23" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" t="s">
         <v>257</v>
       </c>
-      <c r="C23" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -8951,17 +9015,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -8981,31 +9045,31 @@
       <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.1"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.625" customWidth="1"/>
-    <col min="2" max="2" width="100.625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.625" customWidth="1"/>
-    <col min="4" max="4" width="34.875" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="100.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="34.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -9013,428 +9077,428 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="105">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15">
-      <c r="B7" s="3" t="s">
+    </row>
+    <row r="8" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B8" s="3" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="45">
-      <c r="B8" s="3" t="s">
+    <row r="9" spans="1:4" ht="132" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>264</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="150">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>265</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
       </c>
       <c r="D9" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="45">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="3" t="s">
+      <c r="D10" t="s">
         <v>267</v>
       </c>
-      <c r="D10" t="s">
+    </row>
+    <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B11" s="3" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="30">
-      <c r="B11" s="3" t="s">
+      <c r="D11" t="s">
         <v>269</v>
       </c>
-      <c r="D11" t="s">
+    </row>
+    <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="30">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="3" t="s">
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
         <v>271</v>
       </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" t="s">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="3" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15">
-      <c r="B13" s="3" t="s">
+    <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B14" s="3" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="30">
-      <c r="B14" s="3" t="s">
+      <c r="D14" t="s">
         <v>274</v>
       </c>
-      <c r="D14" t="s">
+    </row>
+    <row r="15" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B15" s="3" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="45">
-      <c r="B15" s="3" t="s">
+      <c r="D15" t="s">
         <v>276</v>
       </c>
-      <c r="D15" t="s">
+    </row>
+    <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B16" s="3" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="30">
-      <c r="B16" s="3" t="s">
+      <c r="D16" t="s">
         <v>278</v>
       </c>
-      <c r="D16" t="s">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B17" s="3" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="15">
-      <c r="B17" s="3" t="s">
+      <c r="D17" t="s">
         <v>280</v>
       </c>
-      <c r="D17" t="s">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B18" s="3" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="15">
-      <c r="B18" s="3" t="s">
+      <c r="D18" t="s">
         <v>282</v>
       </c>
-      <c r="D18" t="s">
+    </row>
+    <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="30">
-      <c r="A19" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="3" t="s">
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s">
         <v>284</v>
       </c>
-      <c r="C19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" t="s">
+    </row>
+    <row r="20" spans="1:4" ht="66" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="60">
-      <c r="A20" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="3" t="s">
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
         <v>286</v>
       </c>
-      <c r="C20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" t="s">
+    </row>
+    <row r="21" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="60">
-      <c r="A21" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="3" t="s">
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
         <v>288</v>
       </c>
-      <c r="C21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" t="s">
+    </row>
+    <row r="22" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="45">
-      <c r="A22" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="3" t="s">
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" t="s">
         <v>290</v>
       </c>
-      <c r="C22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" t="s">
+    </row>
+    <row r="23" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="30">
-      <c r="A23" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" s="3" t="s">
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" t="s">
         <v>292</v>
       </c>
-      <c r="C23" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" t="s">
+    </row>
+    <row r="24" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="30">
-      <c r="A24" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" s="3" t="s">
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" t="s">
         <v>294</v>
       </c>
-      <c r="C24" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" t="s">
+    </row>
+    <row r="25" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B25" s="3" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="30">
-      <c r="B25" s="3" t="s">
+      <c r="D25" t="s">
         <v>296</v>
       </c>
-      <c r="D25" t="s">
+    </row>
+    <row r="26" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B26" s="3" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="30">
-      <c r="B26" s="3" t="s">
+      <c r="D26" t="s">
         <v>298</v>
       </c>
-      <c r="D26" t="s">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B27" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15">
-      <c r="B27" s="3" t="s">
+    <row r="28" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="45">
-      <c r="A28" t="s">
-        <v>6</v>
-      </c>
-      <c r="B28" s="3" t="s">
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" t="s">
         <v>301</v>
       </c>
-      <c r="C28" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" t="s">
+    </row>
+    <row r="29" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="45">
-      <c r="A29" t="s">
-        <v>6</v>
-      </c>
-      <c r="B29" s="3" t="s">
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" t="s">
         <v>303</v>
       </c>
-      <c r="C29" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" t="s">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B30" s="3" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="15">
-      <c r="B30" s="3" t="s">
+      <c r="D30" t="s">
         <v>305</v>
       </c>
-      <c r="D30" t="s">
+    </row>
+    <row r="31" spans="1:4" ht="66" x14ac:dyDescent="0.2">
+      <c r="B31" s="3" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="75">
-      <c r="B31" s="3" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B32" s="3" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="15">
-      <c r="B32" s="3" t="s">
+      <c r="D32" t="s">
         <v>308</v>
       </c>
-      <c r="D32" t="s">
+    </row>
+    <row r="33" spans="1:4" ht="43.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="3" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="43.35" customHeight="1">
-      <c r="B33" s="3" t="s">
+      <c r="D33" t="s">
         <v>310</v>
       </c>
-      <c r="D33" t="s">
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B34" s="3" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="15">
-      <c r="B34" s="3" t="s">
+      <c r="D34" t="s">
         <v>312</v>
       </c>
-      <c r="D34" t="s">
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="15">
-      <c r="A35" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" s="3" t="s">
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" t="s">
         <v>314</v>
       </c>
-      <c r="C35" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" t="s">
+    </row>
+    <row r="36" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="60">
-      <c r="A36" t="s">
-        <v>6</v>
-      </c>
-      <c r="B36" s="3" t="s">
+      <c r="C36" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" t="s">
         <v>316</v>
       </c>
-      <c r="C36" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" t="s">
+    </row>
+    <row r="37" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B37" s="3" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="15">
-      <c r="B37" s="3" t="s">
+      <c r="D37" t="s">
         <v>318</v>
       </c>
-      <c r="D37" t="s">
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B38" s="3" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15">
-      <c r="B38" s="3" t="s">
+    <row r="39" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="3" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" ht="42" customHeight="1">
-      <c r="B39" s="3" t="s">
+      <c r="D39" t="s">
         <v>321</v>
       </c>
-      <c r="D39" t="s">
+    </row>
+    <row r="40" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B40" s="3" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="45">
-      <c r="B40" s="3" t="s">
+      <c r="D40" t="s">
         <v>323</v>
       </c>
-      <c r="D40" t="s">
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B41" s="3" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15">
-      <c r="B41" s="3" t="s">
+    <row r="42" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" ht="60">
-      <c r="A42" t="s">
-        <v>6</v>
-      </c>
-      <c r="B42" s="3" t="s">
+      <c r="C42" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" t="s">
         <v>326</v>
       </c>
-      <c r="C42" t="s">
-        <v>6</v>
-      </c>
-      <c r="D42" t="s">
+    </row>
+    <row r="43" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B43" s="3" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" ht="15">
-      <c r="B43" s="3" t="s">
+      <c r="D43" t="s">
         <v>328</v>
       </c>
-      <c r="D43" t="s">
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B44" s="3" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" ht="15">
-      <c r="B44" s="3" t="s">
+      <c r="D44" t="s">
         <v>330</v>
       </c>
-      <c r="D44" t="s">
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B45" s="3" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" ht="15">
-      <c r="B45" s="3" t="s">
+      <c r="D45" t="s">
         <v>332</v>
       </c>
-      <c r="D45" t="s">
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B46" s="3" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" ht="15">
-      <c r="B46" s="3" t="s">
+      <c r="D46" t="s">
         <v>334</v>
       </c>
-      <c r="D46" t="s">
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B47" s="3" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" ht="15">
-      <c r="B47" s="3" t="s">
+      <c r="D47" t="s">
         <v>336</v>
       </c>
-      <c r="D47" t="s">
+    </row>
+    <row r="48" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>6</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" ht="30">
-      <c r="A48" t="s">
-        <v>6</v>
-      </c>
-      <c r="B48" s="3" t="s">
+      <c r="C48" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" t="s">
         <v>338</v>
-      </c>
-      <c r="C48" t="s">
-        <v>6</v>
-      </c>
-      <c r="D48" t="s">
-        <v>339</v>
       </c>
     </row>
   </sheetData>
@@ -9452,31 +9516,31 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.1"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.625" customWidth="1"/>
-    <col min="2" max="2" width="100.625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.625" customWidth="1"/>
-    <col min="4" max="4" width="20.625" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30">
+    <row r="1" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -9484,236 +9548,236 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="184.8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="195">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15">
-      <c r="B7" s="1" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="45">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15">
-      <c r="B9" s="1" t="s">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="15">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
         <v>346</v>
       </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" t="s">
+    </row>
+    <row r="11" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="60">
-      <c r="B11" s="1" t="s">
+      <c r="D11" t="s">
         <v>348</v>
       </c>
-      <c r="D11" t="s">
+    </row>
+    <row r="12" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="60">
-      <c r="B12" s="1" t="s">
+      <c r="D12" t="s">
         <v>350</v>
       </c>
-      <c r="D12" t="s">
+    </row>
+    <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="30">
-      <c r="B13" s="1" t="s">
+      <c r="D13" t="s">
         <v>352</v>
       </c>
-      <c r="D13" t="s">
+    </row>
+    <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B14" s="2" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="15">
-      <c r="B14" s="2" t="s">
+      <c r="D14" t="s">
         <v>354</v>
       </c>
-      <c r="D14" t="s">
+    </row>
+    <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="30">
-      <c r="B15" s="1" t="s">
+      <c r="D15" t="s">
         <v>356</v>
       </c>
-      <c r="D15" t="s">
+    </row>
+    <row r="16" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="45">
-      <c r="B16" s="1" t="s">
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
         <v>358</v>
       </c>
-      <c r="C16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" t="s">
+    </row>
+    <row r="17" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="60">
-      <c r="B17" s="1" t="s">
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
         <v>360</v>
       </c>
-      <c r="C17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" t="s">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15">
-      <c r="B18" s="1" t="s">
+    <row r="19" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="45">
-      <c r="B19" s="1" t="s">
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s">
         <v>363</v>
       </c>
-      <c r="C19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" t="s">
+    </row>
+    <row r="20" spans="1:4" ht="66" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="75">
-      <c r="A20" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="C20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="60">
-      <c r="B21" s="1" t="s">
+      <c r="D21" t="s">
         <v>366</v>
       </c>
-      <c r="D21" t="s">
+    </row>
+    <row r="22" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="120">
-      <c r="A22" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" t="s">
         <v>368</v>
       </c>
-      <c r="C22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" t="s">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15">
-      <c r="B24" s="1" t="s">
+    <row r="25" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="30">
-      <c r="A25" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25" s="1" t="s">
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>371</v>
-      </c>
-      <c r="C25" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="90">
-      <c r="A26" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>372</v>
       </c>
       <c r="C26" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="120">
+    <row r="27" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>6</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C27" t="s">
         <v>18</v>
       </c>
       <c r="D27" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="132" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>374</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="150">
-      <c r="A28" t="s">
-        <v>6</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>375</v>
       </c>
       <c r="C28" t="s">
         <v>18</v>
       </c>
       <c r="D28" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mac: fix a typo in href
</commit_message>
<xml_diff>
--- a/macs+lan.xlsx
+++ b/macs+lan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{994B0864-DD5F-4FB4-8734-8147005953D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71AB0D88-7FB7-4DDD-ADE9-DA88F56235D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7764" tabRatio="772" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6347,7 +6347,7 @@
   </si>
   <si>
     <t>WiFiネットワークを選択の画面。自分が使用できるSSIDを選択してください。 
-このスクリーンショットではパスワードのみの認証の場合を示しますが、アカウントとパスワードの両方が必要なWiFiにも接続できる筈です。もしどうしても接続できない場合(macOSが古いとできない場合があります)は&lt;a href="../../2023/mac+lan/"&gt;2023年版&lt;/a&gt;を参照してください。</t>
+このスクリーンショットではパスワードのみの認証の場合を示しますが、アカウントとパスワードの両方が必要なWiFiにも接続できる筈です。もしどうしても接続できない場合(macOSが古いとできない場合があります)は&lt;a href="../../2023/macs+lan/"&gt;2023年版&lt;/a&gt;を参照してください。</t>
     <rPh sb="62" eb="64">
       <t>ニンショウ</t>
     </rPh>
@@ -6381,10 +6381,10 @@
     <rPh sb="136" eb="138">
       <t>バアイ</t>
     </rPh>
-    <rPh sb="179" eb="181">
+    <rPh sb="180" eb="182">
       <t>ネンバン</t>
     </rPh>
-    <rPh sb="186" eb="188">
+    <rPh sb="187" eb="189">
       <t>サンショウ</t>
     </rPh>
     <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
mac: do first step without network (as 2023)
</commit_message>
<xml_diff>
--- a/macs+lan.xlsx
+++ b/macs+lan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71AB0D88-7FB7-4DDD-ADE9-DA88F56235D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B9E9EB5-8E97-4ED1-86CF-C23DC3946D34}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7764" tabRatio="772" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="445">
   <si>
     <t>header1</t>
   </si>
@@ -441,19 +441,6 @@
   </si>
   <si>
     <t>0_3.jpeg</t>
-  </si>
-  <si>
-    <t>0_4.jpeg</t>
-  </si>
-  <si>
-    <t>ご自宅のWiFiがパスワード保護されている場合は入力してください。 「続ける」をクリックしてください。</t>
-    <rPh sb="0" eb="27">
-      <t>ツヅ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0_5.jpeg</t>
   </si>
   <si>
     <t>「データとプライバシー」の画面になります。ここでは何も設定することができませんが、通知を理解した上で、「続ける」をクリックします。</t>
@@ -6346,48 +6333,22 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>WiFiネットワークを選択の画面。自分が使用できるSSIDを選択してください。 
-このスクリーンショットではパスワードのみの認証の場合を示しますが、アカウントとパスワードの両方が必要なWiFiにも接続できる筈です。もしどうしても接続できない場合(macOSが古いとできない場合があります)は&lt;a href="../../2023/macs+lan/"&gt;2023年版&lt;/a&gt;を参照してください。</t>
-    <rPh sb="62" eb="64">
-      <t>ニンショウ</t>
-    </rPh>
-    <rPh sb="65" eb="67">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="68" eb="69">
-      <t>シメ</t>
-    </rPh>
-    <rPh sb="86" eb="88">
-      <t>リョウホウ</t>
-    </rPh>
-    <rPh sb="89" eb="91">
-      <t>ヒツヨウ</t>
-    </rPh>
-    <rPh sb="98" eb="100">
-      <t>セツゾク</t>
-    </rPh>
-    <rPh sb="103" eb="104">
-      <t>ハズ</t>
-    </rPh>
-    <rPh sb="114" eb="116">
-      <t>セツゾク</t>
-    </rPh>
-    <rPh sb="120" eb="122">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="129" eb="130">
-      <t>フル</t>
-    </rPh>
-    <rPh sb="136" eb="138">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="180" eb="182">
-      <t>ネンバン</t>
-    </rPh>
-    <rPh sb="187" eb="189">
-      <t>サンショウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
+    <t>次に「Wi-Fiネットワークを選択」の画面になりますが、これはあとでやりますので、「その他のネットワークオプション」をクリックします。</t>
+  </si>
+  <si>
+    <t>0_4_1.jpeg</t>
+  </si>
+  <si>
+    <t>次に「インターネットの接続方法」の画面になりますが、いまは「コンピュータをインターネットに接続しない」を選択してください。 「続ける」をクリックします。</t>
+  </si>
+  <si>
+    <t>0_4_2.jpeg</t>
+  </si>
+  <si>
+    <t>本当にネットワーク接続しなくて良いのかしつこくもう一回聞かれますが、「続ける」をクリックして振り切ってください。</t>
+  </si>
+  <si>
+    <t>0_4_3.jpeg</t>
   </si>
 </sst>
 </file>
@@ -6889,7 +6850,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6897,7 +6858,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6913,17 +6874,17 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -6931,7 +6892,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
@@ -6942,13 +6903,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -6956,13 +6917,13 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6970,13 +6931,13 @@
         <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -6984,13 +6945,13 @@
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -6998,13 +6959,13 @@
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="C13" t="s">
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
   </sheetData>
@@ -7032,10 +6993,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7043,7 +7004,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7059,17 +7020,17 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7077,33 +7038,33 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="D9" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="D10" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="171.6" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -7145,7 +7106,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7153,7 +7114,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7169,7 +7130,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -7177,7 +7138,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -7191,7 +7152,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -7201,13 +7162,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7215,24 +7176,24 @@
         <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -7240,13 +7201,13 @@
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C13" t="s">
         <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -7254,40 +7215,40 @@
         <v>6</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="C14" t="s">
         <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="C16" t="s">
         <v>18</v>
       </c>
       <c r="D16" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="C17" t="s">
         <v>18</v>
       </c>
       <c r="D17" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -7295,13 +7256,13 @@
         <v>6</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C18" t="s">
         <v>18</v>
       </c>
       <c r="D18" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7309,24 +7270,24 @@
         <v>6</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="C19" t="s">
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="92.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="C20" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D20" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -7334,13 +7295,13 @@
         <v>6</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="C21" t="s">
         <v>18</v>
       </c>
       <c r="D21" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7348,35 +7309,35 @@
         <v>6</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="C22" t="s">
         <v>18</v>
       </c>
       <c r="D22" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C23" t="s">
         <v>18</v>
       </c>
       <c r="D23" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="C24" t="s">
         <v>18</v>
       </c>
       <c r="D24" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7384,13 +7345,13 @@
         <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="C25" t="s">
         <v>18</v>
       </c>
       <c r="D25" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -7398,18 +7359,18 @@
         <v>6</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="C26" t="s">
         <v>18</v>
       </c>
       <c r="D26" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
   </sheetData>
@@ -7421,10 +7382,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A14" sqref="A14:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -7528,57 +7489,51 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>440</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
       <c r="B12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" t="s">
-        <v>18</v>
+        <v>441</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>442</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
       <c r="B13" s="1" t="s">
-        <v>27</v>
+        <v>443</v>
       </c>
       <c r="C13" t="s">
         <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>444</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>6</v>
-      </c>
       <c r="B14" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
         <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7586,151 +7541,165 @@
         <v>6</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
         <v>18</v>
       </c>
       <c r="D15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>6</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C16" t="s">
         <v>18</v>
       </c>
       <c r="D16" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
       <c r="B17" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
         <v>18</v>
       </c>
       <c r="D17" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C18" t="s">
         <v>18</v>
       </c>
       <c r="D18" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C19" t="s">
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
         <v>18</v>
       </c>
       <c r="D20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C21" t="s">
         <v>18</v>
       </c>
       <c r="D21" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C22" t="s">
         <v>18</v>
       </c>
       <c r="D22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C23" t="s">
         <v>18</v>
       </c>
       <c r="D23" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C24" t="s">
         <v>18</v>
       </c>
       <c r="D24" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C25" t="s">
         <v>18</v>
       </c>
       <c r="D25" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C26" t="s">
         <v>18</v>
       </c>
       <c r="D26" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>6</v>
-      </c>
       <c r="B27" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C27" t="s">
         <v>18</v>
       </c>
       <c r="D27" t="s">
-        <v>56</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -7761,7 +7730,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7769,7 +7738,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7785,7 +7754,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
@@ -7793,7 +7762,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -7807,13 +7776,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -7821,13 +7790,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7835,21 +7804,21 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D10" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -7857,13 +7826,13 @@
         <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -7871,24 +7840,24 @@
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C13" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D13" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7896,24 +7865,24 @@
         <v>6</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C14" t="s">
         <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C15" t="s">
         <v>18</v>
       </c>
       <c r="D15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -7944,7 +7913,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7952,7 +7921,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7968,54 +7937,54 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D9" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D10" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D11" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D12" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8023,29 +7992,29 @@
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C13" t="s">
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D14" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D15" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -8053,18 +8022,18 @@
         <v>6</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D17" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -8072,34 +8041,34 @@
         <v>6</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D18" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D19" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D20" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="83.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D21" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -8107,10 +8076,10 @@
         <v>6</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D22" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -8118,10 +8087,10 @@
         <v>6</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D23" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -8129,18 +8098,18 @@
         <v>6</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D24" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D25" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -8148,10 +8117,10 @@
         <v>6</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D26" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8159,10 +8128,10 @@
         <v>6</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D27" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8170,10 +8139,10 @@
         <v>6</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D28" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8181,10 +8150,10 @@
         <v>6</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D29" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -8192,10 +8161,10 @@
         <v>6</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D30" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -8203,10 +8172,10 @@
         <v>6</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D31" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -8214,10 +8183,10 @@
         <v>6</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D32" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8225,10 +8194,10 @@
         <v>6</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D33" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8236,10 +8205,10 @@
         <v>6</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D34" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -8247,130 +8216,130 @@
         <v>6</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D35" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D36" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D37" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D38" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D39" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D40" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D41" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D42" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D43" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D44" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D45" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D46" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D47" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B48" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D48" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B49" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D49" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B50" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D50" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -8401,7 +8370,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8409,7 +8378,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8425,7 +8394,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8433,7 +8402,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -8444,10 +8413,10 @@
     </row>
     <row r="7" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D7" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -8455,13 +8424,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -8492,7 +8461,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8500,7 +8469,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8516,7 +8485,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -8524,7 +8493,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -8535,7 +8504,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8543,13 +8512,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -8557,13 +8526,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -8571,40 +8540,40 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D13" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -8612,13 +8581,13 @@
         <v>6</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C14" t="s">
         <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -8626,13 +8595,13 @@
         <v>6</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C15" t="s">
         <v>18</v>
       </c>
       <c r="D15" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8640,7 +8609,7 @@
         <v>6</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C16" t="s">
         <v>18</v>
@@ -8651,7 +8620,7 @@
         <v>6</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C17" t="s">
         <v>18</v>
@@ -8662,10 +8631,10 @@
         <v>6</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D18" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8673,98 +8642,98 @@
         <v>6</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D19" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D20" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D21" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D22" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D23" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D24" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D25" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D26" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D27" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D28" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D29" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D30" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -8795,7 +8764,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8803,7 +8772,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8819,7 +8788,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -8827,7 +8796,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -8838,17 +8807,17 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -8856,29 +8825,29 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8886,29 +8855,29 @@
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C13" t="s">
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D14" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D15" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -8916,13 +8885,13 @@
         <v>6</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="198" x14ac:dyDescent="0.2">
@@ -8930,18 +8899,18 @@
         <v>6</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C17" t="s">
         <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8949,21 +8918,21 @@
         <v>6</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C19" t="s">
         <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D20" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8971,21 +8940,21 @@
         <v>6</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
       </c>
       <c r="D21" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D22" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8993,13 +8962,13 @@
         <v>6</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C23" t="s">
         <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -9058,7 +9027,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -9066,7 +9035,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -9082,7 +9051,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -9090,7 +9059,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -9101,12 +9070,12 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="132" x14ac:dyDescent="0.2">
@@ -9114,13 +9083,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -9128,18 +9097,18 @@
         <v>6</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D10" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D11" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9147,58 +9116,58 @@
         <v>6</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="3" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B14" s="3" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D14" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D15" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B16" s="3" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D16" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D17" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D18" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9206,13 +9175,13 @@
         <v>6</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C19" t="s">
         <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -9220,13 +9189,13 @@
         <v>6</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C20" t="s">
         <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -9234,13 +9203,13 @@
         <v>6</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
       </c>
       <c r="D21" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -9248,13 +9217,13 @@
         <v>6</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
       </c>
       <c r="D22" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9262,13 +9231,13 @@
         <v>6</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C23" t="s">
         <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9276,34 +9245,34 @@
         <v>6</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C24" t="s">
         <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B25" s="3" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D25" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B26" s="3" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D26" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" s="3" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -9311,13 +9280,13 @@
         <v>6</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C28" t="s">
         <v>6</v>
       </c>
       <c r="D28" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -9325,50 +9294,50 @@
         <v>6</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C29" t="s">
         <v>6</v>
       </c>
       <c r="D29" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B30" s="3" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D30" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B31" s="3" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B32" s="3" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D32" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="43.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="3" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D33" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B34" s="3" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D34" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -9376,13 +9345,13 @@
         <v>6</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C35" t="s">
         <v>6</v>
       </c>
       <c r="D35" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -9390,47 +9359,47 @@
         <v>6</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C36" t="s">
         <v>6</v>
       </c>
       <c r="D36" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B37" s="3" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D37" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B38" s="3" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="3" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="D39" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B40" s="3" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D40" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B41" s="3" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -9438,53 +9407,53 @@
         <v>6</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C42" t="s">
         <v>6</v>
       </c>
       <c r="D42" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B43" s="3" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D43" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B44" s="3" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="D44" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B45" s="3" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="D45" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B46" s="3" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="D46" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B47" s="3" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D47" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9492,13 +9461,13 @@
         <v>6</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C48" t="s">
         <v>6</v>
       </c>
       <c r="D48" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
   </sheetData>
@@ -9529,7 +9498,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -9537,7 +9506,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -9553,7 +9522,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="184.8" x14ac:dyDescent="0.2">
@@ -9561,7 +9530,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -9572,7 +9541,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -9580,18 +9549,18 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -9599,91 +9568,91 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="D11" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D12" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D13" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D14" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="D15" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C17" t="s">
         <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="C19" t="s">
         <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -9691,21 +9660,21 @@
         <v>6</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C20" t="s">
         <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="D21" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -9713,18 +9682,18 @@
         <v>6</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
       </c>
       <c r="D22" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9732,7 +9701,7 @@
         <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="C25" t="s">
         <v>6</v>
@@ -9746,7 +9715,7 @@
         <v>6</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="C26" t="s">
         <v>18</v>
@@ -9757,13 +9726,13 @@
         <v>6</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="C27" t="s">
         <v>18</v>
       </c>
       <c r="D27" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="132" x14ac:dyDescent="0.2">
@@ -9771,13 +9740,13 @@
         <v>6</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="C28" t="s">
         <v>18</v>
       </c>
       <c r="D28" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mac: fix check number
</commit_message>
<xml_diff>
--- a/macs+lan.xlsx
+++ b/macs+lan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B9E9EB5-8E97-4ED1-86CF-C23DC3946D34}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C21F6A8-7C45-4F3D-A9E4-754F2CCA6BF6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7764" tabRatio="772" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7764" tabRatio="772" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -890,52 +890,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>2023年3月で最新のmacOS Ventura (13.x)ではこのようなパネルが開きます。①チップ、②メモリ、③macOSのバージョン番号をメモしておきましょう。あるいはこのパネルの写真を撮っておきましょう。続いて、④詳細情報に進みます。
-&lt;span class="check"&gt;check 1&lt;/span&gt;
-現在サポートが続いているmacOSはすべて64ビットOSです。
-&lt;span class="check"&gt;check 2&lt;/span&gt;</t>
-    <rPh sb="4" eb="5">
-      <t>ネン</t>
-    </rPh>
-    <rPh sb="6" eb="7">
-      <t>ガツ</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>サイシン</t>
-    </rPh>
-    <rPh sb="42" eb="43">
-      <t>ヒラ</t>
-    </rPh>
-    <rPh sb="69" eb="71">
-      <t>バンゴウ</t>
-    </rPh>
-    <rPh sb="93" eb="95">
-      <t>シャシン</t>
-    </rPh>
-    <rPh sb="96" eb="97">
-      <t>ト</t>
-    </rPh>
-    <rPh sb="106" eb="107">
-      <t>ツヅ</t>
-    </rPh>
-    <rPh sb="111" eb="113">
-      <t>ショウサイ</t>
-    </rPh>
-    <rPh sb="113" eb="115">
-      <t>ジョウホウ</t>
-    </rPh>
-    <rPh sb="116" eb="117">
-      <t>スス</t>
-    </rPh>
-    <rPh sb="157" eb="159">
-      <t>ゲンザイ</t>
-    </rPh>
-    <rPh sb="164" eb="165">
-      <t>ツヅ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>macos-about-ventura.png</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -3137,138 +3091,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">ログインしたら、この画面（ダッシュボード）が出ます。&lt;span class="check"&gt;check 13&lt;/span&gt;
-真ん中に見える「コースツリー」に、あなたがアクセスできるコースが表示されています。これらは、あなたの履修課目に関する授業支援や、広島大学において自習すべき教材などのコースです。（この図は在学生向けの一例で、新入生に表示されるものとは異なります）
-新入生向けに共通で表示されるものを簡単に説明すると：
-&lt;dl&gt;
-&lt;dt&gt;ノートパソコン点検届&lt;/dt&gt;
-&lt;dd&gt;あなたの必携PCが、きちんと大学で使える状態になっているか確認するため、大学に「ノートパソコン点検届」を提出する必要があります。このコースでは、点検届が提出できます。&lt;strong&gt;このテキストによる設定・点検を済ませたあと、できるだけ早くにこのコースを開いて点検届を提出してください。&lt;/strong&gt;&lt;/dd&gt;
-&lt;dt&gt;MFA設定ガイド&lt;/dt&gt;
-&lt;dd&gt;広島大学ではパスワード窃取によるアカウント乗っ取りの防止策として、広大IDを持つ全ての構成員に対しIMCアカウントおよび広大IDの多要素認証（MFA）設定を義務付けています。この「MFA設定ガイド」で、広島大学でMFA設定を行うための手順を説明しています&lt;/dd&gt; &lt;/dl&gt;
-</t>
-    <rPh sb="66" eb="67">
-      <t>ミ</t>
-    </rPh>
-    <rPh sb="112" eb="114">
-      <t>リシュウ</t>
-    </rPh>
-    <rPh sb="114" eb="116">
-      <t>カモク</t>
-    </rPh>
-    <rPh sb="117" eb="118">
-      <t>カン</t>
-    </rPh>
-    <rPh sb="120" eb="122">
-      <t>ジュギョウ</t>
-    </rPh>
-    <rPh sb="122" eb="124">
-      <t>シエン</t>
-    </rPh>
-    <rPh sb="126" eb="128">
-      <t>ヒロシマ</t>
-    </rPh>
-    <rPh sb="128" eb="130">
-      <t>ダイガク</t>
-    </rPh>
-    <rPh sb="134" eb="136">
-      <t>ジシュウ</t>
-    </rPh>
-    <rPh sb="139" eb="141">
-      <t>キョウザイ</t>
-    </rPh>
-    <rPh sb="158" eb="159">
-      <t>ム</t>
-    </rPh>
-    <rPh sb="185" eb="188">
-      <t>シンニュウセイ</t>
-    </rPh>
-    <rPh sb="188" eb="189">
-      <t>ム</t>
-    </rPh>
-    <rPh sb="191" eb="193">
-      <t>キョウツウ</t>
-    </rPh>
-    <rPh sb="194" eb="196">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="341" eb="343">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="344" eb="346">
-      <t>テンケン</t>
-    </rPh>
-    <rPh sb="347" eb="348">
-      <t>ス</t>
-    </rPh>
-    <rPh sb="359" eb="360">
-      <t>ハヤ</t>
-    </rPh>
-    <rPh sb="368" eb="369">
-      <t>ヒラ</t>
-    </rPh>
-    <rPh sb="406" eb="408">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="421" eb="425">
-      <t>ヒロシマダイガク</t>
-    </rPh>
-    <rPh sb="432" eb="434">
-      <t>セッシュ</t>
-    </rPh>
-    <rPh sb="442" eb="443">
-      <t>ノ</t>
-    </rPh>
-    <rPh sb="444" eb="445">
-      <t>ト</t>
-    </rPh>
-    <rPh sb="454" eb="456">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="459" eb="460">
-      <t>モ</t>
-    </rPh>
-    <rPh sb="461" eb="462">
-      <t>スベ</t>
-    </rPh>
-    <rPh sb="464" eb="467">
-      <t>コウセイイン</t>
-    </rPh>
-    <rPh sb="468" eb="469">
-      <t>タイ</t>
-    </rPh>
-    <rPh sb="481" eb="483">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="486" eb="491">
-      <t>タヨウソニンショウ</t>
-    </rPh>
-    <rPh sb="496" eb="498">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="499" eb="502">
-      <t>ギムヅ</t>
-    </rPh>
-    <rPh sb="514" eb="516">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="522" eb="526">
-      <t>ヒロシマダイガク</t>
-    </rPh>
-    <rPh sb="530" eb="532">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="533" eb="534">
-      <t>オコナ</t>
-    </rPh>
-    <rPh sb="538" eb="540">
-      <t>テジュン</t>
-    </rPh>
-    <rPh sb="541" eb="543">
-      <t>セツメイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>moodle-dashboard-ja.svg</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -3341,46 +3163,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>教材の下の方にある「IMCアカウントのMFA利用設定実習」をクリックして、説明に従ってIMCアカウントの多要素認証（MFA）設定を進めましょう。詳細は教材の各項目の資料を見てください。&lt;span class="check"&gt;check 9&lt;/span&gt;</t>
-    <rPh sb="0" eb="2">
-      <t>キョウザイ</t>
-    </rPh>
-    <rPh sb="3" eb="4">
-      <t>シタ</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>ホウ</t>
-    </rPh>
-    <rPh sb="37" eb="39">
-      <t>セツメイ</t>
-    </rPh>
-    <rPh sb="40" eb="41">
-      <t>シタガ</t>
-    </rPh>
-    <rPh sb="52" eb="57">
-      <t>タヨウソニンショウ</t>
-    </rPh>
-    <rPh sb="62" eb="64">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="65" eb="66">
-      <t>スス</t>
-    </rPh>
-    <rPh sb="72" eb="74">
-      <t>ショウサイ</t>
-    </rPh>
-    <rPh sb="78" eb="81">
-      <t>カクコウモク</t>
-    </rPh>
-    <rPh sb="82" eb="84">
-      <t>シリョウ</t>
-    </rPh>
-    <rPh sb="85" eb="86">
-      <t>ミ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>moodle-mfaimc-below.svg</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -3414,50 +3196,6 @@
   </si>
   <si>
     <t>moodle-mfa-hirodai.svg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">教材の下の方にある「広大IDのMFA利用設定実習」をクリックして、説明に従って広大IDの多要素認証（MFA）設定を進めましょう。詳細は教材の各項目の資料を見てください。&lt;span class="check"&gt;check 10&lt;/span&gt;
-</t>
-    <rPh sb="0" eb="2">
-      <t>キョウザイ</t>
-    </rPh>
-    <rPh sb="3" eb="4">
-      <t>シタ</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>ホウ</t>
-    </rPh>
-    <rPh sb="33" eb="35">
-      <t>セツメイ</t>
-    </rPh>
-    <rPh sb="36" eb="37">
-      <t>シタガ</t>
-    </rPh>
-    <rPh sb="39" eb="41">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="44" eb="49">
-      <t>タヨウソニンショウ</t>
-    </rPh>
-    <rPh sb="54" eb="56">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="57" eb="58">
-      <t>スス</t>
-    </rPh>
-    <rPh sb="64" eb="66">
-      <t>ショウサイ</t>
-    </rPh>
-    <rPh sb="70" eb="73">
-      <t>カクコウモク</t>
-    </rPh>
-    <rPh sb="74" eb="76">
-      <t>シリョウ</t>
-    </rPh>
-    <rPh sb="77" eb="78">
-      <t>ミ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -4205,35 +3943,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">Excelの新規作成の画面に戻ります。左上(①)にメディアセンタが登録している貴方の名前、左下(②)にライセンス認証のアイコンがないことを確認してください。これで、PowerPointやWordなどMicrosoft Officeの他のアプリケーションも使えるようになります。&lt;span class="check"&gt;check-12&lt;/span&gt;
-  </t>
-    <rPh sb="14" eb="15">
-      <t>モド</t>
-    </rPh>
-    <rPh sb="19" eb="21">
-      <t>ヒダリウエ</t>
-    </rPh>
-    <rPh sb="33" eb="35">
-      <t>トウロク</t>
-    </rPh>
-    <rPh sb="39" eb="41">
-      <t>アナタ</t>
-    </rPh>
-    <rPh sb="42" eb="44">
-      <t>ナマエ</t>
-    </rPh>
-    <rPh sb="45" eb="47">
-      <t>ヒダリシタ</t>
-    </rPh>
-    <rPh sb="56" eb="58">
-      <t>ニンショウ</t>
-    </rPh>
-    <rPh sb="69" eb="71">
-      <t>カクニン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>mac-4-14.png</t>
   </si>
   <si>
@@ -4456,17 +4165,6 @@
   </si>
   <si>
     <t>ch5-office365-updater-latest-list.png</t>
-  </si>
-  <si>
-    <t>メニューの「Microsoft Autoupdateを終了します」をクリックすると、終了できます。 ウィンドウを閉じるのでも構いません。
-&lt;span class="check"&gt;check 12&lt;/span&gt;</t>
-    <rPh sb="56" eb="57">
-      <t>ト</t>
-    </rPh>
-    <rPh sb="62" eb="63">
-      <t>カマ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>mac-4-18.png</t>
@@ -4825,18 +4523,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">するとこのような画面になります。&lt;span class="check"&gt;check 13&lt;/span&gt;
-これを「Myもみじのトップページ」と呼ぶことにしましょう。
-履修登録をしたり、成績を確認することができます。
-また「掲示」では、授業や学部からの連絡が表示されます。
-このまま引き続いて、次の「Moodle」の使い方に進みましょう。
-  </t>
-    <rPh sb="70" eb="71">
-      <t>ヨ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>win10-6-11a.svg</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -5035,45 +4721,6 @@
   </si>
   <si>
     <t>mac-3-3.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">この画面になったら「続ける」で進めてください。不安がある場合は証明書を表示してください(2023年春の時点ではNII Open Domain CAが発行した証明書が表示されます)。
-これで接続の設定が完了しました。 接続が完了すると「接続済み」と表示されます。&lt;span class="check"&gt;check 14&lt;/span&gt;
-  </t>
-    <rPh sb="15" eb="16">
-      <t>スス</t>
-    </rPh>
-    <rPh sb="23" eb="25">
-      <t>フアン</t>
-    </rPh>
-    <rPh sb="28" eb="30">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="31" eb="34">
-      <t>ショウメイショ</t>
-    </rPh>
-    <rPh sb="35" eb="37">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="48" eb="49">
-      <t>ネン</t>
-    </rPh>
-    <rPh sb="49" eb="50">
-      <t>ハル</t>
-    </rPh>
-    <rPh sb="51" eb="53">
-      <t>ジテン</t>
-    </rPh>
-    <rPh sb="74" eb="76">
-      <t>ハッコウ</t>
-    </rPh>
-    <rPh sb="78" eb="81">
-      <t>ショウメイショ</t>
-    </rPh>
-    <rPh sb="82" eb="84">
-      <t>ヒョウジ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -6349,6 +5996,333 @@
   </si>
   <si>
     <t>0_4_3.jpeg</t>
+  </si>
+  <si>
+    <t>2024年3月で最新のmacOS Sonoma (14.x)ではこのようなパネルが開きます。①チップ、②メモリ、③macOSのバージョン番号をメモしておきましょう。あるいはこのパネルの写真を撮っておきましょう。続いて、④詳細情報に進みます。
+&lt;span class="check"&gt;check 1&lt;/span&gt;</t>
+    <rPh sb="4" eb="5">
+      <t>ネン</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>ガツ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>サイシン</t>
+    </rPh>
+    <rPh sb="41" eb="42">
+      <t>ヒラ</t>
+    </rPh>
+    <rPh sb="68" eb="70">
+      <t>バンゴウ</t>
+    </rPh>
+    <rPh sb="92" eb="94">
+      <t>シャシン</t>
+    </rPh>
+    <rPh sb="95" eb="96">
+      <t>ト</t>
+    </rPh>
+    <rPh sb="105" eb="106">
+      <t>ツヅ</t>
+    </rPh>
+    <rPh sb="110" eb="112">
+      <t>ショウサイ</t>
+    </rPh>
+    <rPh sb="112" eb="114">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="115" eb="116">
+      <t>スス</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ログインしたら、この画面（ダッシュボード）が出ます。&lt;span class="check"&gt;check 12&lt;/span&gt;
+真ん中に見える「コースツリー」に、あなたがアクセスできるコースが表示されています。これらは、あなたの履修課目に関する授業支援や、広島大学において自習すべき教材などのコースです。（この図は在学生向けの一例で、新入生に表示されるものとは異なります）
+新入生向けに共通で表示されるものを簡単に説明すると：
+&lt;dl&gt;
+&lt;dt&gt;ノートパソコン点検届&lt;/dt&gt;
+&lt;dd&gt;あなたの必携PCが、きちんと大学で使える状態になっているか確認するため、大学に「ノートパソコン点検届」を提出する必要があります。このコースでは、点検届が提出できます。&lt;strong&gt;このテキストによる設定・点検を済ませたあと、できるだけ早くにこのコースを開いて点検届を提出してください。&lt;/strong&gt;&lt;/dd&gt;
+&lt;dt&gt;MFA設定ガイド&lt;/dt&gt;
+&lt;dd&gt;広島大学ではパスワード窃取によるアカウント乗っ取りの防止策として、広大IDを持つ全ての構成員に対しIMCアカウントおよび広大IDの多要素認証（MFA）設定を義務付けています。この「MFA設定ガイド」で、広島大学でMFA設定を行うための手順を説明しています&lt;/dd&gt; &lt;/dl&gt;
+</t>
+    <rPh sb="66" eb="67">
+      <t>ミ</t>
+    </rPh>
+    <rPh sb="112" eb="114">
+      <t>リシュウ</t>
+    </rPh>
+    <rPh sb="114" eb="116">
+      <t>カモク</t>
+    </rPh>
+    <rPh sb="117" eb="118">
+      <t>カン</t>
+    </rPh>
+    <rPh sb="120" eb="122">
+      <t>ジュギョウ</t>
+    </rPh>
+    <rPh sb="122" eb="124">
+      <t>シエン</t>
+    </rPh>
+    <rPh sb="126" eb="128">
+      <t>ヒロシマ</t>
+    </rPh>
+    <rPh sb="128" eb="130">
+      <t>ダイガク</t>
+    </rPh>
+    <rPh sb="134" eb="136">
+      <t>ジシュウ</t>
+    </rPh>
+    <rPh sb="139" eb="141">
+      <t>キョウザイ</t>
+    </rPh>
+    <rPh sb="158" eb="159">
+      <t>ム</t>
+    </rPh>
+    <rPh sb="185" eb="188">
+      <t>シンニュウセイ</t>
+    </rPh>
+    <rPh sb="188" eb="189">
+      <t>ム</t>
+    </rPh>
+    <rPh sb="191" eb="193">
+      <t>キョウツウ</t>
+    </rPh>
+    <rPh sb="194" eb="196">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="341" eb="343">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="344" eb="346">
+      <t>テンケン</t>
+    </rPh>
+    <rPh sb="347" eb="348">
+      <t>ス</t>
+    </rPh>
+    <rPh sb="359" eb="360">
+      <t>ハヤ</t>
+    </rPh>
+    <rPh sb="368" eb="369">
+      <t>ヒラ</t>
+    </rPh>
+    <rPh sb="406" eb="408">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="421" eb="425">
+      <t>ヒロシマダイガク</t>
+    </rPh>
+    <rPh sb="432" eb="434">
+      <t>セッシュ</t>
+    </rPh>
+    <rPh sb="442" eb="443">
+      <t>ノ</t>
+    </rPh>
+    <rPh sb="444" eb="445">
+      <t>ト</t>
+    </rPh>
+    <rPh sb="454" eb="456">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="459" eb="460">
+      <t>モ</t>
+    </rPh>
+    <rPh sb="461" eb="462">
+      <t>スベ</t>
+    </rPh>
+    <rPh sb="464" eb="467">
+      <t>コウセイイン</t>
+    </rPh>
+    <rPh sb="468" eb="469">
+      <t>タイ</t>
+    </rPh>
+    <rPh sb="481" eb="483">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="486" eb="491">
+      <t>タヨウソニンショウ</t>
+    </rPh>
+    <rPh sb="496" eb="498">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="499" eb="502">
+      <t>ギムヅ</t>
+    </rPh>
+    <rPh sb="514" eb="516">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="522" eb="526">
+      <t>ヒロシマダイガク</t>
+    </rPh>
+    <rPh sb="530" eb="532">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="533" eb="534">
+      <t>オコナ</t>
+    </rPh>
+    <rPh sb="538" eb="540">
+      <t>テジュン</t>
+    </rPh>
+    <rPh sb="541" eb="543">
+      <t>セツメイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>教材の下の方にある「IMCアカウントのMFA利用設定実習」をクリックして、説明に従ってIMCアカウントの多要素認証（MFA）設定を進めましょう。詳細は教材の各項目の資料を見てください。&lt;span class="check"&gt;check 8&lt;/span&gt;</t>
+    <rPh sb="0" eb="2">
+      <t>キョウザイ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>シタ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>ホウ</t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t>セツメイ</t>
+    </rPh>
+    <rPh sb="40" eb="41">
+      <t>シタガ</t>
+    </rPh>
+    <rPh sb="52" eb="57">
+      <t>タヨウソニンショウ</t>
+    </rPh>
+    <rPh sb="62" eb="64">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="65" eb="66">
+      <t>スス</t>
+    </rPh>
+    <rPh sb="72" eb="74">
+      <t>ショウサイ</t>
+    </rPh>
+    <rPh sb="78" eb="81">
+      <t>カクコウモク</t>
+    </rPh>
+    <rPh sb="82" eb="84">
+      <t>シリョウ</t>
+    </rPh>
+    <rPh sb="85" eb="86">
+      <t>ミ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">教材の下の方にある「広大IDのMFA利用設定実習」をクリックして、説明に従って広大IDの多要素認証（MFA）設定を進めましょう。詳細は教材の各項目の資料を見てください。&lt;span class="check"&gt;check 9&lt;/span&gt;
+</t>
+    <rPh sb="0" eb="2">
+      <t>キョウザイ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>シタ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>ホウ</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>セツメイ</t>
+    </rPh>
+    <rPh sb="36" eb="37">
+      <t>シタガ</t>
+    </rPh>
+    <rPh sb="39" eb="41">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="44" eb="49">
+      <t>タヨウソニンショウ</t>
+    </rPh>
+    <rPh sb="54" eb="56">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="57" eb="58">
+      <t>スス</t>
+    </rPh>
+    <rPh sb="64" eb="66">
+      <t>ショウサイ</t>
+    </rPh>
+    <rPh sb="70" eb="73">
+      <t>カクコウモク</t>
+    </rPh>
+    <rPh sb="74" eb="76">
+      <t>シリョウ</t>
+    </rPh>
+    <rPh sb="77" eb="78">
+      <t>ミ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Excelの新規作成の画面に戻ります。左上(①)にメディアセンタが登録している貴方の名前、左下(②)にライセンス認証のアイコンがないことを確認してください。これで、PowerPointやWordなどMicrosoft Officeの他のアプリケーションも使えるようになります。&lt;span class="check"&gt;check-11&lt;/span&gt;
+  </t>
+    <rPh sb="14" eb="15">
+      <t>モド</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>ヒダリウエ</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>トウロク</t>
+    </rPh>
+    <rPh sb="39" eb="41">
+      <t>アナタ</t>
+    </rPh>
+    <rPh sb="42" eb="44">
+      <t>ナマエ</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>ヒダリシタ</t>
+    </rPh>
+    <rPh sb="56" eb="58">
+      <t>ニンショウ</t>
+    </rPh>
+    <rPh sb="69" eb="71">
+      <t>カクニン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>メニューの「Microsoft Autoupdateを終了します」をクリックすると、終了できます。 ウィンドウを閉じるのでも構いません。
+&lt;span class="check"&gt;check 11&lt;/span&gt;</t>
+    <rPh sb="56" eb="57">
+      <t>ト</t>
+    </rPh>
+    <rPh sb="62" eb="63">
+      <t>カマ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">するとこのような画面になります。&lt;span class="check"&gt;check 12&lt;/span&gt;
+これを「Myもみじのトップページ」と呼ぶことにしましょう。
+履修登録をしたり、成績を確認することができます。
+また「掲示」では、授業や学部からの連絡が表示されます。
+このまま引き続いて、次の「Moodle」の使い方に進みましょう。
+  </t>
+    <rPh sb="70" eb="71">
+      <t>ヨ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">この画面になったら「続ける」で進めてください。不安がある場合は証明書を表示してください(2023年春の時点ではNII Open Domain CAが発行した証明書が表示されます)。
+これで接続の設定が完了しました。 接続が完了すると「接続済み」と表示されます。&lt;span class="check"&gt;check 13&lt;/span&gt;
+  </t>
+    <rPh sb="15" eb="16">
+      <t>スス</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>フアン</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="31" eb="34">
+      <t>ショウメイショ</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -6833,8 +6807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -6850,7 +6824,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6858,7 +6832,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6874,17 +6848,17 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -6892,7 +6866,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
@@ -6903,13 +6877,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -6917,13 +6891,13 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6931,13 +6905,13 @@
         <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -6945,13 +6919,13 @@
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -6959,13 +6933,13 @@
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>387</v>
+        <v>444</v>
       </c>
       <c r="C13" t="s">
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
     </row>
   </sheetData>
@@ -6993,10 +6967,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7004,7 +6978,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7020,17 +6994,17 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7038,33 +7012,33 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="D9" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="D10" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="171.6" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -7106,7 +7080,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7114,7 +7088,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7130,7 +7104,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -7138,7 +7112,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -7152,7 +7126,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -7162,13 +7136,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7176,24 +7150,24 @@
         <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -7201,13 +7175,13 @@
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="C13" t="s">
         <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -7215,40 +7189,40 @@
         <v>6</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="C14" t="s">
         <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="C16" t="s">
         <v>18</v>
       </c>
       <c r="D16" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="C17" t="s">
         <v>18</v>
       </c>
       <c r="D17" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -7256,13 +7230,13 @@
         <v>6</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="C18" t="s">
         <v>18</v>
       </c>
       <c r="D18" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7270,24 +7244,24 @@
         <v>6</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="C19" t="s">
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="92.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="C20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D20" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -7295,13 +7269,13 @@
         <v>6</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
       <c r="C21" t="s">
         <v>18</v>
       </c>
       <c r="D21" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7309,35 +7283,35 @@
         <v>6</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
       <c r="C22" t="s">
         <v>18</v>
       </c>
       <c r="D22" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
       <c r="C23" t="s">
         <v>18</v>
       </c>
       <c r="D23" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
       <c r="C24" t="s">
         <v>18</v>
       </c>
       <c r="D24" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7345,13 +7319,13 @@
         <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
       <c r="C25" t="s">
         <v>18</v>
       </c>
       <c r="D25" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -7359,18 +7333,18 @@
         <v>6</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
       <c r="C26" t="s">
         <v>18</v>
       </c>
       <c r="D26" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
     </row>
   </sheetData>
@@ -7384,8 +7358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD15"/>
+    <sheetView topLeftCell="A17" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="B17" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -7494,21 +7468,21 @@
         <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>439</v>
+        <v>431</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>441</v>
+        <v>433</v>
       </c>
       <c r="D12" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7516,13 +7490,13 @@
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
       <c r="C13" t="s">
         <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7713,8 +7687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B7" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -7785,18 +7759,18 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>60</v>
+        <v>437</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7804,21 +7778,21 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
         <v>62</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" t="s">
         <v>64</v>
-      </c>
-      <c r="D10" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -7826,13 +7800,13 @@
         <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -7840,24 +7814,24 @@
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" t="s">
         <v>70</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>71</v>
-      </c>
-      <c r="D13" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7865,24 +7839,24 @@
         <v>6</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C14" t="s">
         <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C15" t="s">
         <v>18</v>
       </c>
       <c r="D15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -7896,8 +7870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6E56ADE-9B9A-41F5-BFC9-8C8E6A100436}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView topLeftCell="A37" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -7913,7 +7887,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7921,7 +7895,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7937,54 +7911,54 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" t="s">
         <v>83</v>
-      </c>
-      <c r="D9" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" t="s">
         <v>85</v>
-      </c>
-      <c r="D10" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D11" t="s">
         <v>87</v>
-      </c>
-      <c r="D11" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D12" t="s">
         <v>89</v>
-      </c>
-      <c r="D12" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7992,29 +7966,29 @@
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
         <v>91</v>
-      </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" t="s">
         <v>93</v>
-      </c>
-      <c r="D14" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D15" t="s">
         <v>95</v>
-      </c>
-      <c r="D15" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -8022,18 +7996,18 @@
         <v>6</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D16" t="s">
         <v>97</v>
-      </c>
-      <c r="D16" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D17" t="s">
         <v>99</v>
-      </c>
-      <c r="D17" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -8041,34 +8015,34 @@
         <v>6</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D18" t="s">
         <v>101</v>
-      </c>
-      <c r="D18" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D19" t="s">
         <v>103</v>
-      </c>
-      <c r="D19" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D20" t="s">
         <v>105</v>
-      </c>
-      <c r="D20" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="83.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D21" t="s">
         <v>107</v>
-      </c>
-      <c r="D21" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -8076,10 +8050,10 @@
         <v>6</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D22" t="s">
         <v>109</v>
-      </c>
-      <c r="D22" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -8087,10 +8061,10 @@
         <v>6</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D23" t="s">
         <v>111</v>
-      </c>
-      <c r="D23" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -8098,18 +8072,18 @@
         <v>6</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D24" t="s">
         <v>113</v>
-      </c>
-      <c r="D24" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D25" t="s">
         <v>115</v>
-      </c>
-      <c r="D25" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -8117,10 +8091,10 @@
         <v>6</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D26" t="s">
         <v>117</v>
-      </c>
-      <c r="D26" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8128,10 +8102,10 @@
         <v>6</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D27" t="s">
         <v>119</v>
-      </c>
-      <c r="D27" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8139,10 +8113,10 @@
         <v>6</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D28" t="s">
         <v>121</v>
-      </c>
-      <c r="D28" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8150,10 +8124,10 @@
         <v>6</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D29" t="s">
         <v>123</v>
-      </c>
-      <c r="D29" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -8161,10 +8135,10 @@
         <v>6</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D30" t="s">
         <v>125</v>
-      </c>
-      <c r="D30" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -8172,10 +8146,10 @@
         <v>6</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D31" t="s">
         <v>127</v>
-      </c>
-      <c r="D31" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -8183,10 +8157,10 @@
         <v>6</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D32" t="s">
         <v>129</v>
-      </c>
-      <c r="D32" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8194,10 +8168,10 @@
         <v>6</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D33" t="s">
         <v>131</v>
-      </c>
-      <c r="D33" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8205,10 +8179,10 @@
         <v>6</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D34" t="s">
         <v>133</v>
-      </c>
-      <c r="D34" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -8216,130 +8190,130 @@
         <v>6</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D35" t="s">
         <v>135</v>
-      </c>
-      <c r="D35" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D36" t="s">
         <v>137</v>
-      </c>
-      <c r="D36" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D37" t="s">
         <v>139</v>
-      </c>
-      <c r="D37" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D38" t="s">
         <v>141</v>
-      </c>
-      <c r="D38" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D39" t="s">
         <v>143</v>
-      </c>
-      <c r="D39" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D40" t="s">
         <v>145</v>
-      </c>
-      <c r="D40" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D41" t="s">
         <v>147</v>
-      </c>
-      <c r="D41" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D42" t="s">
         <v>149</v>
-      </c>
-      <c r="D42" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D43" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D44" t="s">
         <v>152</v>
-      </c>
-      <c r="D44" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D45" t="s">
         <v>154</v>
-      </c>
-      <c r="D45" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D46" t="s">
         <v>156</v>
-      </c>
-      <c r="D46" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D47" t="s">
         <v>158</v>
-      </c>
-      <c r="D47" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B48" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D48" t="s">
         <v>160</v>
-      </c>
-      <c r="D48" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B49" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D49" t="s">
         <v>162</v>
-      </c>
-      <c r="D49" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B50" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D50" t="s">
         <v>164</v>
-      </c>
-      <c r="D50" t="s">
-        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -8370,7 +8344,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8378,7 +8352,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8394,7 +8368,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8402,7 +8376,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -8413,10 +8387,10 @@
     </row>
     <row r="7" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D7" t="s">
         <v>170</v>
-      </c>
-      <c r="D7" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -8424,13 +8398,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
         <v>172</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
-        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -8444,8 +8418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="B21" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -8461,7 +8435,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8469,7 +8443,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8485,7 +8459,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -8493,7 +8467,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -8504,7 +8478,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8512,13 +8486,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
         <v>179</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -8526,13 +8500,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -8540,40 +8514,40 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D12" t="s">
         <v>187</v>
-      </c>
-      <c r="D12" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D13" t="s">
         <v>189</v>
-      </c>
-      <c r="D13" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -8581,13 +8555,13 @@
         <v>6</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C14" t="s">
         <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -8595,13 +8569,13 @@
         <v>6</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C15" t="s">
         <v>18</v>
       </c>
       <c r="D15" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8609,7 +8583,7 @@
         <v>6</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C16" t="s">
         <v>18</v>
@@ -8620,7 +8594,7 @@
         <v>6</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C17" t="s">
         <v>18</v>
@@ -8631,10 +8605,10 @@
         <v>6</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D18" t="s">
         <v>197</v>
-      </c>
-      <c r="D18" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8642,98 +8616,98 @@
         <v>6</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D19" t="s">
         <v>199</v>
-      </c>
-      <c r="D19" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D20" t="s">
         <v>201</v>
-      </c>
-      <c r="D20" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D21" t="s">
         <v>203</v>
-      </c>
-      <c r="D21" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D22" t="s">
         <v>205</v>
-      </c>
-      <c r="D22" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D23" t="s">
         <v>207</v>
-      </c>
-      <c r="D23" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D24" t="s">
         <v>209</v>
-      </c>
-      <c r="D24" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D25" t="s">
         <v>211</v>
-      </c>
-      <c r="D25" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D26" t="s">
         <v>213</v>
-      </c>
-      <c r="D26" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D27" t="s">
         <v>215</v>
-      </c>
-      <c r="D27" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D28" t="s">
         <v>217</v>
-      </c>
-      <c r="D28" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D29" t="s">
         <v>219</v>
-      </c>
-      <c r="D29" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D30" t="s">
         <v>221</v>
-      </c>
-      <c r="D30" t="s">
-        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -8747,8 +8721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A15" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -8764,7 +8738,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8772,7 +8746,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8788,7 +8762,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -8796,7 +8770,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -8807,17 +8781,17 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -8825,29 +8799,29 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
         <v>230</v>
-      </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
         <v>232</v>
-      </c>
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8855,29 +8829,29 @@
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
         <v>235</v>
-      </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D14" t="s">
         <v>237</v>
-      </c>
-      <c r="D14" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D15" t="s">
         <v>239</v>
-      </c>
-      <c r="D15" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -8885,13 +8859,13 @@
         <v>6</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="198" x14ac:dyDescent="0.2">
@@ -8899,18 +8873,18 @@
         <v>6</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>242</v>
+        <v>438</v>
       </c>
       <c r="C17" t="s">
         <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8918,21 +8892,21 @@
         <v>6</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C19" t="s">
         <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D20" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8940,21 +8914,21 @@
         <v>6</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>249</v>
+        <v>439</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
       </c>
       <c r="D21" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="D22" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8962,13 +8936,13 @@
         <v>6</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>253</v>
+        <v>440</v>
       </c>
       <c r="C23" t="s">
         <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -9010,8 +8984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView topLeftCell="B40" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -9027,7 +9001,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -9035,7 +9009,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -9051,7 +9025,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -9059,7 +9033,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -9070,12 +9044,12 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="132" x14ac:dyDescent="0.2">
@@ -9083,13 +9057,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -9097,18 +9071,18 @@
         <v>6</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="D10" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D11" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9116,58 +9090,58 @@
         <v>6</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="3" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B14" s="3" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="D14" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D15" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B16" s="3" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D16" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D17" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D18" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9175,13 +9149,13 @@
         <v>6</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="C19" t="s">
         <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -9189,13 +9163,13 @@
         <v>6</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="C20" t="s">
         <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -9203,13 +9177,13 @@
         <v>6</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
       </c>
       <c r="D21" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -9217,13 +9191,13 @@
         <v>6</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
       </c>
       <c r="D22" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9231,13 +9205,13 @@
         <v>6</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C23" t="s">
         <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9245,34 +9219,34 @@
         <v>6</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C24" t="s">
         <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B25" s="3" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="D25" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B26" s="3" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D26" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" s="3" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -9280,13 +9254,13 @@
         <v>6</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C28" t="s">
         <v>6</v>
       </c>
       <c r="D28" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -9294,50 +9268,50 @@
         <v>6</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C29" t="s">
         <v>6</v>
       </c>
       <c r="D29" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B30" s="3" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="D30" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B31" s="3" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B32" s="3" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="D32" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="43.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="3" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D33" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B34" s="3" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="D34" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -9345,13 +9319,13 @@
         <v>6</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="C35" t="s">
         <v>6</v>
       </c>
       <c r="D35" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -9359,47 +9333,47 @@
         <v>6</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>312</v>
+        <v>441</v>
       </c>
       <c r="C36" t="s">
         <v>6</v>
       </c>
       <c r="D36" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B37" s="3" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="D37" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B38" s="3" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="3" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="D39" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B40" s="3" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="D40" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B41" s="3" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -9407,53 +9381,53 @@
         <v>6</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="C42" t="s">
         <v>6</v>
       </c>
       <c r="D42" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B43" s="3" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="D43" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B44" s="3" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="D44" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B45" s="3" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="D45" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B46" s="3" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="D46" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B47" s="3" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="D47" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9461,13 +9435,13 @@
         <v>6</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>334</v>
+        <v>442</v>
       </c>
       <c r="C48" t="s">
         <v>6</v>
       </c>
       <c r="D48" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -9481,8 +9455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A687F900-5547-4D89-8494-B67FCE27BE96}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -9498,7 +9472,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -9506,7 +9480,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -9522,7 +9496,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="184.8" x14ac:dyDescent="0.2">
@@ -9530,7 +9504,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -9541,7 +9515,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -9549,18 +9523,18 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -9568,91 +9542,91 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="D11" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="D12" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="D13" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D14" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="D15" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="C17" t="s">
         <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="C19" t="s">
         <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -9660,21 +9634,21 @@
         <v>6</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="C20" t="s">
         <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="D21" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -9682,18 +9656,18 @@
         <v>6</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>364</v>
+        <v>443</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
       </c>
       <c r="D22" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9701,7 +9675,7 @@
         <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="C25" t="s">
         <v>6</v>
@@ -9715,7 +9689,7 @@
         <v>6</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="C26" t="s">
         <v>18</v>
@@ -9726,13 +9700,13 @@
         <v>6</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="C27" t="s">
         <v>18</v>
       </c>
       <c r="D27" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="132" x14ac:dyDescent="0.2">
@@ -9740,13 +9714,13 @@
         <v>6</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="C28" t="s">
         <v>18</v>
       </c>
       <c r="D28" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
do not promote "3TB".
</commit_message>
<xml_diff>
--- a/macs+lan.xlsx
+++ b/macs+lan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20407"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20408"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C21F6A8-7C45-4F3D-A9E4-754F2CCA6BF6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E7A1B89-FBA9-4828-BF71-D089D49C07B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7764" tabRatio="772" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7764" tabRatio="772" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -4381,13 +4381,6 @@
     <t>win11ja-office365-from-outlook-to-onedrive.png</t>
   </si>
   <si>
-    <t xml:space="preserve">ここにはひとりあたり3TBまで、データを置いておくことができます。
-データのバックアップをとっておいたり、外出先でもデータを取り出したりできるようになるので、活用しましょう。
-OneDriveにもアプリがありますので、スマホでも活用できます。
-  </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>win11ja-onedrive-in-browser.png</t>
   </si>
   <si>
@@ -6322,6 +6315,11 @@
     <rPh sb="35" eb="37">
       <t>ヒョウジ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ここには私物MSアカウントよりは多くのデータを置いておくことができます。
+スマホ用のOneDriveアプリもありますので、外出先でもデータを取り出すことがあれば、活用してください。</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -6807,7 +6805,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
+    <sheetView topLeftCell="B9" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -6824,7 +6822,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6832,7 +6830,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6848,17 +6846,17 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -6866,7 +6864,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
@@ -6877,13 +6875,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -6891,13 +6889,13 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
         <v>374</v>
-      </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6905,13 +6903,13 @@
         <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
         <v>376</v>
-      </c>
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -6919,13 +6917,13 @@
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
         <v>378</v>
-      </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -6933,13 +6931,13 @@
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C13" t="s">
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -6967,10 +6965,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>380</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>381</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6978,7 +6976,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6994,17 +6992,17 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7012,12 +7010,12 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D9" t="s">
         <v>239</v>
@@ -7025,20 +7023,20 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="D10" t="s">
         <v>389</v>
-      </c>
-      <c r="D10" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="171.6" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -7080,7 +7078,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7088,7 +7086,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7104,7 +7102,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -7112,7 +7110,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -7126,7 +7124,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -7136,13 +7134,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7150,24 +7148,24 @@
         <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -7175,13 +7173,13 @@
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C13" t="s">
         <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -7189,40 +7187,40 @@
         <v>6</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C14" t="s">
         <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C16" t="s">
         <v>18</v>
       </c>
       <c r="D16" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C17" t="s">
         <v>18</v>
       </c>
       <c r="D17" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -7230,13 +7228,13 @@
         <v>6</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C18" t="s">
         <v>18</v>
       </c>
       <c r="D18" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7244,24 +7242,24 @@
         <v>6</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C19" t="s">
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="92.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C20" t="s">
         <v>70</v>
       </c>
       <c r="D20" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -7269,13 +7267,13 @@
         <v>6</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C21" t="s">
         <v>18</v>
       </c>
       <c r="D21" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -7283,35 +7281,35 @@
         <v>6</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C22" t="s">
         <v>18</v>
       </c>
       <c r="D22" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C23" t="s">
         <v>18</v>
       </c>
       <c r="D23" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C24" t="s">
         <v>18</v>
       </c>
       <c r="D24" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7319,13 +7317,13 @@
         <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C25" t="s">
         <v>18</v>
       </c>
       <c r="D25" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -7333,18 +7331,18 @@
         <v>6</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C26" t="s">
         <v>18</v>
       </c>
       <c r="D26" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
   </sheetData>
@@ -7468,21 +7466,21 @@
         <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="D12" t="s">
         <v>433</v>
-      </c>
-      <c r="D12" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7490,13 +7488,13 @@
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C13" t="s">
         <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7764,7 +7762,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
@@ -8873,7 +8871,7 @@
         <v>6</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C17" t="s">
         <v>6</v>
@@ -8914,7 +8912,7 @@
         <v>6</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
@@ -8936,7 +8934,7 @@
         <v>6</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C23" t="s">
         <v>6</v>
@@ -9333,7 +9331,7 @@
         <v>6</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C36" t="s">
         <v>6</v>
@@ -9435,7 +9433,7 @@
         <v>6</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C48" t="s">
         <v>6</v>
@@ -9455,8 +9453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A687F900-5547-4D89-8494-B67FCE27BE96}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -9602,31 +9600,31 @@
         <v>349</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
         <v>350</v>
-      </c>
-      <c r="C17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s">
         <v>353</v>
-      </c>
-      <c r="C19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -9634,7 +9632,7 @@
         <v>6</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C20" t="s">
         <v>6</v>
@@ -9645,10 +9643,10 @@
     </row>
     <row r="21" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="D21" t="s">
         <v>356</v>
-      </c>
-      <c r="D21" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -9656,18 +9654,18 @@
         <v>6</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
       </c>
       <c r="D22" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -9675,7 +9673,7 @@
         <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C25" t="s">
         <v>6</v>
@@ -9689,7 +9687,7 @@
         <v>6</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C26" t="s">
         <v>18</v>
@@ -9700,13 +9698,13 @@
         <v>6</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C27" t="s">
         <v>18</v>
       </c>
       <c r="D27" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="132" x14ac:dyDescent="0.2">
@@ -9714,13 +9712,13 @@
         <v>6</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C28" t="s">
         <v>18</v>
       </c>
       <c r="D28" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change jpeg to jpg
</commit_message>
<xml_diff>
--- a/macs+lan.xlsx
+++ b/macs+lan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaeltei/Projects/HUProjects/fresta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7BC7141-BCB8-8F41-8E7C-3B9579CEA995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E9911D4-92B3-1E4D-A5EF-8F512180EB61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6960" yWindow="2640" windowWidth="31440" windowHeight="16300" tabRatio="772" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6960" yWindow="2640" windowWidth="31440" windowHeight="16300" tabRatio="772" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -337,9 +337,6 @@
     <t>chartn</t>
   </si>
   <si>
-    <t>0_1.jpeg</t>
-  </si>
-  <si>
     <t>"「文字入力および音声入力の言語」という画面になります。
 「優先する言語」には、「日本語」、「入力ソース」には「日本語 - ローマ字入力」、「音声入力」には「日本語」を選択し、最後に「続ける」をクリックします。"</t>
     <rPh sb="1" eb="3">
@@ -393,9 +390,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>0_2.jpeg</t>
-  </si>
-  <si>
     <t>「アクセシビリティ」の設定画面になりますが、後から設定できるものなので、「今はしない」をクリックします。</t>
     <rPh sb="11" eb="13">
       <t>セッテイ</t>
@@ -415,9 +409,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>0_3.jpeg</t>
-  </si>
-  <si>
     <t>「データとプライバシー」の画面になります。ここでは何も設定することができませんが、通知を理解した上で、「続ける」をクリックします。</t>
     <rPh sb="13" eb="15">
       <t>ガメン</t>
@@ -441,9 +432,6 @@
       <t>ツヅ</t>
     </rPh>
     <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0_6.jpeg</t>
   </si>
   <si>
     <t xml:space="preserve">「移行アシスタント」の画面になりますが、「今はしない」をクリックします。
@@ -454,20 +442,11 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>0_7.jpeg</t>
-  </si>
-  <si>
     <t>Apple IDでサインインの画面です。Apple IDは後で取得できるので、左下にある「後で設定」をクリックします。</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>0_8.jpeg</t>
-  </si>
-  <si>
     <t>ポップアップが表示されるので「スキップ」をクリックします。</t>
-  </si>
-  <si>
-    <t>0_9.jpeg</t>
   </si>
   <si>
     <t>「エクスプレス設定」という画面になります。「設定をカスタマイズ」をクリックして調整しましょう。</t>
@@ -486,9 +465,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>0_10.jpeg</t>
-  </si>
-  <si>
     <t>ポップアップが表示されるので「同意する」をクリックします。</t>
     <rPh sb="1" eb="3">
       <t>イチ</t>
@@ -503,9 +479,6 @@
       <t>ガメンシャアナタチイキダイガクジタクリョコウサキリヨウツイセキキノウケイタイデンワフンシツツイセキキノウホゴムコウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0_11.jpeg</t>
   </si>
   <si>
     <t>このパソコンを使うときのユーザを設定します。
@@ -534,9 +507,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>0_12.jpeg</t>
-  </si>
-  <si>
     <t>位置情報サービスを有効にする画面です。このMacで位置情報サービスにチェックし、「続ける」をクリックします。</t>
     <rPh sb="1" eb="3">
       <t>カイセキ</t>
@@ -559,9 +529,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>0_13.jpeg</t>
-  </si>
-  <si>
     <t>「解析」という画面になります。これは、Mac上のアプリケーションが異常終了した場合のそのレポートをApple社に送って、製品の品質向上に役立てたいので協力してほしいというものです。プライバシー保護のために無効にしておきましょう。「続ける」をクリックします。</t>
     <rPh sb="1" eb="4">
       <t>ジカンタイ</t>
@@ -629,9 +596,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>0_14_1.jpeg</t>
-  </si>
-  <si>
     <t>「スクリーンタイム」という画面になります。これはMacをどのような時間帯に使っているかといった情報を調べたり、家族が使う場合の機能制限をすることができます。後からでも設定できるので、「あとで設定」で進めましょう。</t>
     <rPh sb="13" eb="15">
       <t>ガメン</t>
@@ -678,9 +642,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>0_15.jpeg</t>
-  </si>
-  <si>
     <t>「Siri」という音声でMacを操作する機能を設定できますが、後からでも設定できるので、ここでは有効にしないまま「続ける」をクリックします。</t>
     <rPh sb="9" eb="11">
       <t>オンセイ</t>
@@ -709,9 +670,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>0_16.jpeg</t>
-  </si>
-  <si>
     <t>機種によっては指紋センサーが付属しているため、指紋認証の設定をすることもできます。これも後から設定できるので「Touch IDをあとで設定」で進めましょう。</t>
     <rPh sb="0" eb="2">
       <t>キシュ</t>
@@ -746,9 +704,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>0_17.jpeg</t>
-  </si>
-  <si>
     <t>TouchIDをすぐ設定させようとしてきますが、「続ける」で振り切ってください。</t>
     <rPh sb="10" eb="12">
       <t>セッテイ</t>
@@ -765,9 +720,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>0_18.jpeg</t>
-  </si>
-  <si>
     <t>「外観モードを選択」という画面になります。何もしなければ「ライト」の配色になります。説明にも書いてあるように後で設定可能なので、「続ける」で進めましょう。</t>
     <rPh sb="1" eb="3">
       <t>ガイカン</t>
@@ -808,9 +760,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>0_19.jpeg</t>
-  </si>
-  <si>
     <t xml:space="preserve">ようやくデスクトップの画面が出ました！ これでこの章の作業は終了です。以降の手順はネットワークにつないで行っても大丈夫です。  </t>
     <rPh sb="25" eb="26">
       <t>ショウ</t>
@@ -831,9 +780,6 @@
       <t>ダイジョウブ</t>
     </rPh>
     <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0_20.jpeg</t>
   </si>
   <si>
     <t xml:space="preserve">自分のパソコンの基本的なスペックを確認しておきましょう。CPUの型式、OSのビット数、記憶容量など。 </t>
@@ -5911,19 +5857,10 @@
     <t>次に「Wi-Fiネットワークを選択」の画面になりますが、これはあとでやりますので、「その他のネットワークオプション」をクリックします。</t>
   </si>
   <si>
-    <t>0_4_1.jpeg</t>
-  </si>
-  <si>
     <t>次に「インターネットの接続方法」の画面になりますが、いまは「コンピュータをインターネットに接続しない」を選択してください。 「続ける」をクリックします。</t>
   </si>
   <si>
-    <t>0_4_2.jpeg</t>
-  </si>
-  <si>
     <t>本当にネットワーク接続しなくて良いのかしつこくもう一回聞かれますが、「続ける」をクリックして振り切ってください。</t>
-  </si>
-  <si>
-    <t>0_4_3.jpeg</t>
   </si>
   <si>
     <t>2024年3月で最新のmacOS Sonoma (14.x)ではこのようなパネルが開きます。①チップ、②メモリ、③macOSのバージョン番号をメモしておきましょう。あるいはこのパネルの写真を撮っておきましょう。続いて、④詳細情報に進みます。
@@ -6301,6 +6238,69 @@
   </si>
   <si>
     <t>FRESTA-TEXT-2025 macOS appendix A</t>
+  </si>
+  <si>
+    <t>0_1.jpg</t>
+  </si>
+  <si>
+    <t>0_2.jpg</t>
+  </si>
+  <si>
+    <t>0_3.jpg</t>
+  </si>
+  <si>
+    <t>0_4_1.jpg</t>
+  </si>
+  <si>
+    <t>0_4_2.jpg</t>
+  </si>
+  <si>
+    <t>0_4_3.jpg</t>
+  </si>
+  <si>
+    <t>0_6.jpg</t>
+  </si>
+  <si>
+    <t>0_7.jpg</t>
+  </si>
+  <si>
+    <t>0_8.jpg</t>
+  </si>
+  <si>
+    <t>0_9.jpg</t>
+  </si>
+  <si>
+    <t>0_10.jpg</t>
+  </si>
+  <si>
+    <t>0_11.jpg</t>
+  </si>
+  <si>
+    <t>0_12.jpg</t>
+  </si>
+  <si>
+    <t>0_13.jpg</t>
+  </si>
+  <si>
+    <t>0_14_1.jpg</t>
+  </si>
+  <si>
+    <t>0_15.jpg</t>
+  </si>
+  <si>
+    <t>0_16.jpg</t>
+  </si>
+  <si>
+    <t>0_17.jpg</t>
+  </si>
+  <si>
+    <t>0_18.jpg</t>
+  </si>
+  <si>
+    <t>0_19.jpg</t>
+  </si>
+  <si>
+    <t>0_20.jpg</t>
   </si>
 </sst>
 </file>
@@ -6693,7 +6693,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>431</v>
+        <v>410</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -6709,7 +6709,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>433</v>
+        <v>412</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -6717,7 +6717,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>432</v>
+        <v>411</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -6768,7 +6768,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>354</v>
+        <v>336</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -6776,7 +6776,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>355</v>
+        <v>337</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -6792,17 +6792,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>442</v>
+        <v>421</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>356</v>
+        <v>338</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>357</v>
+        <v>339</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -6810,7 +6810,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>358</v>
+        <v>340</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -6821,13 +6821,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>359</v>
+        <v>341</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>360</v>
+        <v>342</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -6835,13 +6835,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>361</v>
+        <v>343</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>362</v>
+        <v>344</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -6849,13 +6849,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>363</v>
+        <v>345</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>364</v>
+        <v>346</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="96" x14ac:dyDescent="0.2">
@@ -6863,13 +6863,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>365</v>
+        <v>347</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>366</v>
+        <v>348</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="80" x14ac:dyDescent="0.2">
@@ -6877,13 +6877,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>429</v>
+        <v>408</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>367</v>
+        <v>349</v>
       </c>
     </row>
   </sheetData>
@@ -6911,10 +6911,10 @@
   <sheetData>
     <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>368</v>
+        <v>350</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>369</v>
+        <v>351</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -6922,7 +6922,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>370</v>
+        <v>352</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -6938,17 +6938,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>443</v>
+        <v>422</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>371</v>
+        <v>353</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>372</v>
+        <v>354</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -6956,33 +6956,33 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>373</v>
+        <v>355</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>374</v>
+        <v>356</v>
       </c>
       <c r="D9" t="s">
-        <v>230</v>
+        <v>212</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>375</v>
+        <v>357</v>
       </c>
       <c r="D10" t="s">
-        <v>376</v>
+        <v>358</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>377</v>
+        <v>359</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="208" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>378</v>
+        <v>360</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -7007,7 +7007,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A14737B-27B4-430E-A2C9-8E4453FC8EAA}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -7024,7 +7024,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>379</v>
+        <v>361</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -7032,7 +7032,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>379</v>
+        <v>361</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -7048,7 +7048,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>444</v>
+        <v>423</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="96" x14ac:dyDescent="0.2">
@@ -7056,7 +7056,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>380</v>
+        <v>362</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7070,7 +7070,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>381</v>
+        <v>363</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -7080,13 +7080,13 @@
     </row>
     <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>382</v>
+        <v>364</v>
       </c>
       <c r="C10" t="s">
         <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>383</v>
+        <v>365</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -7094,24 +7094,24 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>384</v>
+        <v>366</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>385</v>
+        <v>367</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>386</v>
+        <v>368</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>387</v>
+        <v>369</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -7119,13 +7119,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>388</v>
+        <v>370</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>389</v>
+        <v>371</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -7133,40 +7133,40 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>390</v>
+        <v>372</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>391</v>
+        <v>373</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>392</v>
+        <v>374</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>393</v>
+        <v>375</v>
       </c>
       <c r="C16" t="s">
         <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>394</v>
+        <v>376</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>395</v>
+        <v>377</v>
       </c>
       <c r="C17" t="s">
         <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>396</v>
+        <v>378</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -7174,13 +7174,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>397</v>
+        <v>379</v>
       </c>
       <c r="C18" t="s">
         <v>14</v>
       </c>
       <c r="D18" t="s">
-        <v>398</v>
+        <v>380</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -7188,24 +7188,24 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>399</v>
+        <v>381</v>
       </c>
       <c r="C19" t="s">
         <v>14</v>
       </c>
       <c r="D19" t="s">
-        <v>400</v>
+        <v>382</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="92.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>401</v>
+        <v>383</v>
       </c>
       <c r="C20" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="D20" t="s">
-        <v>402</v>
+        <v>384</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="96" x14ac:dyDescent="0.2">
@@ -7213,13 +7213,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>403</v>
+        <v>385</v>
       </c>
       <c r="C21" t="s">
         <v>14</v>
       </c>
       <c r="D21" t="s">
-        <v>404</v>
+        <v>386</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -7227,35 +7227,35 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>405</v>
+        <v>387</v>
       </c>
       <c r="C22" t="s">
         <v>14</v>
       </c>
       <c r="D22" t="s">
-        <v>406</v>
+        <v>388</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>407</v>
+        <v>389</v>
       </c>
       <c r="C23" t="s">
         <v>14</v>
       </c>
       <c r="D23" t="s">
-        <v>408</v>
+        <v>390</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>409</v>
+        <v>391</v>
       </c>
       <c r="C24" t="s">
         <v>14</v>
       </c>
       <c r="D24" t="s">
-        <v>410</v>
+        <v>392</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -7263,13 +7263,13 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>411</v>
+        <v>393</v>
       </c>
       <c r="C25" t="s">
         <v>14</v>
       </c>
       <c r="D25" t="s">
-        <v>412</v>
+        <v>394</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="80" x14ac:dyDescent="0.2">
@@ -7277,18 +7277,18 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>413</v>
+        <v>395</v>
       </c>
       <c r="C26" t="s">
         <v>14</v>
       </c>
       <c r="D26" t="s">
-        <v>414</v>
+        <v>396</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>415</v>
+        <v>397</v>
       </c>
     </row>
   </sheetData>
@@ -7302,8 +7302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7343,7 +7343,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>434</v>
+        <v>413</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="160" x14ac:dyDescent="0.2">
@@ -7379,7 +7379,7 @@
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>424</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -7387,24 +7387,24 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>425</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
         <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>19</v>
+        <v>426</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -7412,21 +7412,21 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>416</v>
+        <v>398</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>417</v>
+        <v>427</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>418</v>
+        <v>399</v>
       </c>
       <c r="D12" t="s">
-        <v>419</v>
+        <v>428</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -7434,24 +7434,24 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>420</v>
+        <v>400</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>421</v>
+        <v>429</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>21</v>
+        <v>430</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -7459,13 +7459,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s">
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>23</v>
+        <v>431</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -7473,13 +7473,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
         <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>25</v>
+        <v>432</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -7487,123 +7487,123 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
         <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>27</v>
+        <v>433</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
         <v>14</v>
       </c>
       <c r="D18" t="s">
-        <v>29</v>
+        <v>434</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C19" t="s">
         <v>14</v>
       </c>
       <c r="D19" t="s">
-        <v>31</v>
+        <v>435</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="176" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s">
         <v>14</v>
       </c>
       <c r="D20" t="s">
-        <v>33</v>
+        <v>436</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C21" t="s">
         <v>14</v>
       </c>
       <c r="D21" t="s">
-        <v>35</v>
+        <v>437</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C22" t="s">
         <v>14</v>
       </c>
       <c r="D22" t="s">
-        <v>37</v>
+        <v>438</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C23" t="s">
         <v>14</v>
       </c>
       <c r="D23" t="s">
-        <v>39</v>
+        <v>439</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="C24" t="s">
         <v>14</v>
       </c>
       <c r="D24" t="s">
-        <v>41</v>
+        <v>440</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="C25" t="s">
         <v>14</v>
       </c>
       <c r="D25" t="s">
-        <v>43</v>
+        <v>441</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="C26" t="s">
         <v>14</v>
       </c>
       <c r="D26" t="s">
-        <v>45</v>
+        <v>442</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="C27" t="s">
         <v>14</v>
       </c>
       <c r="D27" t="s">
-        <v>47</v>
+        <v>443</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -7611,13 +7611,13 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="C28" t="s">
         <v>14</v>
       </c>
       <c r="D28" t="s">
-        <v>49</v>
+        <v>444</v>
       </c>
     </row>
   </sheetData>
@@ -7648,7 +7648,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -7656,7 +7656,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -7672,7 +7672,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>435</v>
+        <v>414</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="144" x14ac:dyDescent="0.2">
@@ -7680,7 +7680,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7694,13 +7694,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="80" x14ac:dyDescent="0.2">
@@ -7708,13 +7708,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>422</v>
+        <v>401</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -7722,21 +7722,21 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="D10" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="160" x14ac:dyDescent="0.2">
@@ -7744,13 +7744,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -7758,24 +7758,24 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="D13" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="80" x14ac:dyDescent="0.2">
@@ -7783,24 +7783,24 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="112" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="C15" t="s">
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -7831,7 +7831,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -7839,7 +7839,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -7855,54 +7855,54 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>436</v>
+        <v>415</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="144" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="D9" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="D10" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="176" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="D11" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="D12" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -7910,29 +7910,29 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="D14" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="D15" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -7940,18 +7940,18 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="D16" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="D17" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -7959,34 +7959,34 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="D18" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="D19" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="D20" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="83" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="D21" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -7994,10 +7994,10 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="D22" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -8005,10 +8005,10 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="D23" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -8016,18 +8016,18 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="D24" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="D25" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -8035,10 +8035,10 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="D26" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -8046,10 +8046,10 @@
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="D27" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -8057,10 +8057,10 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="D28" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -8068,10 +8068,10 @@
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="D29" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -8079,10 +8079,10 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="D30" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -8090,10 +8090,10 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="D31" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -8101,10 +8101,10 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="D32" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -8112,10 +8112,10 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="D33" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -8123,10 +8123,10 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="D34" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -8134,130 +8134,130 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="D35" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="D36" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="D37" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="D38" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="D39" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="D40" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="D41" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="D42" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="D43" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="D44" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="D45" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="D46" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="D47" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B48" s="1" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="D48" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
     </row>
     <row r="49" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B49" s="1" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="D49" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
     </row>
     <row r="50" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B50" s="1" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
       <c r="D50" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -8288,7 +8288,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -8296,7 +8296,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -8312,7 +8312,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>437</v>
+        <v>416</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -8320,7 +8320,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8331,10 +8331,10 @@
     </row>
     <row r="7" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
       <c r="D7" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="80" x14ac:dyDescent="0.2">
@@ -8342,13 +8342,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -8379,7 +8379,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -8387,7 +8387,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -8403,7 +8403,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>438</v>
+        <v>417</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="112" x14ac:dyDescent="0.2">
@@ -8411,7 +8411,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8422,7 +8422,7 @@
     </row>
     <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -8430,13 +8430,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -8444,13 +8444,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>172</v>
+        <v>154</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>173</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -8458,40 +8458,40 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="C10" t="s">
         <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
       <c r="D12" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>180</v>
+        <v>162</v>
       </c>
       <c r="D13" t="s">
-        <v>181</v>
+        <v>163</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -8499,13 +8499,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>182</v>
+        <v>164</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>183</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -8513,13 +8513,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>184</v>
+        <v>166</v>
       </c>
       <c r="C15" t="s">
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>185</v>
+        <v>167</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -8527,7 +8527,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>186</v>
+        <v>168</v>
       </c>
       <c r="C16" t="s">
         <v>14</v>
@@ -8538,7 +8538,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>187</v>
+        <v>169</v>
       </c>
       <c r="C17" t="s">
         <v>14</v>
@@ -8549,10 +8549,10 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>188</v>
+        <v>170</v>
       </c>
       <c r="D18" t="s">
-        <v>189</v>
+        <v>171</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -8560,98 +8560,98 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>190</v>
+        <v>172</v>
       </c>
       <c r="D19" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>192</v>
+        <v>174</v>
       </c>
       <c r="D20" t="s">
-        <v>193</v>
+        <v>175</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>194</v>
+        <v>176</v>
       </c>
       <c r="D21" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="96" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
       <c r="D22" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="D23" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>200</v>
+        <v>182</v>
       </c>
       <c r="D24" t="s">
-        <v>201</v>
+        <v>183</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="D25" t="s">
-        <v>203</v>
+        <v>185</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>204</v>
+        <v>186</v>
       </c>
       <c r="D26" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="96" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>206</v>
+        <v>188</v>
       </c>
       <c r="D27" t="s">
-        <v>207</v>
+        <v>189</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>208</v>
+        <v>190</v>
       </c>
       <c r="D28" t="s">
-        <v>209</v>
+        <v>191</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
       <c r="D29" t="s">
-        <v>211</v>
+        <v>193</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="D30" t="s">
-        <v>213</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -8682,7 +8682,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -8690,7 +8690,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>215</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -8706,7 +8706,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>439</v>
+        <v>418</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="112" x14ac:dyDescent="0.2">
@@ -8714,7 +8714,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8725,17 +8725,17 @@
     </row>
     <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>217</v>
+        <v>199</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="128" x14ac:dyDescent="0.2">
@@ -8743,29 +8743,29 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>224</v>
+        <v>206</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -8773,29 +8773,29 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>226</v>
+        <v>208</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>227</v>
+        <v>209</v>
       </c>
       <c r="D14" t="s">
-        <v>228</v>
+        <v>210</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>229</v>
+        <v>211</v>
       </c>
       <c r="D15" t="s">
-        <v>230</v>
+        <v>212</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="112" x14ac:dyDescent="0.2">
@@ -8803,13 +8803,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>231</v>
+        <v>213</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="240" x14ac:dyDescent="0.2">
@@ -8817,18 +8817,18 @@
         <v>4</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>423</v>
+        <v>402</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>232</v>
+        <v>214</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -8836,21 +8836,21 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>234</v>
+        <v>216</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>235</v>
+        <v>217</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>236</v>
+        <v>218</v>
       </c>
       <c r="D20" t="s">
-        <v>237</v>
+        <v>219</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -8858,21 +8858,21 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>424</v>
+        <v>403</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>238</v>
+        <v>220</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>239</v>
+        <v>221</v>
       </c>
       <c r="D22" t="s">
-        <v>240</v>
+        <v>222</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -8880,13 +8880,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>425</v>
+        <v>404</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>241</v>
+        <v>223</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -8945,7 +8945,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>242</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -8953,7 +8953,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>243</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -8969,7 +8969,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>440</v>
+        <v>419</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="112" x14ac:dyDescent="0.2">
@@ -8977,7 +8977,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>244</v>
+        <v>226</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8988,12 +8988,12 @@
     </row>
     <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>245</v>
+        <v>227</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
-        <v>246</v>
+        <v>228</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="176" x14ac:dyDescent="0.2">
@@ -9001,13 +9001,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>247</v>
+        <v>229</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>248</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -9015,18 +9015,18 @@
         <v>4</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>249</v>
+        <v>231</v>
       </c>
       <c r="D10" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
       <c r="D11" t="s">
-        <v>252</v>
+        <v>234</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -9034,58 +9034,58 @@
         <v>4</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>253</v>
+        <v>235</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>254</v>
+        <v>236</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B13" s="3" t="s">
-        <v>255</v>
+        <v>237</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B14" s="3" t="s">
-        <v>256</v>
+        <v>238</v>
       </c>
       <c r="D14" t="s">
-        <v>257</v>
+        <v>239</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
-        <v>258</v>
+        <v>240</v>
       </c>
       <c r="D15" t="s">
-        <v>259</v>
+        <v>241</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B16" s="3" t="s">
-        <v>260</v>
+        <v>242</v>
       </c>
       <c r="D16" t="s">
-        <v>261</v>
+        <v>243</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
-        <v>262</v>
+        <v>244</v>
       </c>
       <c r="D17" t="s">
-        <v>263</v>
+        <v>245</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
-        <v>264</v>
+        <v>246</v>
       </c>
       <c r="D18" t="s">
-        <v>265</v>
+        <v>247</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -9093,13 +9093,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>266</v>
+        <v>248</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>267</v>
+        <v>249</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="96" x14ac:dyDescent="0.2">
@@ -9107,13 +9107,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>268</v>
+        <v>250</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>269</v>
+        <v>251</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -9121,13 +9121,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>270</v>
+        <v>252</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>271</v>
+        <v>253</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -9135,13 +9135,13 @@
         <v>4</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>272</v>
+        <v>254</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>273</v>
+        <v>255</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -9149,13 +9149,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>274</v>
+        <v>256</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>275</v>
+        <v>257</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -9163,34 +9163,34 @@
         <v>4</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>276</v>
+        <v>258</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>277</v>
+        <v>259</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B25" s="3" t="s">
-        <v>278</v>
+        <v>260</v>
       </c>
       <c r="D25" t="s">
-        <v>279</v>
+        <v>261</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B26" s="3" t="s">
-        <v>280</v>
+        <v>262</v>
       </c>
       <c r="D26" t="s">
-        <v>281</v>
+        <v>263</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B27" s="3" t="s">
-        <v>282</v>
+        <v>264</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -9198,13 +9198,13 @@
         <v>4</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>283</v>
+        <v>265</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -9212,50 +9212,50 @@
         <v>4</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>285</v>
+        <v>267</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>286</v>
+        <v>268</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B30" s="3" t="s">
-        <v>287</v>
+        <v>269</v>
       </c>
       <c r="D30" t="s">
-        <v>288</v>
+        <v>270</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="96" x14ac:dyDescent="0.2">
       <c r="B31" s="3" t="s">
-        <v>289</v>
+        <v>271</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B32" s="3" t="s">
-        <v>290</v>
+        <v>272</v>
       </c>
       <c r="D32" t="s">
-        <v>291</v>
+        <v>273</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="3" t="s">
-        <v>292</v>
+        <v>274</v>
       </c>
       <c r="D33" t="s">
-        <v>293</v>
+        <v>275</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B34" s="3" t="s">
-        <v>294</v>
+        <v>276</v>
       </c>
       <c r="D34" t="s">
-        <v>295</v>
+        <v>277</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -9263,13 +9263,13 @@
         <v>4</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>296</v>
+        <v>278</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>297</v>
+        <v>279</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -9277,47 +9277,47 @@
         <v>4</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>426</v>
+        <v>405</v>
       </c>
       <c r="C36" t="s">
         <v>4</v>
       </c>
       <c r="D36" t="s">
-        <v>298</v>
+        <v>280</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B37" s="3" t="s">
-        <v>299</v>
+        <v>281</v>
       </c>
       <c r="D37" t="s">
-        <v>300</v>
+        <v>282</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B38" s="3" t="s">
-        <v>301</v>
+        <v>283</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="3" t="s">
-        <v>302</v>
+        <v>284</v>
       </c>
       <c r="D39" t="s">
-        <v>303</v>
+        <v>285</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B40" s="3" t="s">
-        <v>304</v>
+        <v>286</v>
       </c>
       <c r="D40" t="s">
-        <v>305</v>
+        <v>287</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B41" s="3" t="s">
-        <v>306</v>
+        <v>288</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -9325,53 +9325,53 @@
         <v>4</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>307</v>
+        <v>289</v>
       </c>
       <c r="C42" t="s">
         <v>4</v>
       </c>
       <c r="D42" t="s">
-        <v>308</v>
+        <v>290</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B43" s="3" t="s">
-        <v>309</v>
+        <v>291</v>
       </c>
       <c r="D43" t="s">
-        <v>310</v>
+        <v>292</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B44" s="3" t="s">
-        <v>311</v>
+        <v>293</v>
       </c>
       <c r="D44" t="s">
-        <v>312</v>
+        <v>294</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B45" s="3" t="s">
-        <v>313</v>
+        <v>295</v>
       </c>
       <c r="D45" t="s">
-        <v>314</v>
+        <v>296</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B46" s="3" t="s">
-        <v>315</v>
+        <v>297</v>
       </c>
       <c r="D46" t="s">
-        <v>316</v>
+        <v>298</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B47" s="3" t="s">
-        <v>317</v>
+        <v>299</v>
       </c>
       <c r="D47" t="s">
-        <v>318</v>
+        <v>300</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -9379,13 +9379,13 @@
         <v>4</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>427</v>
+        <v>406</v>
       </c>
       <c r="C48" t="s">
         <v>4</v>
       </c>
       <c r="D48" t="s">
-        <v>319</v>
+        <v>301</v>
       </c>
     </row>
   </sheetData>
@@ -9416,7 +9416,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>320</v>
+        <v>302</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -9424,7 +9424,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>321</v>
+        <v>303</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -9440,7 +9440,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>441</v>
+        <v>420</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="224" x14ac:dyDescent="0.2">
@@ -9448,7 +9448,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>322</v>
+        <v>304</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -9459,7 +9459,7 @@
     </row>
     <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -9467,18 +9467,18 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>323</v>
+        <v>305</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>324</v>
+        <v>306</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -9486,91 +9486,91 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>325</v>
+        <v>307</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>326</v>
+        <v>308</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>327</v>
+        <v>309</v>
       </c>
       <c r="D11" t="s">
-        <v>328</v>
+        <v>310</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>329</v>
+        <v>311</v>
       </c>
       <c r="D12" t="s">
-        <v>330</v>
+        <v>312</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>331</v>
+        <v>313</v>
       </c>
       <c r="D13" t="s">
-        <v>332</v>
+        <v>314</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
-        <v>333</v>
+        <v>315</v>
       </c>
       <c r="D14" t="s">
-        <v>334</v>
+        <v>316</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>335</v>
+        <v>317</v>
       </c>
       <c r="D15" t="s">
-        <v>336</v>
+        <v>318</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>337</v>
+        <v>319</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>338</v>
+        <v>320</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>430</v>
+        <v>409</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>339</v>
+        <v>321</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>340</v>
+        <v>322</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>341</v>
+        <v>323</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>342</v>
+        <v>324</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="96" x14ac:dyDescent="0.2">
@@ -9578,21 +9578,21 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>343</v>
+        <v>325</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>344</v>
+        <v>326</v>
       </c>
       <c r="D21" t="s">
-        <v>345</v>
+        <v>327</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="128" x14ac:dyDescent="0.2">
@@ -9600,18 +9600,18 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>428</v>
+        <v>407</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>346</v>
+        <v>328</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>347</v>
+        <v>329</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -9619,7 +9619,7 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>348</v>
+        <v>330</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
@@ -9633,7 +9633,7 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>349</v>
+        <v>331</v>
       </c>
       <c r="C26" t="s">
         <v>14</v>
@@ -9644,13 +9644,13 @@
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>350</v>
+        <v>332</v>
       </c>
       <c r="C27" t="s">
         <v>14</v>
       </c>
       <c r="D27" t="s">
-        <v>351</v>
+        <v>333</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="160" x14ac:dyDescent="0.2">
@@ -9658,13 +9658,13 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>352</v>
+        <v>334</v>
       </c>
       <c r="C28" t="s">
         <v>14</v>
       </c>
       <c r="D28" t="s">
-        <v>353</v>
+        <v>335</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Unify Mac MFA with Win11
</commit_message>
<xml_diff>
--- a/macs+lan.xlsx
+++ b/macs+lan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaeltei/Projects/HUProjects/fresta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E9911D4-92B3-1E4D-A5EF-8F512180EB61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED85CC33-EF44-9343-BE40-64120043CA2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6960" yWindow="2640" windowWidth="31440" windowHeight="16300" tabRatio="772" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6960" yWindow="2640" windowWidth="31440" windowHeight="16300" tabRatio="772" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="443">
   <si>
     <t>header1</t>
   </si>
@@ -2993,114 +2993,6 @@
   </si>
   <si>
     <t>moodle-dashboard-ja.svg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;h2&gt;&lt;a name="mfa"&gt;&lt;/a&gt;多要素認証(MFA)の設定&lt;/h2&gt; </t>
-    <rPh sb="22" eb="27">
-      <t>タヨウソニンショウ</t>
-    </rPh>
-    <rPh sb="33" eb="35">
-      <t>セッテイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>広大moodleの「コースツリー」の中の「MFA設定ガイド」をクリックすると、コースのトップページが表示されます。まず「コメントシート」欄に表示される説明を読んでください。</t>
-    <rPh sb="0" eb="2">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="18" eb="19">
-      <t>ナカ</t>
-    </rPh>
-    <rPh sb="24" eb="26">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="50" eb="52">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="68" eb="69">
-      <t>ラン</t>
-    </rPh>
-    <rPh sb="70" eb="72">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="75" eb="77">
-      <t>セツメイ</t>
-    </rPh>
-    <rPh sb="78" eb="79">
-      <t>ヨ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>moodle-mfa-top.svg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>さらに下の方にある「IMCアカウントのMFA設定」をクリックしてIMCアカウントのMFA設定教材を表示しましょう。</t>
-    <rPh sb="3" eb="4">
-      <t>シタ</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>ホウ</t>
-    </rPh>
-    <rPh sb="22" eb="24">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="44" eb="46">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="46" eb="48">
-      <t>キョウザイ</t>
-    </rPh>
-    <rPh sb="49" eb="51">
-      <t>ヒョウジ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>moodle-mfa-imc.svg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>moodle-mfaimc-below.svg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>さらに下の方にある「広大IDのMFA設定」をクリックして広大IDのMFA設定教材を表示しましょう。</t>
-    <rPh sb="3" eb="4">
-      <t>シタ</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>ホウ</t>
-    </rPh>
-    <rPh sb="10" eb="12">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="18" eb="20">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="28" eb="30">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="36" eb="38">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="38" eb="40">
-      <t>キョウザイ</t>
-    </rPh>
-    <rPh sb="41" eb="43">
-      <t>ヒョウジ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>moodle-mfa-hirodai.svg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>moodle-mfahirodai-below.svg</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -6033,90 +5925,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>教材の下の方にある「IMCアカウントのMFA利用設定実習」をクリックして、説明に従ってIMCアカウントの多要素認証（MFA）設定を進めましょう。詳細は教材の各項目の資料を見てください。&lt;span class="check"&gt;check 8&lt;/span&gt;</t>
-    <rPh sb="0" eb="2">
-      <t>キョウザイ</t>
-    </rPh>
-    <rPh sb="3" eb="4">
-      <t>シタ</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>ホウ</t>
-    </rPh>
-    <rPh sb="37" eb="39">
-      <t>セツメイ</t>
-    </rPh>
-    <rPh sb="40" eb="41">
-      <t>シタガ</t>
-    </rPh>
-    <rPh sb="52" eb="57">
-      <t>タヨウソニンショウ</t>
-    </rPh>
-    <rPh sb="62" eb="64">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="65" eb="66">
-      <t>スス</t>
-    </rPh>
-    <rPh sb="72" eb="74">
-      <t>ショウサイ</t>
-    </rPh>
-    <rPh sb="78" eb="81">
-      <t>カクコウモク</t>
-    </rPh>
-    <rPh sb="82" eb="84">
-      <t>シリョウ</t>
-    </rPh>
-    <rPh sb="85" eb="86">
-      <t>ミ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">教材の下の方にある「広大IDのMFA利用設定実習」をクリックして、説明に従って広大IDの多要素認証（MFA）設定を進めましょう。詳細は教材の各項目の資料を見てください。&lt;span class="check"&gt;check 9&lt;/span&gt;
-</t>
-    <rPh sb="0" eb="2">
-      <t>キョウザイ</t>
-    </rPh>
-    <rPh sb="3" eb="4">
-      <t>シタ</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>ホウ</t>
-    </rPh>
-    <rPh sb="33" eb="35">
-      <t>セツメイ</t>
-    </rPh>
-    <rPh sb="36" eb="37">
-      <t>シタガ</t>
-    </rPh>
-    <rPh sb="39" eb="41">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="44" eb="49">
-      <t>タヨウソニンショウ</t>
-    </rPh>
-    <rPh sb="54" eb="56">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="57" eb="58">
-      <t>スス</t>
-    </rPh>
-    <rPh sb="64" eb="66">
-      <t>ショウサイ</t>
-    </rPh>
-    <rPh sb="70" eb="73">
-      <t>カクコウモク</t>
-    </rPh>
-    <rPh sb="74" eb="76">
-      <t>シリョウ</t>
-    </rPh>
-    <rPh sb="77" eb="78">
-      <t>ミ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve">Excelの新規作成の画面に戻ります。左上(①)にメディアセンタが登録している貴方の名前、左下(②)にライセンス認証のアイコンがないことを確認してください。これで、PowerPointやWordなどMicrosoft Officeの他のアプリケーションも使えるようになります。&lt;span class="check"&gt;check-11&lt;/span&gt;
   </t>
     <rPh sb="14" eb="15">
@@ -6301,6 +6109,95 @@
   </si>
   <si>
     <t>0_20.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;h2&gt;&lt;a name="mfa"&gt;&lt;/a&gt;広大IDのMFA設定&lt;/h2&gt; </t>
+  </si>
+  <si>
+    <t>このPDFは広大IDのMFA設定の全体の操作の流れを説明しています。</t>
+    <rPh sb="6" eb="8">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>ゼンタイ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>ソウサ</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>ナガ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>セツメイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>raw:&lt;iframe width="100%" height="100%" style="aspect-ratio: 1000 / 1414" src="https://www.media.hiroshima-u.ac.jp/wp-content/uploads/2023/03/mfa-easymanual-20230327_HIRODAIID.pdf"&gt;&lt;/iframe&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PDFが見づらい場合は、Webマニュアルを参照しながら広大IDのMFA設定を開始してください。</t>
+    <rPh sb="4" eb="5">
+      <t>ミ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>サンショウ</t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="38" eb="40">
+      <t>カイシ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>raw:&lt;iframe width="100%" height="400px" src="https://www.media.hiroshima-u.ac.jp/services/mfa/mfa4hirodaiid/#mfa-hu-webmanu"&gt;&lt;/iframe&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h2 id="mfa-imc-account"&gt;IMCアカウントのMFA設定&lt;/h2&gt;</t>
+    <rPh sb="37" eb="39">
+      <t>セッテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>このPDFはIMCアカウントのMFA設定の全体の操作の流れを説明しています。</t>
+    <rPh sb="18" eb="20">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>ゼンタイ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>ソウサ</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>ナガ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>セツメイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>raw:&lt;iframe width="100%" height="100%" style="aspect-ratio: 1000 / 1414" src="https://www.media.hiroshima-u.ac.jp/wp-content/uploads/2025/02/mfa-easymanual-20250225_IMCaccount.pdf"&gt;&lt;/iframe&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>raw:&lt;iframe width="100%" height="400px" src="https://www.media.hiroshima-u.ac.jp/services/mfa/mfa4imcaccount/#mfa-imcaccount-setting-web"&gt;&lt;/iframe&gt;</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -6356,7 +6253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -6369,6 +6266,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6693,7 +6593,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>410</v>
+        <v>399</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -6709,7 +6609,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>412</v>
+        <v>401</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -6717,7 +6617,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>411</v>
+        <v>400</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -6768,7 +6668,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -6776,7 +6676,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -6792,17 +6692,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>421</v>
+        <v>410</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -6810,7 +6710,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -6821,13 +6721,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -6835,13 +6735,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -6849,13 +6749,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="96" x14ac:dyDescent="0.2">
@@ -6863,13 +6763,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="80" x14ac:dyDescent="0.2">
@@ -6877,13 +6777,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>408</v>
+        <v>397</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>
@@ -6911,10 +6811,10 @@
   <sheetData>
     <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -6922,7 +6822,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>352</v>
+        <v>343</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -6938,17 +6838,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>422</v>
+        <v>411</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -6956,12 +6856,12 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
       <c r="D9" t="s">
         <v>212</v>
@@ -6969,20 +6869,20 @@
     </row>
     <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
       <c r="D10" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="208" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -7024,7 +6924,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -7032,7 +6932,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -7048,7 +6948,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>423</v>
+        <v>412</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="96" x14ac:dyDescent="0.2">
@@ -7056,7 +6956,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7070,7 +6970,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -7080,13 +6980,13 @@
     </row>
     <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="C10" t="s">
         <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -7094,24 +6994,24 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -7119,13 +7019,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -7133,40 +7033,40 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="C16" t="s">
         <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
       <c r="C17" t="s">
         <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -7174,13 +7074,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="C18" t="s">
         <v>14</v>
       </c>
       <c r="D18" t="s">
-        <v>380</v>
+        <v>371</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -7188,24 +7088,24 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
       <c r="C19" t="s">
         <v>14</v>
       </c>
       <c r="D19" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="92.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
       <c r="C20" t="s">
         <v>47</v>
       </c>
       <c r="D20" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="96" x14ac:dyDescent="0.2">
@@ -7213,13 +7113,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
       <c r="C21" t="s">
         <v>14</v>
       </c>
       <c r="D21" t="s">
-        <v>386</v>
+        <v>377</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -7227,35 +7127,35 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>387</v>
+        <v>378</v>
       </c>
       <c r="C22" t="s">
         <v>14</v>
       </c>
       <c r="D22" t="s">
-        <v>388</v>
+        <v>379</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>389</v>
+        <v>380</v>
       </c>
       <c r="C23" t="s">
         <v>14</v>
       </c>
       <c r="D23" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>391</v>
+        <v>382</v>
       </c>
       <c r="C24" t="s">
         <v>14</v>
       </c>
       <c r="D24" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -7263,13 +7163,13 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>393</v>
+        <v>384</v>
       </c>
       <c r="C25" t="s">
         <v>14</v>
       </c>
       <c r="D25" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="80" x14ac:dyDescent="0.2">
@@ -7277,18 +7177,18 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
       <c r="C26" t="s">
         <v>14</v>
       </c>
       <c r="D26" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>397</v>
+        <v>388</v>
       </c>
     </row>
   </sheetData>
@@ -7302,7 +7202,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+    <sheetView topLeftCell="A20" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -7343,7 +7243,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>413</v>
+        <v>402</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="160" x14ac:dyDescent="0.2">
@@ -7379,7 +7279,7 @@
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>424</v>
+        <v>413</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -7393,7 +7293,7 @@
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>425</v>
+        <v>414</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -7404,7 +7304,7 @@
         <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>426</v>
+        <v>415</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -7412,21 +7312,21 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>398</v>
+        <v>389</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>427</v>
+        <v>416</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>399</v>
+        <v>390</v>
       </c>
       <c r="D12" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -7434,13 +7334,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>400</v>
+        <v>391</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>429</v>
+        <v>418</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -7451,7 +7351,7 @@
         <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>430</v>
+        <v>419</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -7465,7 +7365,7 @@
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>431</v>
+        <v>420</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -7479,7 +7379,7 @@
         <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>432</v>
+        <v>421</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -7493,7 +7393,7 @@
         <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>433</v>
+        <v>422</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -7504,7 +7404,7 @@
         <v>14</v>
       </c>
       <c r="D18" t="s">
-        <v>434</v>
+        <v>423</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -7515,7 +7415,7 @@
         <v>14</v>
       </c>
       <c r="D19" t="s">
-        <v>435</v>
+        <v>424</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="176" x14ac:dyDescent="0.2">
@@ -7526,7 +7426,7 @@
         <v>14</v>
       </c>
       <c r="D20" t="s">
-        <v>436</v>
+        <v>425</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -7537,7 +7437,7 @@
         <v>14</v>
       </c>
       <c r="D21" t="s">
-        <v>437</v>
+        <v>426</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -7548,7 +7448,7 @@
         <v>14</v>
       </c>
       <c r="D22" t="s">
-        <v>438</v>
+        <v>427</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -7559,7 +7459,7 @@
         <v>14</v>
       </c>
       <c r="D23" t="s">
-        <v>439</v>
+        <v>428</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -7570,7 +7470,7 @@
         <v>14</v>
       </c>
       <c r="D24" t="s">
-        <v>440</v>
+        <v>429</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -7581,7 +7481,7 @@
         <v>14</v>
       </c>
       <c r="D25" t="s">
-        <v>441</v>
+        <v>430</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -7592,7 +7492,7 @@
         <v>14</v>
       </c>
       <c r="D26" t="s">
-        <v>442</v>
+        <v>431</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -7603,7 +7503,7 @@
         <v>14</v>
       </c>
       <c r="D27" t="s">
-        <v>443</v>
+        <v>432</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -7617,7 +7517,7 @@
         <v>14</v>
       </c>
       <c r="D28" t="s">
-        <v>444</v>
+        <v>433</v>
       </c>
     </row>
   </sheetData>
@@ -7672,7 +7572,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>414</v>
+        <v>403</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="144" x14ac:dyDescent="0.2">
@@ -7708,7 +7608,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>401</v>
+        <v>392</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
@@ -7855,7 +7755,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>415</v>
+        <v>404</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="80" x14ac:dyDescent="0.2">
@@ -8312,7 +8212,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>416</v>
+        <v>405</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -8403,7 +8303,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>417</v>
+        <v>406</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="112" x14ac:dyDescent="0.2">
@@ -8665,8 +8565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8706,7 +8606,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="112" x14ac:dyDescent="0.2">
@@ -8817,7 +8717,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>402</v>
+        <v>393</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -8828,70 +8728,80 @@
     </row>
     <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" t="s">
-        <v>217</v>
+      <c r="B19" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B20" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="D20" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="B20" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>403</v>
-      </c>
-      <c r="C21" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B22" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="D22" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="B21" s="3"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B22" s="3"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+    </row>
+    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="C23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B23" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+    </row>
+    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>4</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B25" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -8945,7 +8855,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -8953,7 +8863,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -8969,7 +8879,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="112" x14ac:dyDescent="0.2">
@@ -8977,7 +8887,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8988,12 +8898,12 @@
     </row>
     <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="176" x14ac:dyDescent="0.2">
@@ -9001,13 +8911,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -9015,18 +8925,18 @@
         <v>4</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="D10" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="D11" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -9034,58 +8944,58 @@
         <v>4</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B13" s="3" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B14" s="3" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="D14" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="D15" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B16" s="3" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="D16" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="D17" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="D18" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -9093,13 +9003,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="96" x14ac:dyDescent="0.2">
@@ -9107,13 +9017,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -9121,13 +9031,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -9135,13 +9045,13 @@
         <v>4</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -9149,13 +9059,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -9163,34 +9073,34 @@
         <v>4</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B25" s="3" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="D25" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B26" s="3" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="D26" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B27" s="3" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -9198,13 +9108,13 @@
         <v>4</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -9212,50 +9122,50 @@
         <v>4</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B30" s="3" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="D30" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="96" x14ac:dyDescent="0.2">
       <c r="B31" s="3" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B32" s="3" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="D32" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="3" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="D33" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B34" s="3" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="D34" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -9263,13 +9173,13 @@
         <v>4</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -9277,47 +9187,47 @@
         <v>4</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>405</v>
+        <v>394</v>
       </c>
       <c r="C36" t="s">
         <v>4</v>
       </c>
       <c r="D36" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B37" s="3" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="D37" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B38" s="3" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="3" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="D39" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B40" s="3" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="D40" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B41" s="3" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -9325,53 +9235,53 @@
         <v>4</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="C42" t="s">
         <v>4</v>
       </c>
       <c r="D42" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B43" s="3" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="D43" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B44" s="3" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="D44" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B45" s="3" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="D45" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B46" s="3" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="D46" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B47" s="3" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="D47" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -9379,13 +9289,13 @@
         <v>4</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>406</v>
+        <v>395</v>
       </c>
       <c r="C48" t="s">
         <v>4</v>
       </c>
       <c r="D48" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -9416,7 +9326,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -9424,7 +9334,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -9440,7 +9350,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="224" x14ac:dyDescent="0.2">
@@ -9448,7 +9358,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -9467,7 +9377,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -9478,7 +9388,7 @@
     </row>
     <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -9486,91 +9396,91 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="D11" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="D12" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="D13" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="D14" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="D15" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>409</v>
+        <v>398</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="96" x14ac:dyDescent="0.2">
@@ -9578,7 +9488,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
@@ -9589,10 +9499,10 @@
     </row>
     <row r="21" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="D21" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="128" x14ac:dyDescent="0.2">
@@ -9600,18 +9510,18 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>407</v>
+        <v>396</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -9619,7 +9529,7 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
@@ -9633,7 +9543,7 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="C26" t="s">
         <v>14</v>
@@ -9644,13 +9554,13 @@
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="C27" t="s">
         <v>14</v>
       </c>
       <c r="D27" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="160" x14ac:dyDescent="0.2">
@@ -9658,13 +9568,13 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="C28" t="s">
         <v>14</v>
       </c>
       <c r="D28" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mac+lan.xlsx: update checklist numbers
</commit_message>
<xml_diff>
--- a/macs+lan.xlsx
+++ b/macs+lan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaeltei/Projects/HUProjects/fresta/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta2025\fresta-github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED85CC33-EF44-9343-BE40-64120043CA2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA52BE4-1ADC-42D3-AA54-75B4C6282541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6960" yWindow="2640" windowWidth="31440" windowHeight="16300" tabRatio="772" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="17496" windowHeight="10296" tabRatio="772" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="446">
   <si>
     <t>header1</t>
   </si>
@@ -2028,25 +2028,6 @@
     <t>2_33.png</t>
   </si>
   <si>
-    <t>全ての設定が完了をしたとのお知らせのウィンドウが開きます。「完了」をクリックします。</t>
-    <rPh sb="0" eb="1">
-      <t>スベテ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>カンリョウ</t>
-    </rPh>
-    <rPh sb="24" eb="25">
-      <t>ヒラキ</t>
-    </rPh>
-    <rPh sb="30" eb="32">
-      <t>カンリョウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>2_34.png</t>
   </si>
   <si>
@@ -2096,17 +2077,6 @@
   </si>
   <si>
     <t>2_37.png</t>
-  </si>
-  <si>
-    <t>表示されたESET Endpoint Antivirusの「アップデート」の部分をクリックします。
-&lt;span class="check"&gt;check 4&lt;/span&gt;</t>
-    <rPh sb="0" eb="1">
-      <t>ヒョウ</t>
-    </rPh>
-    <rPh sb="38" eb="40">
-      <t>ブブn</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>2_38.png</t>
@@ -2308,26 +2278,6 @@
     <t>4_2.png</t>
   </si>
   <si>
-    <t>自動アップデートの右側の赤枠で囲っている部分をクリックします。
-&lt;span class="check"&gt;check 3&lt;/span&gt;</t>
-    <rPh sb="0" eb="2">
-      <t>ジドウ</t>
-    </rPh>
-    <rPh sb="9" eb="11">
-      <t>ミギ</t>
-    </rPh>
-    <rPh sb="12" eb="14">
-      <t>アカワク</t>
-    </rPh>
-    <rPh sb="15" eb="16">
-      <t>カコ</t>
-    </rPh>
-    <rPh sb="20" eb="22">
-      <t>ブブn</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>4_3.png</t>
   </si>
   <si>
@@ -2463,31 +2413,6 @@
   </si>
   <si>
     <t>4_8.png</t>
-  </si>
-  <si>
-    <t>左側の概要が選択された状態で、右側の表示が「すべてのモジュールは最新です」となっていたらOKです。&lt;span class="check"&gt;check-5&lt;/span&gt;</t>
-    <rPh sb="0" eb="1">
-      <t>ヒダリ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>ガイヨウ</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>センタク</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>ジョウタイ</t>
-    </rPh>
-    <rPh sb="15" eb="17">
-      <t>ミギ</t>
-    </rPh>
-    <rPh sb="18" eb="20">
-      <t>ヒョウ</t>
-    </rPh>
-    <rPh sb="32" eb="34">
-      <t>サイシn</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>4_9.png</t>
@@ -2621,26 +2546,6 @@
   </si>
   <si>
     <t>4_16.png</t>
-  </si>
-  <si>
-    <t>赤枠で囲った部分をクリックします。検査対象となるものが表示されるので「Macintosh HD」をクリックします。Macintosh HDは、Macに内蔵されている副記憶装置(HDDもしくはSSD）を指します。「検査」をクリックすると、フルスキャンが始まります。&lt;span class="check"&gt;check-7&lt;/span&gt;
-フルスキャンの実行には数時間かかりますので、時間の余裕のあるときにできるだけ早く実行し、点検届を完成させてください。&lt;span class="check"&gt;check 6&lt;/span&gt;</t>
-    <rPh sb="0" eb="2">
-      <t>アカワク</t>
-    </rPh>
-    <rPh sb="3" eb="4">
-      <t>カコ</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>ブブn</t>
-    </rPh>
-    <rPh sb="17" eb="21">
-      <t>ケンサ</t>
-    </rPh>
-    <rPh sb="27" eb="29">
-      <t>ヒョウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>4_17.png</t>
@@ -3253,32 +3158,6 @@
   </si>
   <si>
     <t>ch5-hirodai-login-keep-signin.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Microsoft365にサインインした状態になります。&lt;span class="check"&gt;check-11&lt;/span&gt;
-ここでは左右を縮めて表示していますが、画面の右側のほうに「アプリをインストール」というメニュー(①)がありますので、そこから「Microsoft365 Apps」(②)を選びます。</t>
-    <rPh sb="20" eb="22">
-      <t>ジョウタイ</t>
-    </rPh>
-    <rPh sb="68" eb="70">
-      <t>サユウ</t>
-    </rPh>
-    <rPh sb="71" eb="72">
-      <t>チヂ</t>
-    </rPh>
-    <rPh sb="74" eb="76">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="83" eb="85">
-      <t>ガメン</t>
-    </rPh>
-    <rPh sb="86" eb="88">
-      <t>ミギガワ</t>
-    </rPh>
-    <rPh sb="149" eb="150">
-      <t>エラ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -5755,8 +5634,210 @@
     <t>本当にネットワーク接続しなくて良いのかしつこくもう一回聞かれますが、「続ける」をクリックして振り切ってください。</t>
   </si>
   <si>
+    <t>ここには私物MSアカウントよりは多くのデータを置いておくことができます。
+スマホ用のOneDriveアプリもありますので、外出先でもデータを取り出すことがあれば、活用してください。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>広島大学 2025年度 必携PC初期実習テキスト</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;h3&gt;macOS編&lt;/h3&gt;
+2025年3月&lt;br&gt;
+ 広島大学 情報メディア教育研究センター&lt;br&gt;
+ </t>
+  </si>
+  <si>
+    <t>FRESTA-TEXT-2025 Mac</t>
+  </si>
+  <si>
+    <t>FRESTA-TEXT-2025 Mac chap.0</t>
+  </si>
+  <si>
+    <t>FRESTA-TEXT-2025 Mac chap.1</t>
+  </si>
+  <si>
+    <t>FRESTA-TEXT-2025 Mac chap.2</t>
+  </si>
+  <si>
+    <t>FRESTA-TEXT-2025 Mac chap.3</t>
+  </si>
+  <si>
+    <t>FRESTA-TEXT-2025 Mac chap.4</t>
+  </si>
+  <si>
+    <t>FRESTA-TEXT-2025 Mac chap.5</t>
+  </si>
+  <si>
+    <t>FRESTA-TEXT-2025 Mac chap.6</t>
+  </si>
+  <si>
+    <t>FRESTA-TEXT-2025 Mac chap.7</t>
+  </si>
+  <si>
+    <t>FRESTA-TEXT-2025 Mac chap.8</t>
+  </si>
+  <si>
+    <t>FRESTA-TEXT-2025 Mac conclusion</t>
+  </si>
+  <si>
+    <t>FRESTA-TEXT-2025 macOS appendix A</t>
+  </si>
+  <si>
+    <t>0_1.jpg</t>
+  </si>
+  <si>
+    <t>0_2.jpg</t>
+  </si>
+  <si>
+    <t>0_3.jpg</t>
+  </si>
+  <si>
+    <t>0_4_1.jpg</t>
+  </si>
+  <si>
+    <t>0_4_2.jpg</t>
+  </si>
+  <si>
+    <t>0_4_3.jpg</t>
+  </si>
+  <si>
+    <t>0_6.jpg</t>
+  </si>
+  <si>
+    <t>0_7.jpg</t>
+  </si>
+  <si>
+    <t>0_8.jpg</t>
+  </si>
+  <si>
+    <t>0_9.jpg</t>
+  </si>
+  <si>
+    <t>0_10.jpg</t>
+  </si>
+  <si>
+    <t>0_11.jpg</t>
+  </si>
+  <si>
+    <t>0_12.jpg</t>
+  </si>
+  <si>
+    <t>0_13.jpg</t>
+  </si>
+  <si>
+    <t>0_14_1.jpg</t>
+  </si>
+  <si>
+    <t>0_15.jpg</t>
+  </si>
+  <si>
+    <t>0_16.jpg</t>
+  </si>
+  <si>
+    <t>0_17.jpg</t>
+  </si>
+  <si>
+    <t>0_18.jpg</t>
+  </si>
+  <si>
+    <t>0_19.jpg</t>
+  </si>
+  <si>
+    <t>0_20.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;h2&gt;&lt;a name="mfa"&gt;&lt;/a&gt;広大IDのMFA設定&lt;/h2&gt; </t>
+  </si>
+  <si>
+    <t>このPDFは広大IDのMFA設定の全体の操作の流れを説明しています。</t>
+    <rPh sb="6" eb="8">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>ゼンタイ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>ソウサ</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>ナガ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>セツメイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>raw:&lt;iframe width="100%" height="100%" style="aspect-ratio: 1000 / 1414" src="https://www.media.hiroshima-u.ac.jp/wp-content/uploads/2023/03/mfa-easymanual-20230327_HIRODAIID.pdf"&gt;&lt;/iframe&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PDFが見づらい場合は、Webマニュアルを参照しながら広大IDのMFA設定を開始してください。</t>
+    <rPh sb="4" eb="5">
+      <t>ミ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>サンショウ</t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="38" eb="40">
+      <t>カイシ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>raw:&lt;iframe width="100%" height="400px" src="https://www.media.hiroshima-u.ac.jp/services/mfa/mfa4hirodaiid/#mfa-hu-webmanu"&gt;&lt;/iframe&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h2 id="mfa-imc-account"&gt;IMCアカウントのMFA設定&lt;/h2&gt;</t>
+    <rPh sb="37" eb="39">
+      <t>セッテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>このPDFはIMCアカウントのMFA設定の全体の操作の流れを説明しています。</t>
+    <rPh sb="18" eb="20">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>ゼンタイ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>ソウサ</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>ナガ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>セツメイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>raw:&lt;iframe width="100%" height="100%" style="aspect-ratio: 1000 / 1414" src="https://www.media.hiroshima-u.ac.jp/wp-content/uploads/2025/02/mfa-easymanual-20250225_IMCaccount.pdf"&gt;&lt;/iframe&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>raw:&lt;iframe width="100%" height="400px" src="https://www.media.hiroshima-u.ac.jp/services/mfa/mfa4imcaccount/#mfa-imcaccount-setting-web"&gt;&lt;/iframe&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>2024年3月で最新のmacOS Sonoma (14.x)ではこのようなパネルが開きます。①チップ、②メモリ、③macOSのバージョン番号をメモしておきましょう。あるいはこのパネルの写真を撮っておきましょう。続いて、④詳細情報に進みます。
-&lt;span class="check"&gt;check 1&lt;/span&gt;</t>
+&lt;span class="check"&gt;check 2&lt;/span&gt;</t>
     <rPh sb="4" eb="5">
       <t>ネン</t>
     </rPh>
@@ -5793,7 +5874,27 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">ログインしたら、この画面（ダッシュボード）が出ます。&lt;span class="check"&gt;check 12&lt;/span&gt;
+    <t>赤枠で囲った部分をクリックします。検査対象となるものが表示されるので「Macintosh HD」をクリックします。Macintosh HDは、Macに内蔵されている副記憶装置(HDDもしくはSSD）を指します。「検査」をクリックすると、フルスキャンが始まります。&lt;span class="check"&gt;check 6&lt;/span&gt;
+フルスキャンの実行には数時間かかりますので、時間の余裕のあるときにできるだけ早く実行し、点検届を完成させてください。</t>
+    <rPh sb="0" eb="2">
+      <t>アカワク</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>カコ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>ブブn</t>
+    </rPh>
+    <rPh sb="17" eb="21">
+      <t>ケンサ</t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t>ヒョウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ログインしたら、この画面（ダッシュボード）が出ます。
 真ん中に見える「コースツリー」に、あなたがアクセスできるコースが表示されています。これらは、あなたの履修課目に関する授業支援や、広島大学において自習すべき教材などのコースです。（この図は在学生向けの一例で、新入生に表示されるものとは異なります）
 新入生向けに共通で表示されるものを簡単に説明すると：
 &lt;dl&gt;
@@ -5802,130 +5903,156 @@
 &lt;dt&gt;MFA設定ガイド&lt;/dt&gt;
 &lt;dd&gt;広島大学ではパスワード窃取によるアカウント乗っ取りの防止策として、広大IDを持つ全ての構成員に対しIMCアカウントおよび広大IDの多要素認証（MFA）設定を義務付けています。この「MFA設定ガイド」で、広島大学でMFA設定を行うための手順を説明しています&lt;/dd&gt; &lt;/dl&gt;
 </t>
-    <rPh sb="66" eb="67">
+    <rPh sb="31" eb="32">
       <t>ミ</t>
     </rPh>
-    <rPh sb="112" eb="114">
+    <rPh sb="77" eb="79">
       <t>リシュウ</t>
     </rPh>
-    <rPh sb="114" eb="116">
+    <rPh sb="79" eb="81">
       <t>カモク</t>
     </rPh>
-    <rPh sb="117" eb="118">
+    <rPh sb="82" eb="83">
       <t>カン</t>
     </rPh>
-    <rPh sb="120" eb="122">
+    <rPh sb="85" eb="87">
       <t>ジュギョウ</t>
     </rPh>
-    <rPh sb="122" eb="124">
+    <rPh sb="87" eb="89">
       <t>シエン</t>
     </rPh>
-    <rPh sb="126" eb="128">
+    <rPh sb="91" eb="93">
       <t>ヒロシマ</t>
     </rPh>
-    <rPh sb="128" eb="130">
+    <rPh sb="93" eb="95">
       <t>ダイガク</t>
     </rPh>
-    <rPh sb="134" eb="136">
+    <rPh sb="99" eb="101">
       <t>ジシュウ</t>
     </rPh>
-    <rPh sb="139" eb="141">
+    <rPh sb="104" eb="106">
       <t>キョウザイ</t>
     </rPh>
-    <rPh sb="158" eb="159">
+    <rPh sb="123" eb="124">
       <t>ム</t>
     </rPh>
-    <rPh sb="185" eb="188">
+    <rPh sb="150" eb="153">
       <t>シンニュウセイ</t>
     </rPh>
-    <rPh sb="188" eb="189">
+    <rPh sb="153" eb="154">
       <t>ム</t>
     </rPh>
-    <rPh sb="191" eb="193">
+    <rPh sb="156" eb="158">
       <t>キョウツウ</t>
     </rPh>
-    <rPh sb="194" eb="196">
+    <rPh sb="159" eb="161">
       <t>ヒョウジ</t>
     </rPh>
-    <rPh sb="341" eb="343">
+    <rPh sb="306" eb="308">
       <t>セッテイ</t>
     </rPh>
-    <rPh sb="344" eb="346">
+    <rPh sb="309" eb="311">
       <t>テンケン</t>
     </rPh>
-    <rPh sb="347" eb="348">
+    <rPh sb="312" eb="313">
       <t>ス</t>
     </rPh>
-    <rPh sb="359" eb="360">
+    <rPh sb="324" eb="325">
       <t>ハヤ</t>
     </rPh>
-    <rPh sb="368" eb="369">
+    <rPh sb="333" eb="334">
       <t>ヒラ</t>
     </rPh>
-    <rPh sb="406" eb="408">
+    <rPh sb="371" eb="373">
       <t>セッテイ</t>
     </rPh>
-    <rPh sb="421" eb="425">
+    <rPh sb="386" eb="390">
       <t>ヒロシマダイガク</t>
     </rPh>
-    <rPh sb="432" eb="434">
+    <rPh sb="397" eb="399">
       <t>セッシュ</t>
     </rPh>
-    <rPh sb="442" eb="443">
+    <rPh sb="407" eb="408">
       <t>ノ</t>
     </rPh>
-    <rPh sb="444" eb="445">
+    <rPh sb="409" eb="410">
       <t>ト</t>
     </rPh>
-    <rPh sb="454" eb="456">
+    <rPh sb="419" eb="421">
       <t>ヒロダイ</t>
     </rPh>
-    <rPh sb="459" eb="460">
+    <rPh sb="424" eb="425">
       <t>モ</t>
     </rPh>
-    <rPh sb="461" eb="462">
+    <rPh sb="426" eb="427">
       <t>スベ</t>
     </rPh>
+    <rPh sb="429" eb="432">
+      <t>コウセイイン</t>
+    </rPh>
+    <rPh sb="433" eb="434">
+      <t>タイ</t>
+    </rPh>
+    <rPh sb="446" eb="448">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="451" eb="456">
+      <t>タヨウソニンショウ</t>
+    </rPh>
+    <rPh sb="461" eb="463">
+      <t>セッテイ</t>
+    </rPh>
     <rPh sb="464" eb="467">
-      <t>コウセイイン</t>
-    </rPh>
-    <rPh sb="468" eb="469">
-      <t>タイ</t>
-    </rPh>
-    <rPh sb="481" eb="483">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="486" eb="491">
-      <t>タヨウソニンショウ</t>
-    </rPh>
-    <rPh sb="496" eb="498">
+      <t>ギムヅ</t>
+    </rPh>
+    <rPh sb="479" eb="481">
       <t>セッテイ</t>
     </rPh>
-    <rPh sb="499" eb="502">
-      <t>ギムヅ</t>
-    </rPh>
-    <rPh sb="514" eb="516">
+    <rPh sb="487" eb="491">
+      <t>ヒロシマダイガク</t>
+    </rPh>
+    <rPh sb="495" eb="497">
       <t>セッテイ</t>
     </rPh>
-    <rPh sb="522" eb="526">
-      <t>ヒロシマダイガク</t>
-    </rPh>
-    <rPh sb="530" eb="532">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="533" eb="534">
+    <rPh sb="498" eb="499">
       <t>オコナ</t>
     </rPh>
-    <rPh sb="538" eb="540">
+    <rPh sb="503" eb="505">
       <t>テジュン</t>
     </rPh>
-    <rPh sb="541" eb="543">
+    <rPh sb="506" eb="508">
       <t>セツメイ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">Excelの新規作成の画面に戻ります。左上(①)にメディアセンタが登録している貴方の名前、左下(②)にライセンス認証のアイコンがないことを確認してください。これで、PowerPointやWordなどMicrosoft Officeの他のアプリケーションも使えるようになります。&lt;span class="check"&gt;check-11&lt;/span&gt;
+    <t>Microsoft365にサインインした状態になります。&lt;span class="check"&gt;check 8&lt;/span&gt;
+ここでは左右を縮めて表示していますが、画面の右側のほうに「アプリをインストール」というメニュー(①)がありますので、そこから「Microsoft365 Apps」(②)を選びます。</t>
+    <rPh sb="20" eb="22">
+      <t>ジョウタイ</t>
+    </rPh>
+    <rPh sb="67" eb="69">
+      <t>サユウ</t>
+    </rPh>
+    <rPh sb="70" eb="71">
+      <t>チヂ</t>
+    </rPh>
+    <rPh sb="73" eb="75">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="82" eb="84">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="85" eb="87">
+      <t>ミギガワ</t>
+    </rPh>
+    <rPh sb="148" eb="149">
+      <t>エラ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Excelの新規作成の画面に戻ります。左上(①)にメディアセンタが登録している貴方の名前、左下(②)にライセンス認証のアイコンがないことを確認してください。これで、PowerPointやWordなどMicrosoft Officeの他のアプリケーションも使えるようになります。&lt;span class="check"&gt;check 9&lt;/span&gt;
   </t>
     <rPh sb="14" eb="15">
       <t>モド</t>
@@ -5955,7 +6082,7 @@
   </si>
   <si>
     <t>メニューの「Microsoft Autoupdateを終了します」をクリックすると、終了できます。 ウィンドウを閉じるのでも構いません。
-&lt;span class="check"&gt;check 11&lt;/span&gt;</t>
+&lt;span class="check"&gt;check 4&lt;/span&gt;</t>
     <rPh sb="56" eb="57">
       <t>ト</t>
     </rPh>
@@ -5965,20 +6092,20 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">するとこのような画面になります。&lt;span class="check"&gt;check 12&lt;/span&gt;
+    <t xml:space="preserve">するとこのような画面になります。&lt;span class="check"&gt;check 7&lt;/span&gt;
 これを「Myもみじのトップページ」と呼ぶことにしましょう。
 履修登録をしたり、成績を確認することができます。
 また「掲示」では、授業や学部からの連絡が表示されます。
 このまま引き続いて、次の「Moodle」の使い方に進みましょう。
   </t>
-    <rPh sb="70" eb="71">
+    <rPh sb="69" eb="70">
       <t>ヨ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t xml:space="preserve">この画面になったら「続ける」で進めてください。不安がある場合は証明書を表示してください(2023年春の時点ではNII Open Domain CAが発行した証明書が表示されます)。
-これで接続の設定が完了しました。 接続が完了すると「接続済み」と表示されます。&lt;span class="check"&gt;check 13&lt;/span&gt;
+これで接続の設定が完了しました。 接続が完了すると「接続済み」と表示されます。&lt;span class="check"&gt;check 10&lt;/span&gt;
   </t>
     <rPh sb="15" eb="16">
       <t>スス</t>
@@ -5998,149 +6125,104 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ここには私物MSアカウントよりは多くのデータを置いておくことができます。
-スマホ用のOneDriveアプリもありますので、外出先でもデータを取り出すことがあれば、活用してください。</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>広島大学 2025年度 必携PC初期実習テキスト</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;h3&gt;macOS編&lt;/h3&gt;
-2025年3月&lt;br&gt;
- 広島大学 情報メディア教育研究センター&lt;br&gt;
- </t>
-  </si>
-  <si>
-    <t>FRESTA-TEXT-2025 Mac</t>
-  </si>
-  <si>
-    <t>FRESTA-TEXT-2025 Mac chap.0</t>
-  </si>
-  <si>
-    <t>FRESTA-TEXT-2025 Mac chap.1</t>
-  </si>
-  <si>
-    <t>FRESTA-TEXT-2025 Mac chap.2</t>
-  </si>
-  <si>
-    <t>FRESTA-TEXT-2025 Mac chap.3</t>
-  </si>
-  <si>
-    <t>FRESTA-TEXT-2025 Mac chap.4</t>
-  </si>
-  <si>
-    <t>FRESTA-TEXT-2025 Mac chap.5</t>
-  </si>
-  <si>
-    <t>FRESTA-TEXT-2025 Mac chap.6</t>
-  </si>
-  <si>
-    <t>FRESTA-TEXT-2025 Mac chap.7</t>
-  </si>
-  <si>
-    <t>FRESTA-TEXT-2025 Mac chap.8</t>
-  </si>
-  <si>
-    <t>FRESTA-TEXT-2025 Mac conclusion</t>
-  </si>
-  <si>
-    <t>FRESTA-TEXT-2025 macOS appendix A</t>
-  </si>
-  <si>
-    <t>0_1.jpg</t>
-  </si>
-  <si>
-    <t>0_2.jpg</t>
-  </si>
-  <si>
-    <t>0_3.jpg</t>
-  </si>
-  <si>
-    <t>0_4_1.jpg</t>
-  </si>
-  <si>
-    <t>0_4_2.jpg</t>
-  </si>
-  <si>
-    <t>0_4_3.jpg</t>
-  </si>
-  <si>
-    <t>0_6.jpg</t>
-  </si>
-  <si>
-    <t>0_7.jpg</t>
-  </si>
-  <si>
-    <t>0_8.jpg</t>
-  </si>
-  <si>
-    <t>0_9.jpg</t>
-  </si>
-  <si>
-    <t>0_10.jpg</t>
-  </si>
-  <si>
-    <t>0_11.jpg</t>
-  </si>
-  <si>
-    <t>0_12.jpg</t>
-  </si>
-  <si>
-    <t>0_13.jpg</t>
-  </si>
-  <si>
-    <t>0_14_1.jpg</t>
-  </si>
-  <si>
-    <t>0_15.jpg</t>
-  </si>
-  <si>
-    <t>0_16.jpg</t>
-  </si>
-  <si>
-    <t>0_17.jpg</t>
-  </si>
-  <si>
-    <t>0_18.jpg</t>
-  </si>
-  <si>
-    <t>0_19.jpg</t>
-  </si>
-  <si>
-    <t>0_20.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;h2&gt;&lt;a name="mfa"&gt;&lt;/a&gt;広大IDのMFA設定&lt;/h2&gt; </t>
-  </si>
-  <si>
-    <t>このPDFは広大IDのMFA設定の全体の操作の流れを説明しています。</t>
+    <t>全ての設定が完了をしたとのお知らせのウィンドウが開きます。「完了」をクリックします。&lt;span class="check"&gt;check 1&lt;/span&gt;</t>
+    <rPh sb="0" eb="1">
+      <t>スベテ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>セッテイ</t>
+    </rPh>
     <rPh sb="6" eb="8">
+      <t>カンリョウ</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>ヒラキ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>カンリョウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>表示されたESET Endpoint Antivirusの「アップデート」の部分をクリックします。
+&lt;span class="check"&gt;check 5&lt;/span&gt;</t>
+    <rPh sb="0" eb="1">
+      <t>ヒョウ</t>
+    </rPh>
+    <rPh sb="38" eb="40">
+      <t>ブブn</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>自動アップデートの右側の赤枠で囲っている部分をクリックします。
+&lt;span class="check"&gt;check 4&lt;/span&gt;</t>
+    <rPh sb="0" eb="2">
+      <t>ジドウ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ミギ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>アカワク</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>カコ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>ブブn</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>左側の概要が選択された状態で、右側の表示が「すべてのモジュールは最新です」となっていたらOKです。&lt;span class="check"&gt;check 5&lt;/span&gt;</t>
+    <rPh sb="0" eb="1">
+      <t>ヒダリ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ガイヨウ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>センタク</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>ジョウタイ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>ミギ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>ヒョウ</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>サイシn</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>広大IDのMFA設定は点検届で回答が求められます。&lt;span class="check"&gt;check 11&lt;/span&gt;</t>
+    <rPh sb="0" eb="2">
       <t>ヒロダイ</t>
     </rPh>
-    <rPh sb="14" eb="16">
+    <rPh sb="8" eb="10">
       <t>セッテイ</t>
     </rPh>
-    <rPh sb="17" eb="19">
-      <t>ゼンタイ</t>
-    </rPh>
-    <rPh sb="20" eb="22">
-      <t>ソウサ</t>
-    </rPh>
-    <rPh sb="23" eb="24">
-      <t>ナガ</t>
-    </rPh>
-    <rPh sb="26" eb="28">
-      <t>セツメイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>raw:&lt;iframe width="100%" height="100%" style="aspect-ratio: 1000 / 1414" src="https://www.media.hiroshima-u.ac.jp/wp-content/uploads/2023/03/mfa-easymanual-20230327_HIRODAIID.pdf"&gt;&lt;/iframe&gt;</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>PDFが見づらい場合は、Webマニュアルを参照しながら広大IDのMFA設定を開始してください。</t>
+    <rPh sb="11" eb="13">
+      <t>テンケン</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>トドケ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>カイトウ</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>モト</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PDFが見づらい場合は、Webマニュアルを参照しながらIMCアカウントのMFA設定を開始してください。</t>
     <rPh sb="4" eb="5">
       <t>ミ</t>
     </rPh>
@@ -6150,53 +6232,34 @@
     <rPh sb="21" eb="23">
       <t>サンショウ</t>
     </rPh>
-    <rPh sb="27" eb="29">
+    <rPh sb="39" eb="41">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="42" eb="44">
+      <t>カイシ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>広大IDのMFA設定は点検届で回答が求められます。&lt;span class="check"&gt;check 12&lt;/span&gt;</t>
+    <rPh sb="0" eb="2">
       <t>ヒロダイ</t>
     </rPh>
-    <rPh sb="35" eb="37">
+    <rPh sb="8" eb="10">
       <t>セッテイ</t>
     </rPh>
-    <rPh sb="38" eb="40">
-      <t>カイシ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>raw:&lt;iframe width="100%" height="400px" src="https://www.media.hiroshima-u.ac.jp/services/mfa/mfa4hirodaiid/#mfa-hu-webmanu"&gt;&lt;/iframe&gt;</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>&lt;h2 id="mfa-imc-account"&gt;IMCアカウントのMFA設定&lt;/h2&gt;</t>
-    <rPh sb="37" eb="39">
-      <t>セッテイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>このPDFはIMCアカウントのMFA設定の全体の操作の流れを説明しています。</t>
-    <rPh sb="18" eb="20">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="21" eb="23">
-      <t>ゼンタイ</t>
-    </rPh>
-    <rPh sb="24" eb="26">
-      <t>ソウサ</t>
-    </rPh>
-    <rPh sb="27" eb="28">
-      <t>ナガ</t>
-    </rPh>
-    <rPh sb="30" eb="32">
-      <t>セツメイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>raw:&lt;iframe width="100%" height="100%" style="aspect-ratio: 1000 / 1414" src="https://www.media.hiroshima-u.ac.jp/wp-content/uploads/2025/02/mfa-easymanual-20250225_IMCaccount.pdf"&gt;&lt;/iframe&gt;</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>raw:&lt;iframe width="100%" height="400px" src="https://www.media.hiroshima-u.ac.jp/services/mfa/mfa4imcaccount/#mfa-imcaccount-setting-web"&gt;&lt;/iframe&gt;</t>
+    <rPh sb="11" eb="13">
+      <t>テンケン</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>トドケ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>カイトウ</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>モト</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -6208,26 +6271,26 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -6272,7 +6335,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -6580,7 +6643,7 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
@@ -6588,15 +6651,15 @@
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -6604,20 +6667,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>400</v>
+        <v>388</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -6626,7 +6689,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -6651,11 +6714,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
@@ -6663,23 +6726,23 @@
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -6687,103 +6750,103 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="160" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="D9" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="1" t="s">
+    <row r="13" spans="1:4" ht="66" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
         <v>334</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="96" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>340</v>
       </c>
     </row>
   </sheetData>
@@ -6801,7 +6864,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
@@ -6809,23 +6872,23 @@
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -6833,56 +6896,56 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="D9" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="D10" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
+    <row r="13" spans="1:4" ht="171.6" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
         <v>345</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="B9" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="D9" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B10" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="D10" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="208" x14ac:dyDescent="0.2">
-      <c r="B13" s="1" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -6907,11 +6970,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A14737B-27B4-430E-A2C9-8E4453FC8EAA}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
@@ -6919,23 +6982,23 @@
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -6943,20 +7006,20 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="96" x14ac:dyDescent="0.2">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6965,12 +7028,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="96" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -6978,217 +7041,217 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="C10" t="s">
         <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="C16" t="s">
         <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="C17" t="s">
         <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="C18" t="s">
         <v>14</v>
       </c>
       <c r="D18" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="C19" t="s">
         <v>14</v>
       </c>
       <c r="D19" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="92.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="92.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="C20" t="s">
         <v>47</v>
       </c>
       <c r="D20" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="96" x14ac:dyDescent="0.2">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="C21" t="s">
         <v>14</v>
       </c>
       <c r="D21" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="C22" t="s">
         <v>14</v>
       </c>
       <c r="D22" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="C23" t="s">
         <v>14</v>
       </c>
       <c r="D23" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="C24" t="s">
         <v>14</v>
       </c>
       <c r="D24" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="C25" t="s">
         <v>14</v>
       </c>
       <c r="D25" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="C26" t="s">
         <v>14</v>
       </c>
       <c r="D26" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -7202,19 +7265,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="84.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="84.109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" customWidth="1"/>
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -7222,7 +7285,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -7230,7 +7293,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -7238,15 +7301,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="160" x14ac:dyDescent="0.2">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -7260,7 +7323,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="112" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
@@ -7268,7 +7331,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -7279,10 +7342,10 @@
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -7293,10 +7356,10 @@
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
@@ -7304,46 +7367,46 @@
         <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="D12" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>17</v>
       </c>
@@ -7351,10 +7414,10 @@
         <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -7365,10 +7428,10 @@
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -7379,10 +7442,10 @@
         <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -7393,10 +7456,10 @@
         <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>21</v>
       </c>
@@ -7404,10 +7467,10 @@
         <v>14</v>
       </c>
       <c r="D18" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>22</v>
       </c>
@@ -7415,10 +7478,10 @@
         <v>14</v>
       </c>
       <c r="D19" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="176" x14ac:dyDescent="0.2">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>23</v>
       </c>
@@ -7426,10 +7489,10 @@
         <v>14</v>
       </c>
       <c r="D20" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>24</v>
       </c>
@@ -7437,10 +7500,10 @@
         <v>14</v>
       </c>
       <c r="D21" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>25</v>
       </c>
@@ -7448,10 +7511,10 @@
         <v>14</v>
       </c>
       <c r="D22" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>26</v>
       </c>
@@ -7459,10 +7522,10 @@
         <v>14</v>
       </c>
       <c r="D23" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>27</v>
       </c>
@@ -7470,10 +7533,10 @@
         <v>14</v>
       </c>
       <c r="D24" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>28</v>
       </c>
@@ -7481,10 +7544,10 @@
         <v>14</v>
       </c>
       <c r="D25" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>29</v>
       </c>
@@ -7492,10 +7555,10 @@
         <v>14</v>
       </c>
       <c r="D26" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
         <v>30</v>
       </c>
@@ -7503,10 +7566,10 @@
         <v>14</v>
       </c>
       <c r="D27" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -7517,7 +7580,7 @@
         <v>14</v>
       </c>
       <c r="D28" t="s">
-        <v>433</v>
+        <v>421</v>
       </c>
     </row>
   </sheetData>
@@ -7532,18 +7595,18 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="77.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="77.77734375" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" customWidth="1"/>
     <col min="4" max="4" width="30.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -7551,7 +7614,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -7559,7 +7622,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -7567,15 +7630,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="144" x14ac:dyDescent="0.2">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -7589,7 +7652,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -7603,12 +7666,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>392</v>
+        <v>431</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
@@ -7617,7 +7680,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -7631,7 +7694,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>40</v>
       </c>
@@ -7639,7 +7702,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="160" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -7653,7 +7716,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -7667,7 +7730,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>46</v>
       </c>
@@ -7678,7 +7741,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -7692,7 +7755,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="112" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>51</v>
       </c>
@@ -7715,18 +7778,18 @@
   <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="74.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="5.1640625" customWidth="1"/>
-    <col min="4" max="4" width="49.1640625" customWidth="1"/>
+    <col min="2" max="2" width="74.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="5.109375" customWidth="1"/>
+    <col min="4" max="4" width="49.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -7734,7 +7797,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -7742,7 +7805,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -7750,30 +7813,30 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="144" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>58</v>
       </c>
@@ -7781,7 +7844,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>60</v>
       </c>
@@ -7789,7 +7852,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="176" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>62</v>
       </c>
@@ -7797,7 +7860,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>64</v>
       </c>
@@ -7805,7 +7868,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -7819,7 +7882,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>68</v>
       </c>
@@ -7827,7 +7890,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>70</v>
       </c>
@@ -7835,7 +7898,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -7846,7 +7909,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>74</v>
       </c>
@@ -7854,7 +7917,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -7865,7 +7928,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>78</v>
       </c>
@@ -7873,7 +7936,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>80</v>
       </c>
@@ -7881,7 +7944,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="83" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="82.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>82</v>
       </c>
@@ -7889,7 +7952,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -7900,7 +7963,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -7911,7 +7974,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -7922,7 +7985,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>90</v>
       </c>
@@ -7930,7 +7993,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -7941,7 +8004,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -7952,7 +8015,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -7963,7 +8026,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -7974,7 +8037,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>4</v>
       </c>
@@ -7985,7 +8048,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -7996,7 +8059,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -8007,7 +8070,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -8018,7 +8081,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>4</v>
       </c>
@@ -8029,7 +8092,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>4</v>
       </c>
@@ -8040,7 +8103,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
         <v>112</v>
       </c>
@@ -8048,7 +8111,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
         <v>114</v>
       </c>
@@ -8056,7 +8119,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
         <v>116</v>
       </c>
@@ -8064,7 +8127,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
         <v>118</v>
       </c>
@@ -8072,7 +8135,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
         <v>120</v>
       </c>
@@ -8080,7 +8143,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
         <v>122</v>
       </c>
@@ -8088,7 +8151,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
         <v>124</v>
       </c>
@@ -8096,7 +8159,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
         <v>116</v>
       </c>
@@ -8104,60 +8167,60 @@
         <v>126</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="D44" t="s">
         <v>127</v>
       </c>
-      <c r="D44" t="s">
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B45" s="1" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B45" s="1" t="s">
+      <c r="D45" t="s">
         <v>129</v>
       </c>
-      <c r="D45" t="s">
+    </row>
+    <row r="46" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B46" s="1" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="B46" s="1" t="s">
+      <c r="D46" t="s">
         <v>131</v>
       </c>
-      <c r="D46" t="s">
+    </row>
+    <row r="47" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B47" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="B47" s="1" t="s">
+      <c r="D47" t="s">
         <v>133</v>
       </c>
-      <c r="D47" t="s">
+    </row>
+    <row r="48" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B48" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="D48" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="B48" s="1" t="s">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B49" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D49" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="49" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B49" s="1" t="s">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B50" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D50" t="s">
         <v>138</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B50" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D50" t="s">
-        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -8175,7 +8238,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
@@ -8183,23 +8246,23 @@
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -8207,48 +8270,48 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="66" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D7" t="s">
         <v>143</v>
       </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
+    </row>
+    <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D7" t="s">
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
         <v>145</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
-        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -8262,11 +8325,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
@@ -8274,23 +8337,23 @@
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -8298,260 +8361,260 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="112" x14ac:dyDescent="0.2">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="1" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>154</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C10" t="s">
         <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>158</v>
+        <v>441</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
       </c>
       <c r="D11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
+      <c r="D13" t="s">
         <v>160</v>
       </c>
-      <c r="D12" t="s">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>161</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="B13" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="D13" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>164</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C15" t="s">
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D18" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="D19" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D20" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="1" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D21" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="B20" s="1" t="s">
+    <row r="22" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D22" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B21" s="1" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D23" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="96" x14ac:dyDescent="0.2">
-      <c r="B22" s="1" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D24" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B23" s="1" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D25" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B24" s="1" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D26" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B25" s="1" t="s">
+    <row r="27" spans="1:4" ht="66" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="D27" t="s">
         <v>184</v>
       </c>
-      <c r="D25" t="s">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B28" s="1" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B26" s="1" t="s">
+      <c r="D28" t="s">
         <v>186</v>
       </c>
-      <c r="D26" t="s">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B29" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="96" x14ac:dyDescent="0.2">
-      <c r="B27" s="1" t="s">
+      <c r="D29" t="s">
         <v>188</v>
       </c>
-      <c r="D27" t="s">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B30" s="1" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B28" s="1" t="s">
+      <c r="D30" t="s">
         <v>190</v>
-      </c>
-      <c r="D28" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B29" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="D29" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B30" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="D30" t="s">
-        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -8565,11 +8628,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
@@ -8577,23 +8640,23 @@
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -8601,109 +8664,109 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="112" x14ac:dyDescent="0.2">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
         <v>198</v>
       </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
+    </row>
+    <row r="11" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="B8" s="1" t="s">
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B9" s="1" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="128" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="1" t="s">
+    <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="B11" s="1" t="s">
+    <row r="14" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="D14" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="1" t="s">
+      <c r="D15" t="s">
         <v>207</v>
       </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
+    </row>
+    <row r="16" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>208</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="B14" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="D14" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B15" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="D15" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="112" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>213</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -8712,55 +8775,57 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="240" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="198" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>4</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>393</v>
+        <v>433</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>4</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>435</v>
+        <v>423</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="3" t="s">
-        <v>437</v>
+        <v>425</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>438</v>
+        <v>426</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="3"/>
+      <c r="B21" s="3" t="s">
+        <v>443</v>
+      </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
     </row>
@@ -8769,44 +8834,47 @@
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
     </row>
-    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>4</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>439</v>
+        <v>427</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
     </row>
-    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>4</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>440</v>
+        <v>428</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B25" s="3" t="s">
-        <v>437</v>
+        <v>444</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>442</v>
+        <v>430</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>4</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>445</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
@@ -8838,35 +8906,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="B42" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="100.6640625" style="3" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="34.83203125" customWidth="1"/>
+    <col min="4" max="4" width="34.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -8874,20 +8942,20 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="112" x14ac:dyDescent="0.2">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8896,406 +8964,406 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="176" x14ac:dyDescent="0.2">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="132" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="D9" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D10" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B11" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D11" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="3" t="s">
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
         <v>222</v>
       </c>
-      <c r="D10" t="s">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="3" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="B11" s="3" t="s">
+    <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B14" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D14" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="3" t="s">
+    <row r="15" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B15" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="D15" t="s">
         <v>226</v>
       </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
+    </row>
+    <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B16" s="3" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B13" s="3" t="s">
+      <c r="D16" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="B14" s="3" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B17" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D17" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="B15" s="3" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B18" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D18" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="B16" s="3" t="s">
+    <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="D16" t="s">
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="B17" s="3" t="s">
+    <row r="20" spans="1:4" ht="66" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="D17" t="s">
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B18" s="3" t="s">
+    <row r="21" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="D18" t="s">
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="3" t="s">
+    <row r="22" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="C19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="96" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="3" t="s">
+    <row r="23" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="C20" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" s="3" t="s">
+    <row r="24" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="C21" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="3" t="s">
+    <row r="25" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B25" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="C22" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="D25" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" s="3" t="s">
+    <row r="26" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B26" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="C23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="D26" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="3" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B27" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="C24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" t="s">
+    </row>
+    <row r="28" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="B25" s="3" t="s">
+      <c r="C28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" t="s">
         <v>251</v>
       </c>
-      <c r="D25" t="s">
+    </row>
+    <row r="29" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="B26" s="3" t="s">
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" t="s">
         <v>253</v>
       </c>
-      <c r="D26" t="s">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B30" s="3" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B27" s="3" t="s">
+      <c r="D30" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>4</v>
-      </c>
-      <c r="B28" s="3" t="s">
+    <row r="31" spans="1:4" ht="66" x14ac:dyDescent="0.2">
+      <c r="B31" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="C28" t="s">
-        <v>4</v>
-      </c>
-      <c r="D28" t="s">
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B32" s="3" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>4</v>
-      </c>
-      <c r="B29" s="3" t="s">
+      <c r="D32" t="s">
         <v>258</v>
       </c>
-      <c r="C29" t="s">
-        <v>4</v>
-      </c>
-      <c r="D29" t="s">
+    </row>
+    <row r="33" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="3" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="B30" s="3" t="s">
+      <c r="D33" t="s">
         <v>260</v>
       </c>
-      <c r="D30" t="s">
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B34" s="3" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="96" x14ac:dyDescent="0.2">
-      <c r="B31" s="3" t="s">
+      <c r="D34" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B32" s="3" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="D32" t="s">
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="3" t="s">
+    <row r="36" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="C36" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" t="s">
         <v>265</v>
       </c>
-      <c r="D33" t="s">
+    </row>
+    <row r="37" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B37" s="3" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B34" s="3" t="s">
+      <c r="D37" t="s">
         <v>267</v>
       </c>
-      <c r="D34" t="s">
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B38" s="3" t="s">
         <v>268</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>4</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="C35" t="s">
-        <v>4</v>
-      </c>
-      <c r="D35" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>4</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>394</v>
-      </c>
-      <c r="C36" t="s">
-        <v>4</v>
-      </c>
-      <c r="D36" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="B37" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="D37" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B38" s="3" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="D39" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B40" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="D40" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B41" s="3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="C42" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" t="s">
         <v>275</v>
       </c>
-      <c r="D39" t="s">
+    </row>
+    <row r="43" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B43" s="3" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="B40" s="3" t="s">
+      <c r="D43" t="s">
         <v>277</v>
       </c>
-      <c r="D40" t="s">
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B44" s="3" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B41" s="3" t="s">
+      <c r="D44" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>4</v>
-      </c>
-      <c r="B42" s="3" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B45" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="C42" t="s">
-        <v>4</v>
-      </c>
-      <c r="D42" t="s">
+      <c r="D45" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="B43" s="3" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B46" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D46" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B44" s="3" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B47" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D47" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B45" s="3" t="s">
+    <row r="48" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>4</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="C48" t="s">
+        <v>4</v>
+      </c>
+      <c r="D48" t="s">
         <v>286</v>
-      </c>
-      <c r="D45" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B46" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="D46" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B47" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="D47" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>4</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>395</v>
-      </c>
-      <c r="C48" t="s">
-        <v>4</v>
-      </c>
-      <c r="D48" t="s">
-        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -9309,11 +9377,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A687F900-5547-4D89-8494-B67FCE27BE96}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A18" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
@@ -9321,23 +9389,23 @@
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -9345,150 +9413,150 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="224" x14ac:dyDescent="0.2">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="184.8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="D11" t="s">
         <v>295</v>
       </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="1" t="s">
+    </row>
+    <row r="12" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B9" s="1" t="s">
+      <c r="D12" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="1" t="s">
+    <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="D13" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="B11" s="1" t="s">
+    <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B14" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D14" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
+    <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D15" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="B13" s="1" t="s">
+    <row r="16" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="D13" t="s">
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="B14" s="2" t="s">
+    <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
         <v>306</v>
       </c>
-      <c r="D14" t="s">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="B15" s="1" t="s">
+    <row r="19" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="D15" t="s">
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="B16" s="1" t="s">
+    <row r="20" spans="1:4" ht="66" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>310</v>
-      </c>
-      <c r="C16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="B17" s="1" t="s">
-        <v>398</v>
-      </c>
-      <c r="C17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B18" s="1" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="B19" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="C19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="96" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>316</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
@@ -9497,39 +9565,39 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="D21" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="128" x14ac:dyDescent="0.2">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>396</v>
+        <v>437</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
@@ -9538,43 +9606,43 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="112" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="C26" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="144" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="C27" t="s">
         <v>14</v>
       </c>
       <c r="D27" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="160" x14ac:dyDescent="0.2">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="132" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="C28" t="s">
         <v>14</v>
       </c>
       <c r="D28" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mac+lan.xlsx: fix a typo (hirodai-id -> imc-account)
</commit_message>
<xml_diff>
--- a/macs+lan.xlsx
+++ b/macs+lan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta2025\fresta-github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA52BE4-1ADC-42D3-AA54-75B4C6282541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB7D920-1DDD-4306-8E64-E62D04E7A25C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="17496" windowHeight="10296" tabRatio="772" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="17496" windowHeight="10296" tabRatio="772" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -6241,23 +6241,20 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>広大IDのMFA設定は点検届で回答が求められます。&lt;span class="check"&gt;check 12&lt;/span&gt;</t>
-    <rPh sb="0" eb="2">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="8" eb="10">
+    <t>IMCアカウントのMFA設定は点検届で回答が求められます。&lt;span class="check"&gt;check 12&lt;/span&gt;</t>
+    <rPh sb="12" eb="14">
       <t>セッテイ</t>
     </rPh>
-    <rPh sb="11" eb="13">
+    <rPh sb="15" eb="17">
       <t>テンケン</t>
     </rPh>
-    <rPh sb="13" eb="14">
+    <rPh sb="17" eb="18">
       <t>トドケ</t>
     </rPh>
-    <rPh sb="15" eb="17">
+    <rPh sb="19" eb="21">
       <t>カイトウ</t>
     </rPh>
-    <rPh sb="18" eb="19">
+    <rPh sb="22" eb="23">
       <t>モト</t>
     </rPh>
     <phoneticPr fontId="1"/>
@@ -6714,7 +6711,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -6860,7 +6857,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -6970,7 +6967,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A14737B-27B4-430E-A2C9-8E4453FC8EAA}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+    <sheetView topLeftCell="A23" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -8628,8 +8625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -9377,7 +9374,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A687F900-5547-4D89-8494-B67FCE27BE96}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A27" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix ESET for Mac
</commit_message>
<xml_diff>
--- a/macs+lan.xlsx
+++ b/macs+lan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta2025\fresta-github\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Projects/IMC/HikkeiPC/fresta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB7D920-1DDD-4306-8E64-E62D04E7A25C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20FC6D8E-6250-B848-9BAE-A903CE48C696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="17496" windowHeight="10296" tabRatio="772" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-60" yWindow="3280" windowWidth="31060" windowHeight="17480" tabRatio="772" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="447">
   <si>
     <t>header1</t>
   </si>
@@ -1333,42 +1333,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>以下のサイト「ダウンロード（マイクロソフト包括ライセンス）」をsafariブラウザで開いて、その中の「WindowsOS, ウィルス対策ソフト(ESET)」「学生の個人所有PC用のダウンロードはこちらから」のリンクをクリックしてください。
-※ ESET はマイクロソフト製品ではありませんが、大学で提供するソフトウェアとしてまとめてサービスしています
-&lt;a href="https://www.media.hiroshima-u.ac.jp/services/ms-ees/ms-download/"&gt;https://www.media.hiroshima-u.ac.jp/services/ms-ees/ms-download/&lt;/a&gt;</t>
-    <rPh sb="21" eb="23">
-      <t>ホウカツ</t>
-    </rPh>
-    <rPh sb="48" eb="49">
-      <t>ナカ</t>
-    </rPh>
-    <rPh sb="66" eb="68">
-      <t>タイサク</t>
-    </rPh>
-    <rPh sb="79" eb="81">
-      <t>ガクセイ</t>
-    </rPh>
-    <rPh sb="82" eb="84">
-      <t>コジン</t>
-    </rPh>
-    <rPh sb="84" eb="86">
-      <t>ショユウ</t>
-    </rPh>
-    <rPh sb="88" eb="89">
-      <t>ヨウ</t>
-    </rPh>
-    <rPh sb="135" eb="137">
-      <t>セイヒン</t>
-    </rPh>
-    <rPh sb="146" eb="148">
-      <t>ダイガク</t>
-    </rPh>
-    <rPh sb="149" eb="151">
-      <t>テイキョウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>2_1.png</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1388,31 +1352,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>&lt;font color="red"&gt;※ 図のスクリーンイメージは現在のものと少し異なりますが、作業内容は下記のとおりです&lt;/font&gt;
-下のほうにある「ESET Endpoint Antivirus for Mac」からダウンロードします。
-※ このページの「インストールマニュアル」をクリックすると、インストール手順を書いたマニュアルが表示されます。できればこのマニュアルを別ウィンドウで表示したままにしておくと、あとの作業がやりやすいでしょう。
-ESETアクティベーションキー表示をクリックしアクティベーションキーをメモしておきましょう。&lt;/p&gt;</t>
-    <rPh sb="20" eb="21">
-      <t>ズ</t>
-    </rPh>
-    <rPh sb="32" eb="34">
-      <t>ゲンザイ</t>
-    </rPh>
-    <rPh sb="38" eb="39">
-      <t>スコ</t>
-    </rPh>
-    <rPh sb="40" eb="41">
-      <t>コト</t>
-    </rPh>
-    <rPh sb="47" eb="49">
-      <t>サギョウ</t>
-    </rPh>
-    <rPh sb="49" eb="51">
-      <t>ナイヨウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>2_2.png</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1629,228 +1568,39 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>インストールが開始されます・</t>
-    <rPh sb="0" eb="14">
-      <t>カクニンスイショウセッテイスス</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>2_12.png</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>インストールが完了するまで待ちましょう。</t>
-    <rPh sb="1" eb="2">
-      <t>ノゾ</t>
-    </rPh>
-    <rPh sb="7" eb="10">
-      <t>カノウセイケンシュツカクニンキテイススカマ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>2_13.png</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>インストールが完了するとウィンドウが表示されます。「続行」のボタンをクリックします。</t>
-    <rPh sb="17" eb="19">
-      <t>カクニン</t>
-    </rPh>
-    <rPh sb="41" eb="42">
-      <t>ヨウスス</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>2_14.png</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>推奨される保護設定の画面が表示されます。</t>
-    <rPh sb="0" eb="2">
-      <t>ショウヒ</t>
-    </rPh>
-    <rPh sb="10" eb="12">
-      <t>ヨウリョウ</t>
-    </rPh>
-    <rPh sb="13" eb="14">
-      <t>シメカアヨウリョウスクバアイモヌシソウダンヘ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>2_15.png</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>チェックボックスを全てチェックし、「全て有効にして続行」をクリックします。</t>
-    <rPh sb="0" eb="2">
-      <t>ジッサイ</t>
-    </rPh>
-    <rPh sb="8" eb="9">
-      <t>カ</t>
-    </rPh>
-    <rPh sb="10" eb="11">
-      <t>コ</t>
-    </rPh>
-    <rPh sb="12" eb="14">
-      <t>ダンカイ</t>
-    </rPh>
-    <rPh sb="21" eb="23">
-      <t>カクニン</t>
-    </rPh>
-    <rPh sb="24" eb="25">
-      <t>モト</t>
-    </rPh>
-    <rPh sb="31" eb="32">
-      <t>イマ</t>
-    </rPh>
-    <rPh sb="32" eb="35">
-      <t>シヨウチュウスデニュウリョクオモニュウリョクデンゲントウニュウチョクゴセッテイツカシャシアタラカチュウイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>2_16.png:</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>機能拡張がブロックされましたのポップアップが表示されます。「システム設定を開く」をクリックします。</t>
-    <rPh sb="7" eb="9">
-      <t>カイシ</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>サイチュウ</t>
-    </rPh>
-    <rPh sb="21" eb="23">
-      <t>キノウ</t>
-    </rPh>
-    <rPh sb="23" eb="25">
-      <t>カクチョウ</t>
-    </rPh>
-    <rPh sb="45" eb="47">
-      <t>ホゴデカンリョウゴタイショオ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>2_17.png</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>「システム設定」のウィンドウが開かれるので、「プライバシーとセキュリティ」の中のセキュリティの部分の「詳細」ボタンをクリックします。</t>
-    <rPh sb="0" eb="2">
-      <t>カンリョウ</t>
-    </rPh>
-    <rPh sb="6" eb="7">
-      <t>ト</t>
-    </rPh>
-    <rPh sb="14" eb="15">
-      <t>オ</t>
-    </rPh>
-    <rPh sb="17" eb="18">
-      <t>カマ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>2_18.png</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>自分のパソコンの管理者権限が要求されるので、自分のパソコンにログインするときのアカウントとパスワードを入力し、「設定を変更」jをクリックします。</t>
-    <rPh sb="0" eb="2">
-      <t>イコウ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>サギョウ</t>
-    </rPh>
-    <rPh sb="10" eb="12">
-      <t>サイチュウ</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>コウセイ</t>
-    </rPh>
-    <rPh sb="20" eb="22">
-      <t>ツイカ</t>
-    </rPh>
-    <rPh sb="23" eb="24">
-      <t>モト</t>
-    </rPh>
-    <rPh sb="32" eb="33">
-      <t>デ</t>
-    </rPh>
-    <rPh sb="37" eb="39">
-      <t>キョカ</t>
-    </rPh>
-    <rPh sb="41" eb="42">
-      <t>スス</t>
-    </rPh>
-    <rPh sb="47" eb="49">
-      <t>キョカ</t>
-    </rPh>
-    <rPh sb="54" eb="55">
-      <t>ト</t>
-    </rPh>
-    <rPh sb="59" eb="60">
-      <t>ナニ</t>
-    </rPh>
-    <rPh sb="61" eb="63">
-      <t>ツウシンデエツランツカバアイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>2_19.png</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>表示されているスイッチを有効にします。</t>
-    <rPh sb="1" eb="3">
-      <t>キノウ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>カクチョウセッテイヒラ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>2_20.png</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>「OK」をクリックします。</t>
-    <rPh sb="0" eb="13">
-      <t>セッテイヒライチブミギショウサイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>2_21.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ESETシステムの拡張機能を有効にする画面が表示されるので、「続行」をクリックします。</t>
-    <rPh sb="0" eb="2">
-      <t>ショウサイ</t>
-    </rPh>
-    <rPh sb="6" eb="7">
-      <t>ヒラ</t>
-    </rPh>
-    <rPh sb="14" eb="16">
-      <t>ツイカ</t>
-    </rPh>
-    <rPh sb="29" eb="31">
-      <t>キョカ</t>
-    </rPh>
-    <rPh sb="31" eb="33">
-      <t>ジョウタイ</t>
-    </rPh>
-    <rPh sb="34" eb="36">
-      <t>ヒョウジサイショト</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1878,22 +1628,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>"ESET Web and Email Protection"がプロキシ構成の追加を求めていますの画面が表示されます。許可をクリックします。</t>
-    <rPh sb="17" eb="18">
-      <t>デ</t>
-    </rPh>
-    <rPh sb="23" eb="25">
-      <t>ミギガワ</t>
-    </rPh>
-    <rPh sb="33" eb="34">
-      <t>スベ</t>
-    </rPh>
-    <rPh sb="67" eb="69">
-      <t>シュウリョウアラヒョウジアトオコナトサイキドウユウコウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>2_24.png</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1949,79 +1683,15 @@
     <t>2_28.png</t>
   </si>
   <si>
-    <t>製品のアクティベーションの画面が表示されます。[2]でメモしたアクティベーションキーを入力し「続行」クリックします。</t>
-    <rPh sb="0" eb="2">
-      <t>セイヒn</t>
-    </rPh>
-    <rPh sb="13" eb="15">
-      <t>ガメn</t>
-    </rPh>
-    <rPh sb="16" eb="18">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="43" eb="45">
-      <t>ニュウリョク</t>
-    </rPh>
-    <rPh sb="47" eb="49">
-      <t>ゾッコウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>2_29.png</t>
   </si>
   <si>
-    <t>通知を許可する画面が表示されます。システム設定の部分をクリックします。</t>
-    <rPh sb="0" eb="2">
-      <t>ツウティ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>キョカ</t>
-    </rPh>
-    <rPh sb="7" eb="9">
-      <t>ガメn</t>
-    </rPh>
-    <rPh sb="10" eb="12">
-      <t>ヒョウ</t>
-    </rPh>
-    <rPh sb="21" eb="23">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="24" eb="26">
-      <t>ブブn</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>2_30.png</t>
   </si>
   <si>
-    <t>システム設定の通知をクリックします。ESET Endpoint Antivirusをクリックします。</t>
-    <rPh sb="0" eb="2">
-      <t>システムセッテイ</t>
-    </rPh>
-    <rPh sb="7" eb="9">
-      <t>ツウティ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>2_31.png</t>
   </si>
   <si>
-    <t>通知を許可を有効にします。</t>
-    <rPh sb="0" eb="1">
-      <t>ツウティ</t>
-    </rPh>
-    <rPh sb="3" eb="4">
-      <t>キョカ</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>ユウコウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>2_32.png</t>
   </si>
   <si>
@@ -2031,75 +1701,19 @@
     <t>2_34.png</t>
   </si>
   <si>
-    <t>インストールウィザードの「閉じる」をクリックします。</t>
-    <rPh sb="13" eb="14">
-      <t>トジ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>2_35.png</t>
   </si>
   <si>
-    <t>ダウンロードしたファイルをゴミ箱に入れるかどうか聞いてくるポップアップが表示されます。「ゴミ箱に入れる」をクリックします。</t>
-    <rPh sb="17" eb="18">
-      <t>イレ</t>
-    </rPh>
-    <rPh sb="24" eb="25">
-      <t>キイテ</t>
-    </rPh>
-    <rPh sb="36" eb="38">
-      <t>ヒョウ</t>
-    </rPh>
-    <rPh sb="48" eb="49">
-      <t>イレ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>2_36.png</t>
   </si>
   <si>
-    <t>全てのウィンドウを閉じて、ESET Endpoint Antivirusの部分をクリックし、ESET Endpoint Antivirusを表示をクリックします。</t>
-    <rPh sb="0" eb="2">
-      <t>スベテ</t>
-    </rPh>
-    <rPh sb="9" eb="10">
-      <t>トジ</t>
-    </rPh>
-    <rPh sb="37" eb="39">
-      <t>ブブn</t>
-    </rPh>
-    <rPh sb="70" eb="72">
-      <t>ヒョウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>2_37.png</t>
   </si>
   <si>
     <t>2_38.png</t>
   </si>
   <si>
-    <t>「アップデートの確認」をクリックします。</t>
-    <rPh sb="8" eb="10">
-      <t>カクニn</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>2_39.png</t>
-  </si>
-  <si>
-    <t>アップデートが完了した画面です。</t>
-    <rPh sb="7" eb="9">
-      <t>カn</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>ガメn</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>2_40.png</t>
@@ -6125,36 +5739,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>全ての設定が完了をしたとのお知らせのウィンドウが開きます。「完了」をクリックします。&lt;span class="check"&gt;check 1&lt;/span&gt;</t>
-    <rPh sb="0" eb="1">
-      <t>スベテ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>カンリョウ</t>
-    </rPh>
-    <rPh sb="24" eb="25">
-      <t>ヒラキ</t>
-    </rPh>
-    <rPh sb="30" eb="32">
-      <t>カンリョウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>表示されたESET Endpoint Antivirusの「アップデート」の部分をクリックします。
-&lt;span class="check"&gt;check 5&lt;/span&gt;</t>
-    <rPh sb="0" eb="1">
-      <t>ヒョウ</t>
-    </rPh>
-    <rPh sb="38" eb="40">
-      <t>ブブn</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>自動アップデートの右側の赤枠で囲っている部分をクリックします。
 &lt;span class="check"&gt;check 4&lt;/span&gt;</t>
     <rPh sb="0" eb="2">
@@ -6258,6 +5842,92 @@
       <t>モト</t>
     </rPh>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>以下のサイト「ダウンロード（マイクロソフト包括ライセンス）」をsafariブラウザで開いて、その中の「WindowsOS, ウィルス対策ソフト(ESET)」「学生の個人所有PC用のダウンロードはこちらから」のリンクをクリックしてください。
+※ ESET はマイクロソフト製品ではありませんが、大学で提供するソフトウェアとしてまとめてサービスしています
+&lt;a href="https://www.media.hiroshima-u.ac.jp/services/antivirus/vs-download/"&gt;https://www.media.hiroshima-u.ac.jp/services/antivirus/vs-download/&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>2_16.png</t>
+  </si>
+  <si>
+    <t>&lt;font color="red"&gt;※ 図のスクリーンイメージは現在のものと少し異なりますが、作業内容は下記のとおりです&lt;/font&gt;
+下のほうにある「ESET Endpoint Security for Mac」からダウンロードします。
+※ このページの「インストールマニュアル」をクリックすると、インストール手順を書いたマニュアルが表示されます。できればこのマニュアルを別ウィンドウで表示したままにしておくと、あとの作業がやりやすいでしょう。
+ESETアクティベーションキー表示をクリックしアクティベーションキーをメモしておきましょう。&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>インストールが完了するまで待ちましょう。</t>
+  </si>
+  <si>
+    <t>インストールが完了するとウィンドウが表示されます。「続行」のボタンをクリックします。</t>
+  </si>
+  <si>
+    <t>推奨される保護設定の画面が表示されます。</t>
+  </si>
+  <si>
+    <t>チェックボックスを全てチェックし、「すべて有効にして続行」をクリックします。</t>
+  </si>
+  <si>
+    <t>コンポーネントインストールの画面が表示されます。「続行」のボタンをクリックします。</t>
+  </si>
+  <si>
+    <t>製品のアクティベーションの画面が表示されます。[5]でメモしたアクティベーションキーを入力し「続行」クリックします。</t>
+  </si>
+  <si>
+    <t>機能拡張を有効するポップアップが表示されます。「システム設定を開く」をクリックします。</t>
+  </si>
+  <si>
+    <t>表示されているスイッチを有効にします。「完了」をクリックします。自分のパソコンの管理者権限が要求される場合、自分のパソコンにログインするときのアカウントとパスワードを入力します。</t>
+  </si>
+  <si>
+    <t>再度に機能拡張を有効するポップアップが表示されます。「システム設定を開く」をクリックします。</t>
+  </si>
+  <si>
+    <t>ESETシステムの拡張機能を有効にする画面が表示されるので、「続行」をクリックします。</t>
+  </si>
+  <si>
+    <t>プロキシ設定を追加画面が表示されます。「続行」をクリックします。</t>
+  </si>
+  <si>
+    <t>通知を許可する画面が表示されます。システム設定の部分をクリックします。</t>
+  </si>
+  <si>
+    <t>システム設定の通知をクリックします。ESET Endpoint Securityをクリックします。</t>
+  </si>
+  <si>
+    <t>通知を許可を有効にします。</t>
+  </si>
+  <si>
+    <t>有効にした状態です。</t>
+  </si>
+  <si>
+    <t>インストールウィザードの「閉じる」をクリックします。</t>
+  </si>
+  <si>
+    <t>ダウンロードしたファイルをゴミ箱に入れるかどうか聞いてくるポップアップが表示されます。「ゴミ箱に入れる」をクリックします。</t>
+  </si>
+  <si>
+    <t>検索ウィンドウを開き、ESET Endpoint Securityをクリックします。</t>
+  </si>
+  <si>
+    <t>表示されたESET Endpoint Securityの「アップデート」の部分をクリックします。</t>
+  </si>
+  <si>
+    <t>アップデートが完了した概要画面です。「検査」の部分をクリックします。</t>
+  </si>
+  <si>
+    <t>全ての設定が完了をしたとのお知らせのウィンドウが開きます。「完了」をクリックします。</t>
+  </si>
+  <si>
+    <t>「今すぐアップデート」が表示された場合、それををクリックします。常にこの画面を確認し、最新版を確保します。</t>
+  </si>
+  <si>
+    <t>「今すぐ検査」をクリックします。</t>
+  </si>
+  <si>
+    <t>検査が完了した画面です。</t>
   </si>
 </sst>
 </file>
@@ -6268,26 +5938,26 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -6332,7 +6002,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -6640,7 +6310,7 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
@@ -6648,15 +6318,15 @@
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -6664,20 +6334,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>388</v>
+        <v>364</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -6686,7 +6356,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -6711,11 +6381,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
@@ -6723,23 +6393,23 @@
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -6747,103 +6417,103 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="160" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>326</v>
+        <v>302</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>328</v>
+        <v>304</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>330</v>
+        <v>306</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="96" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>332</v>
+        <v>308</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="66" x14ac:dyDescent="0.2">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>438</v>
+        <v>414</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>334</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>
@@ -6861,7 +6531,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
@@ -6869,23 +6539,23 @@
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>335</v>
+        <v>311</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -6893,56 +6563,56 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>341</v>
+        <v>317</v>
       </c>
       <c r="D9" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>342</v>
+        <v>318</v>
       </c>
       <c r="D10" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="171.6" x14ac:dyDescent="0.2">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="208" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>345</v>
+        <v>321</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -6971,7 +6641,7 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
@@ -6979,23 +6649,23 @@
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -7003,20 +6673,20 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="96" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7025,12 +6695,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="96" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>348</v>
+        <v>324</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -7038,217 +6708,217 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>349</v>
+        <v>325</v>
       </c>
       <c r="C10" t="s">
         <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>351</v>
+        <v>327</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>353</v>
+        <v>329</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>355</v>
+        <v>331</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>357</v>
+        <v>333</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>360</v>
+        <v>336</v>
       </c>
       <c r="C16" t="s">
         <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>362</v>
+        <v>338</v>
       </c>
       <c r="C17" t="s">
         <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>364</v>
+        <v>340</v>
       </c>
       <c r="C18" t="s">
         <v>14</v>
       </c>
       <c r="D18" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="C19" t="s">
         <v>14</v>
       </c>
       <c r="D19" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="92.55" customHeight="1" x14ac:dyDescent="0.2">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="92.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>368</v>
+        <v>344</v>
       </c>
       <c r="C20" t="s">
         <v>47</v>
       </c>
       <c r="D20" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="96" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>370</v>
+        <v>346</v>
       </c>
       <c r="C21" t="s">
         <v>14</v>
       </c>
       <c r="D21" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>372</v>
+        <v>348</v>
       </c>
       <c r="C22" t="s">
         <v>14</v>
       </c>
       <c r="D22" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>374</v>
+        <v>350</v>
       </c>
       <c r="C23" t="s">
         <v>14</v>
       </c>
       <c r="D23" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="66" x14ac:dyDescent="0.2">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>376</v>
+        <v>352</v>
       </c>
       <c r="C24" t="s">
         <v>14</v>
       </c>
       <c r="D24" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>378</v>
+        <v>354</v>
       </c>
       <c r="C25" t="s">
         <v>14</v>
       </c>
       <c r="D25" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="66" x14ac:dyDescent="0.2">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>380</v>
+        <v>356</v>
       </c>
       <c r="C26" t="s">
         <v>14</v>
       </c>
       <c r="D26" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>382</v>
+        <v>358</v>
       </c>
     </row>
   </sheetData>
@@ -7266,15 +6936,15 @@
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="84.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="84.1640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" customWidth="1"/>
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -7282,7 +6952,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -7290,7 +6960,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -7298,15 +6968,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="160" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -7320,7 +6990,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="112" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
@@ -7328,7 +6998,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -7339,10 +7009,10 @@
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -7353,10 +7023,10 @@
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
@@ -7364,46 +7034,46 @@
         <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>383</v>
+        <v>359</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>384</v>
+        <v>360</v>
       </c>
       <c r="D12" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>385</v>
+        <v>361</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>17</v>
       </c>
@@ -7411,10 +7081,10 @@
         <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -7425,10 +7095,10 @@
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -7439,10 +7109,10 @@
         <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -7453,10 +7123,10 @@
         <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>21</v>
       </c>
@@ -7464,10 +7134,10 @@
         <v>14</v>
       </c>
       <c r="D18" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>22</v>
       </c>
@@ -7475,10 +7145,10 @@
         <v>14</v>
       </c>
       <c r="D19" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="176" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>23</v>
       </c>
@@ -7486,10 +7156,10 @@
         <v>14</v>
       </c>
       <c r="D20" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>24</v>
       </c>
@@ -7497,10 +7167,10 @@
         <v>14</v>
       </c>
       <c r="D21" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>25</v>
       </c>
@@ -7508,10 +7178,10 @@
         <v>14</v>
       </c>
       <c r="D22" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>26</v>
       </c>
@@ -7519,10 +7189,10 @@
         <v>14</v>
       </c>
       <c r="D23" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>27</v>
       </c>
@@ -7530,10 +7200,10 @@
         <v>14</v>
       </c>
       <c r="D24" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>28</v>
       </c>
@@ -7541,10 +7211,10 @@
         <v>14</v>
       </c>
       <c r="D25" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>29</v>
       </c>
@@ -7552,10 +7222,10 @@
         <v>14</v>
       </c>
       <c r="D26" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
         <v>30</v>
       </c>
@@ -7563,10 +7233,10 @@
         <v>14</v>
       </c>
       <c r="D27" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -7577,7 +7247,7 @@
         <v>14</v>
       </c>
       <c r="D28" t="s">
-        <v>421</v>
+        <v>397</v>
       </c>
     </row>
   </sheetData>
@@ -7595,15 +7265,15 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="77.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="77.83203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" customWidth="1"/>
     <col min="4" max="4" width="30.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -7611,7 +7281,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -7619,7 +7289,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -7627,15 +7297,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="144" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -7649,7 +7319,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -7663,12 +7333,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>431</v>
+        <v>407</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
@@ -7677,7 +7347,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -7691,7 +7361,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>40</v>
       </c>
@@ -7699,7 +7369,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="144" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -7713,7 +7383,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -7727,7 +7397,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>46</v>
       </c>
@@ -7738,7 +7408,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -7752,7 +7422,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="112" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>51</v>
       </c>
@@ -7772,21 +7442,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6E56ADE-9B9A-41F5-BFC9-8C8E6A100436}">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="74.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="5.109375" customWidth="1"/>
-    <col min="4" max="4" width="49.109375" customWidth="1"/>
+    <col min="2" max="2" width="74.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="5.1640625" customWidth="1"/>
+    <col min="4" max="4" width="49.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -7794,7 +7464,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -7802,7 +7472,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -7810,414 +7480,419 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="144" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="D9" t="s">
         <v>58</v>
       </c>
-      <c r="D9" t="s">
+    </row>
+    <row r="10" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B10" s="1" t="s">
+      <c r="D10" t="s">
         <v>60</v>
       </c>
-      <c r="D10" t="s">
+    </row>
+    <row r="11" spans="1:4" ht="176" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="D11" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
-      <c r="B11" s="1" t="s">
+    <row r="12" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
+    <row r="13" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D12" t="s">
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="1" t="s">
+    <row r="14" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B14" s="1" t="s">
+    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D15" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B15" s="1" t="s">
+    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="1" t="s">
+    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B17" s="1" t="s">
+    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="1" t="s">
+    <row r="19" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D19" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B19" s="1" t="s">
+    <row r="20" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D20" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B20" s="1" t="s">
+    <row r="21" spans="1:4" ht="83" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="82.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="1" t="s">
+    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="D22" t="s">
         <v>82</v>
       </c>
-      <c r="D21" t="s">
+    </row>
+    <row r="23" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="D23" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="1" t="s">
+    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="D24" t="s">
         <v>84</v>
       </c>
-      <c r="D22" t="s">
+    </row>
+    <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="D25" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" s="1" t="s">
+    <row r="26" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="D26" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="D27" t="s">
         <v>86</v>
       </c>
-      <c r="D23" t="s">
+    </row>
+    <row r="28" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="D28" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="1" t="s">
+    <row r="29" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="D29" t="s">
         <v>88</v>
       </c>
-      <c r="D24" t="s">
+    </row>
+    <row r="30" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="D30" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B25" s="1" t="s">
+    <row r="31" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="D31" t="s">
         <v>90</v>
       </c>
-      <c r="D25" t="s">
+    </row>
+    <row r="32" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="D32" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>4</v>
-      </c>
-      <c r="B26" s="1" t="s">
+    <row r="33" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D33" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>4</v>
-      </c>
-      <c r="B27" s="1" t="s">
+    <row r="34" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="D34" t="s">
         <v>94</v>
       </c>
-      <c r="D27" t="s">
+    </row>
+    <row r="35" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>4</v>
-      </c>
-      <c r="B28" s="1" t="s">
+      <c r="D35" t="s">
         <v>96</v>
       </c>
-      <c r="D28" t="s">
+    </row>
+    <row r="36" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="B36" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>4</v>
-      </c>
-      <c r="B29" s="1" t="s">
+      <c r="D36" t="s">
         <v>98</v>
       </c>
-      <c r="D29" t="s">
+    </row>
+    <row r="37" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B37" s="1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>4</v>
-      </c>
-      <c r="B30" s="1" t="s">
+      <c r="D37" t="s">
         <v>100</v>
       </c>
-      <c r="D30" t="s">
+    </row>
+    <row r="38" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B38" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>4</v>
-      </c>
-      <c r="B31" s="1" t="s">
+      <c r="D38" t="s">
         <v>102</v>
       </c>
-      <c r="D31" t="s">
+    </row>
+    <row r="39" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B39" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="D39" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>4</v>
-      </c>
-      <c r="B32" s="1" t="s">
+    <row r="40" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B40" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="D40" t="s">
         <v>104</v>
       </c>
-      <c r="D32" t="s">
+    </row>
+    <row r="41" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B41" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="D41" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>4</v>
-      </c>
-      <c r="B33" s="1" t="s">
+    <row r="42" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B42" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="D42" t="s">
         <v>106</v>
       </c>
-      <c r="D33" t="s">
+    </row>
+    <row r="43" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="B43" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="D43" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>4</v>
-      </c>
-      <c r="B34" s="1" t="s">
+    <row r="44" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B44" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="D44" t="s">
         <v>108</v>
       </c>
-      <c r="D34" t="s">
+    </row>
+    <row r="45" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="B45" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="D45" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>4</v>
-      </c>
-      <c r="B35" s="1" t="s">
+    <row r="46" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B46" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="D46" t="s">
         <v>110</v>
       </c>
-      <c r="D35" t="s">
+    </row>
+    <row r="47" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B47" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="D47" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B36" s="1" t="s">
+    <row r="48" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="B48" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="D48" t="s">
         <v>112</v>
       </c>
-      <c r="D36" t="s">
+    </row>
+    <row r="49" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B49" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="D49" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B37" s="1" t="s">
+    <row r="50" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B50" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="D50" t="s">
         <v>114</v>
       </c>
-      <c r="D37" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B38" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D38" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B39" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D39" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B40" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D40" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B41" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D41" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B42" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D42" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B43" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D43" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B44" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="D44" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B45" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D45" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B46" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D46" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B47" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D47" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B48" s="1" t="s">
-        <v>440</v>
-      </c>
-      <c r="D48" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B49" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D49" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B50" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D50" t="s">
-        <v>138</v>
+    </row>
+    <row r="51" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B51" s="1" t="s">
+        <v>446</v>
       </c>
     </row>
   </sheetData>
@@ -8235,7 +7910,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
@@ -8243,23 +7918,23 @@
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -8267,20 +7942,20 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>141</v>
+        <v>117</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8289,26 +7964,26 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="66" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>142</v>
+        <v>118</v>
       </c>
       <c r="D7" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>145</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -8326,7 +8001,7 @@
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
@@ -8334,23 +8009,23 @@
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -8358,20 +8033,20 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="112" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>148</v>
+        <v>124</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8380,238 +8055,238 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>150</v>
+        <v>126</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>154</v>
+        <v>130</v>
       </c>
       <c r="C10" t="s">
         <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>441</v>
+        <v>415</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>157</v>
+        <v>133</v>
       </c>
       <c r="D12" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>159</v>
+        <v>135</v>
       </c>
       <c r="D13" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>163</v>
+        <v>139</v>
       </c>
       <c r="C15" t="s">
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>165</v>
+        <v>141</v>
       </c>
       <c r="C16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
       <c r="C17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="D18" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>442</v>
+        <v>416</v>
       </c>
       <c r="D19" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="D20" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="D21" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="96" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="D22" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>176</v>
+        <v>152</v>
       </c>
       <c r="D23" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>178</v>
+        <v>154</v>
       </c>
       <c r="D24" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>180</v>
+        <v>156</v>
       </c>
       <c r="D25" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>182</v>
+        <v>158</v>
       </c>
       <c r="D26" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="66" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="96" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>432</v>
+        <v>408</v>
       </c>
       <c r="D27" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>185</v>
+        <v>161</v>
       </c>
       <c r="D28" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
-        <v>187</v>
+        <v>163</v>
       </c>
       <c r="D29" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>189</v>
+        <v>165</v>
       </c>
       <c r="D30" t="s">
-        <v>190</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -8625,11 +8300,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
@@ -8637,23 +8312,23 @@
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -8661,20 +8336,20 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="112" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>193</v>
+        <v>169</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8683,145 +8358,145 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="128" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>197</v>
+        <v>173</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>199</v>
+        <v>175</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>202</v>
+        <v>178</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>204</v>
+        <v>180</v>
       </c>
       <c r="D14" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>206</v>
+        <v>182</v>
       </c>
       <c r="D15" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="112" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>208</v>
+        <v>184</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="198" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="240" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>4</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>433</v>
+        <v>409</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>4</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>423</v>
+        <v>399</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B20" s="3" t="s">
-        <v>425</v>
+        <v>401</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>4</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>443</v>
+        <v>417</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -8831,47 +8506,47 @@
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>4</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>427</v>
+        <v>403</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>4</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>428</v>
+        <v>404</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B25" s="3" t="s">
-        <v>444</v>
+        <v>418</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>4</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>445</v>
+        <v>419</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
@@ -8903,35 +8578,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView topLeftCell="B42" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="100.6640625" style="3" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="34.77734375" customWidth="1"/>
+    <col min="4" max="4" width="34.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -8939,20 +8614,20 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="112" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>212</v>
+        <v>188</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8961,406 +8636,406 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="132" x14ac:dyDescent="0.2">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="176" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>215</v>
+        <v>191</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="D9" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D10" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="B11" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D11" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B13" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="B14" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D14" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="B15" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="D15" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="B16" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D16" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="B17" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D17" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B18" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D18" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="96" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="3" t="s">
+    <row r="23" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="D10" t="s">
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B11" s="3" t="s">
+    <row r="24" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="D11" t="s">
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="3" t="s">
+    <row r="25" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="B25" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="D25" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B13" s="3" t="s">
+    <row r="26" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="B26" s="3" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B14" s="3" t="s">
+      <c r="D26" t="s">
         <v>224</v>
       </c>
-      <c r="D14" t="s">
+    </row>
+    <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B27" s="3" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B15" s="3" t="s">
-        <v>434</v>
-      </c>
-      <c r="D15" t="s">
+    <row r="28" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B16" s="3" t="s">
+      <c r="C28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" t="s">
         <v>227</v>
       </c>
-      <c r="D16" t="s">
+    </row>
+    <row r="29" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B17" s="3" t="s">
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" t="s">
         <v>229</v>
       </c>
-      <c r="D17" t="s">
+    </row>
+    <row r="30" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="B30" s="3" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B18" s="3" t="s">
+      <c r="D30" t="s">
         <v>231</v>
       </c>
-      <c r="D18" t="s">
+    </row>
+    <row r="31" spans="1:4" ht="96" x14ac:dyDescent="0.2">
+      <c r="B31" s="3" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="3" t="s">
+    <row r="32" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B32" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="C19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="D32" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="66" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="3" t="s">
+    <row r="33" spans="1:4" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="C20" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="D33" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" s="3" t="s">
+    <row r="34" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B34" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="C21" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="D34" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="3" t="s">
+    <row r="35" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="C22" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" s="3" t="s">
+    <row r="36" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="C36" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" t="s">
         <v>241</v>
       </c>
-      <c r="C23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" t="s">
+    </row>
+    <row r="37" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="B37" s="3" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="3" t="s">
+      <c r="D37" t="s">
         <v>243</v>
       </c>
-      <c r="C24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" t="s">
+    </row>
+    <row r="38" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B38" s="3" t="s">
         <v>244</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B25" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="D25" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B26" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="D26" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B27" s="3" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>4</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="C28" t="s">
-        <v>4</v>
-      </c>
-      <c r="D28" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>4</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="C29" t="s">
-        <v>4</v>
-      </c>
-      <c r="D29" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B30" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="D30" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="66" x14ac:dyDescent="0.2">
-      <c r="B31" s="3" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B32" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="D32" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="D33" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B34" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="D34" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>4</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="C35" t="s">
-        <v>4</v>
-      </c>
-      <c r="D35" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>4</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>435</v>
-      </c>
-      <c r="C36" t="s">
-        <v>4</v>
-      </c>
-      <c r="D36" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B37" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="D37" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B38" s="3" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="3" t="s">
-        <v>269</v>
+        <v>245</v>
       </c>
       <c r="D39" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B40" s="3" t="s">
-        <v>271</v>
+        <v>247</v>
       </c>
       <c r="D40" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B41" s="3" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>4</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>274</v>
+        <v>250</v>
       </c>
       <c r="C42" t="s">
         <v>4</v>
       </c>
       <c r="D42" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B43" s="3" t="s">
-        <v>276</v>
+        <v>252</v>
       </c>
       <c r="D43" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B44" s="3" t="s">
-        <v>278</v>
+        <v>254</v>
       </c>
       <c r="D44" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B45" s="3" t="s">
-        <v>280</v>
+        <v>256</v>
       </c>
       <c r="D45" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B46" s="3" t="s">
-        <v>282</v>
+        <v>258</v>
       </c>
       <c r="D46" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B47" s="3" t="s">
-        <v>284</v>
+        <v>260</v>
       </c>
       <c r="D47" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>4</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>436</v>
+        <v>412</v>
       </c>
       <c r="C48" t="s">
         <v>4</v>
       </c>
       <c r="D48" t="s">
-        <v>286</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -9374,11 +9049,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A687F900-5547-4D89-8494-B67FCE27BE96}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
@@ -9386,23 +9061,23 @@
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -9410,236 +9085,236 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="184.8" x14ac:dyDescent="0.2">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="224" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D11" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D12" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D13" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="B14" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D14" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="D15" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="96" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="D21" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="128" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
         <v>289</v>
       </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="1" t="s">
+    </row>
+    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B9" s="1" t="s">
+    </row>
+    <row r="25" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="1" t="s">
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="112" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>292</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
-      <c r="B11" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="D11" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="D12" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B13" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="D13" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B14" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="D14" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B15" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="D15" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B16" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="C16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B17" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="C17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B18" s="1" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B19" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="C19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="66" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="C20" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
-      <c r="B21" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="D21" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>437</v>
-      </c>
-      <c r="C22" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B24" s="1" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>4</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="C25" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>4</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>316</v>
       </c>
       <c r="C26" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="144" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>317</v>
+        <v>293</v>
       </c>
       <c r="C27" t="s">
         <v>14</v>
       </c>
       <c r="D27" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="132" x14ac:dyDescent="0.2">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="160" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>319</v>
+        <v>295</v>
       </c>
       <c r="C28" t="s">
         <v>14</v>
       </c>
       <c r="D28" t="s">
-        <v>320</v>
+        <v>296</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix typos in Mac doc.
</commit_message>
<xml_diff>
--- a/macs+lan.xlsx
+++ b/macs+lan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Projects/IMC/HikkeiPC/fresta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD8DB1DE-3DAC-5C4D-84B4-F24687B027D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EBBC85E-E71B-954B-8E03-8D6FD99E66EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="3280" windowWidth="31060" windowHeight="17480" tabRatio="772" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14100" yWindow="3140" windowWidth="31060" windowHeight="17480" tabRatio="772" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -1468,30 +1468,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve"> 利用許諾契約が表示されます。「続ける」で進めましょう。</t>
-    <rPh sb="7" eb="9">
-      <t>カイシ</t>
-    </rPh>
-    <rPh sb="15" eb="16">
-      <t>ツヅ</t>
-    </rPh>
-    <rPh sb="20" eb="21">
-      <t>スス</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>2_7.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> 利用許諾契約を確認した上で「同意する」で進めてください。</t>
-    <rPh sb="5" eb="7">
-      <t>ヨウケン</t>
-    </rPh>
-    <rPh sb="9" eb="11">
-      <t>ヒョウジサイシンバンキノウハクシキミョウツヅ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -5864,18 +5841,9 @@
     <t>インストールが完了するとウィンドウが表示されます。「続行」のボタンをクリックします。</t>
   </si>
   <si>
-    <t>推奨される保護設定の画面が表示されます。</t>
-  </si>
-  <si>
-    <t>チェックボックスを全てチェックし、「すべて有効にして続行」をクリックします。</t>
-  </si>
-  <si>
     <t>コンポーネントインストールの画面が表示されます。「続行」のボタンをクリックします。</t>
   </si>
   <si>
-    <t>製品のアクティベーションの画面が表示されます。[5]でメモしたアクティベーションキーを入力し「続行」クリックします。</t>
-  </si>
-  <si>
     <t>機能拡張を有効するポップアップが表示されます。「システム設定を開く」をクリックします。</t>
   </si>
   <si>
@@ -5885,9 +5853,6 @@
     <t>再度に機能拡張を有効するポップアップが表示されます。「システム設定を開く」をクリックします。</t>
   </si>
   <si>
-    <t>ESETシステムの拡張機能を有効にする画面が表示されるので、「続行」をクリックします。</t>
-  </si>
-  <si>
     <t>プロキシ設定を追加画面が表示されます。「続行」をクリックします。</t>
   </si>
   <si>
@@ -5931,6 +5896,24 @@
   </si>
   <si>
     <t>2_41.png</t>
+  </si>
+  <si>
+    <t>使用許諾契約が表示されます。「続ける」で進めましょう。</t>
+  </si>
+  <si>
+    <t>使用許諾契約を確認した上で「同意する」で進めてください。</t>
+  </si>
+  <si>
+    <t>「すべて有効にして続行」をクリックします。</t>
+  </si>
+  <si>
+    <t>推奨される保護設定の画面が表示されます。チェックボックスを全てチェックします。</t>
+  </si>
+  <si>
+    <t>製品のアクティベーションの画面が表示されます。[5]でメモしたアクティベーションキーを入力し、「続行」クリックします。</t>
+  </si>
+  <si>
+    <t>ESETシステムの拡張機能を有効にする画面で、「続行」をクリックします。</t>
   </si>
 </sst>
 </file>
@@ -6326,7 +6309,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -6342,7 +6325,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -6350,7 +6333,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -6401,7 +6384,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -6409,7 +6392,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -6425,17 +6408,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -6443,7 +6426,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -6454,13 +6437,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -6468,13 +6451,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -6482,13 +6465,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="96" x14ac:dyDescent="0.2">
@@ -6496,13 +6479,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="80" x14ac:dyDescent="0.2">
@@ -6510,13 +6493,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -6544,10 +6527,10 @@
   <sheetData>
     <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -6555,7 +6538,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -6571,17 +6554,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -6589,33 +6572,33 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D9" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D10" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="208" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -6657,7 +6640,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -6665,7 +6648,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -6681,7 +6664,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="96" x14ac:dyDescent="0.2">
@@ -6689,7 +6672,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6703,7 +6686,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -6713,13 +6696,13 @@
     </row>
     <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C10" t="s">
         <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -6727,24 +6710,24 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -6752,13 +6735,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -6766,40 +6749,40 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C16" t="s">
         <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C17" t="s">
         <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -6807,13 +6790,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C18" t="s">
         <v>14</v>
       </c>
       <c r="D18" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -6821,24 +6804,24 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C19" t="s">
         <v>14</v>
       </c>
       <c r="D19" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="92.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C20" t="s">
         <v>47</v>
       </c>
       <c r="D20" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="96" x14ac:dyDescent="0.2">
@@ -6846,13 +6829,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C21" t="s">
         <v>14</v>
       </c>
       <c r="D21" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -6860,35 +6843,35 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C22" t="s">
         <v>14</v>
       </c>
       <c r="D22" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C23" t="s">
         <v>14</v>
       </c>
       <c r="D23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C24" t="s">
         <v>14</v>
       </c>
       <c r="D24" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -6896,13 +6879,13 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C25" t="s">
         <v>14</v>
       </c>
       <c r="D25" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="80" x14ac:dyDescent="0.2">
@@ -6910,18 +6893,18 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C26" t="s">
         <v>14</v>
       </c>
       <c r="D26" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
   </sheetData>
@@ -6976,7 +6959,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="160" x14ac:dyDescent="0.2">
@@ -7012,7 +6995,7 @@
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -7026,7 +7009,7 @@
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -7037,7 +7020,7 @@
         <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -7045,21 +7028,21 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D12" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -7067,13 +7050,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -7084,7 +7067,7 @@
         <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -7098,7 +7081,7 @@
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -7112,7 +7095,7 @@
         <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -7126,7 +7109,7 @@
         <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -7137,7 +7120,7 @@
         <v>14</v>
       </c>
       <c r="D18" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -7148,7 +7131,7 @@
         <v>14</v>
       </c>
       <c r="D19" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="176" x14ac:dyDescent="0.2">
@@ -7159,7 +7142,7 @@
         <v>14</v>
       </c>
       <c r="D20" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -7170,7 +7153,7 @@
         <v>14</v>
       </c>
       <c r="D21" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -7181,7 +7164,7 @@
         <v>14</v>
       </c>
       <c r="D22" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -7192,7 +7175,7 @@
         <v>14</v>
       </c>
       <c r="D23" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -7203,7 +7186,7 @@
         <v>14</v>
       </c>
       <c r="D24" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -7214,7 +7197,7 @@
         <v>14</v>
       </c>
       <c r="D25" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -7225,7 +7208,7 @@
         <v>14</v>
       </c>
       <c r="D26" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -7236,7 +7219,7 @@
         <v>14</v>
       </c>
       <c r="D27" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -7250,7 +7233,7 @@
         <v>14</v>
       </c>
       <c r="D28" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
   </sheetData>
@@ -7305,7 +7288,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="144" x14ac:dyDescent="0.2">
@@ -7341,7 +7324,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
@@ -7447,8 +7430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6E56ADE-9B9A-41F5-BFC9-8C8E6A100436}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7488,7 +7471,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="80" x14ac:dyDescent="0.2">
@@ -7508,7 +7491,7 @@
     </row>
     <row r="9" spans="1:4" ht="144" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D9" t="s">
         <v>58</v>
@@ -7524,7 +7507,7 @@
     </row>
     <row r="11" spans="1:4" ht="176" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D11" t="s">
         <v>61</v>
@@ -7581,10 +7564,10 @@
     </row>
     <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="D17" t="s">
         <v>72</v>
-      </c>
-      <c r="D17" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -7592,34 +7575,34 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>74</v>
+        <v>443</v>
       </c>
       <c r="D18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D19" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D20" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="83" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D21" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -7627,10 +7610,10 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D22" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -7638,10 +7621,10 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D23" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -7649,18 +7632,18 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>425</v>
+        <v>445</v>
       </c>
       <c r="D24" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>426</v>
+        <v>444</v>
       </c>
       <c r="D25" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -7668,10 +7651,10 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="D26" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -7679,10 +7662,10 @@
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>428</v>
+        <v>446</v>
       </c>
       <c r="D27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -7690,10 +7673,10 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="D28" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -7701,10 +7684,10 @@
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="D29" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -7712,10 +7695,10 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="D30" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -7723,21 +7706,21 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="D31" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>432</v>
+        <v>447</v>
       </c>
       <c r="D32" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -7745,10 +7728,10 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D33" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -7756,10 +7739,10 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
       <c r="D34" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -7767,138 +7750,138 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D35" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D36" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D37" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D38" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
       <c r="D39" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="D40" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="D41" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
       <c r="D42" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
       <c r="D43" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
       <c r="D44" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="D45" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
       <c r="D46" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="D47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B48" s="1" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="D48" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="49" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B49" s="1" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
       <c r="D49" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="50" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B50" s="1" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="D50" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="51" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B51" s="1" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="D51" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
     </row>
   </sheetData>
@@ -7929,7 +7912,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -7937,7 +7920,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -7953,7 +7936,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -7961,7 +7944,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7972,10 +7955,10 @@
     </row>
     <row r="7" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="80" x14ac:dyDescent="0.2">
@@ -7983,13 +7966,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -8020,7 +8003,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -8028,7 +8011,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -8044,7 +8027,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="112" x14ac:dyDescent="0.2">
@@ -8052,7 +8035,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8063,7 +8046,7 @@
     </row>
     <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -8071,13 +8054,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -8085,13 +8068,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -8099,40 +8082,40 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C10" t="s">
         <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -8140,13 +8123,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -8154,13 +8137,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C15" t="s">
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -8168,7 +8151,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C16" t="s">
         <v>14</v>
@@ -8179,7 +8162,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C17" t="s">
         <v>14</v>
@@ -8190,10 +8173,10 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D18" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -8201,98 +8184,98 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D19" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D20" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="96" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D22" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D23" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D24" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D25" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D26" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="96" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D27" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D28" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D29" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D30" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -8323,7 +8306,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -8331,7 +8314,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -8347,7 +8330,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="112" x14ac:dyDescent="0.2">
@@ -8355,7 +8338,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8366,17 +8349,17 @@
     </row>
     <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="128" x14ac:dyDescent="0.2">
@@ -8384,29 +8367,29 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -8414,29 +8397,29 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D14" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D15" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="112" x14ac:dyDescent="0.2">
@@ -8444,7 +8427,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -8458,18 +8441,18 @@
         <v>4</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -8477,24 +8460,24 @@
         <v>4</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B20" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -8502,7 +8485,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -8517,7 +8500,7 @@
         <v>4</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -8527,24 +8510,24 @@
         <v>4</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B25" s="3" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -8552,7 +8535,7 @@
         <v>4</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
@@ -8601,7 +8584,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -8609,7 +8592,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -8625,7 +8608,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="112" x14ac:dyDescent="0.2">
@@ -8633,7 +8616,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8644,12 +8627,12 @@
     </row>
     <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="176" x14ac:dyDescent="0.2">
@@ -8657,13 +8640,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -8671,18 +8654,18 @@
         <v>4</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D10" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D11" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -8690,58 +8673,58 @@
         <v>4</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B13" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B14" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D14" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D15" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B16" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D16" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D17" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D18" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -8749,13 +8732,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="96" x14ac:dyDescent="0.2">
@@ -8763,13 +8746,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -8777,13 +8760,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -8791,13 +8774,13 @@
         <v>4</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -8805,13 +8788,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -8819,34 +8802,34 @@
         <v>4</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B25" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D25" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B26" s="3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D26" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B27" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -8854,13 +8837,13 @@
         <v>4</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -8868,50 +8851,50 @@
         <v>4</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B30" s="3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D30" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="96" x14ac:dyDescent="0.2">
       <c r="B31" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B32" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D32" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D33" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B34" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D34" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -8919,13 +8902,13 @@
         <v>4</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -8933,47 +8916,47 @@
         <v>4</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C36" t="s">
         <v>4</v>
       </c>
       <c r="D36" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B37" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D37" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B38" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D39" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B40" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D40" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B41" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -8981,53 +8964,53 @@
         <v>4</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C42" t="s">
         <v>4</v>
       </c>
       <c r="D42" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B43" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D43" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B44" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D44" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B45" s="3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D45" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B46" s="3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D46" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B47" s="3" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D47" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -9035,13 +9018,13 @@
         <v>4</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C48" t="s">
         <v>4</v>
       </c>
       <c r="D48" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -9072,7 +9055,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -9080,7 +9063,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -9096,7 +9079,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="224" x14ac:dyDescent="0.2">
@@ -9104,7 +9087,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -9115,7 +9098,7 @@
     </row>
     <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -9123,18 +9106,18 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -9142,91 +9125,91 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D11" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D12" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D13" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D14" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D15" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="96" x14ac:dyDescent="0.2">
@@ -9234,7 +9217,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
@@ -9245,10 +9228,10 @@
     </row>
     <row r="21" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D21" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="128" x14ac:dyDescent="0.2">
@@ -9256,18 +9239,18 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -9275,7 +9258,7 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
@@ -9289,7 +9272,7 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C26" t="s">
         <v>14</v>
@@ -9300,13 +9283,13 @@
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C27" t="s">
         <v>14</v>
       </c>
       <c r="D27" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="160" x14ac:dyDescent="0.2">
@@ -9314,13 +9297,13 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C28" t="s">
         <v>14</v>
       </c>
       <c r="D28" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
   </sheetData>

</xml_diff>